<commit_message>
Added final columns for configuration 1
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0831EF6D-0FB4-4051-AE42-0B0E3B9D6621}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6481310-65DA-40F3-8865-EDE26DFB0DAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Benchmarks" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="48">
   <si>
     <t>Benchmark</t>
   </si>
@@ -214,12 +214,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -234,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -249,6 +255,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7E4829A-9C93-4D4A-85F2-271118D8F455}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -593,6 +604,7 @@
       <c r="C2" s="5" t="s">
         <v>47</v>
       </c>
+      <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -718,7 +730,7 @@
       <c r="B14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="7" t="s">
         <v>33</v>
       </c>
     </row>
@@ -729,7 +741,7 @@
       <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="7" t="s">
         <v>26</v>
       </c>
     </row>
@@ -740,7 +752,7 @@
       <c r="B16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="7" t="s">
         <v>15</v>
       </c>
     </row>
@@ -751,7 +763,7 @@
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -762,7 +774,7 @@
       <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="7" t="s">
         <v>5</v>
       </c>
     </row>
@@ -773,7 +785,7 @@
       <c r="B19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="7" t="s">
         <v>16</v>
       </c>
     </row>
@@ -784,7 +796,7 @@
       <c r="B20" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="7" t="s">
         <v>19</v>
       </c>
     </row>
@@ -795,7 +807,7 @@
       <c r="B21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="7" t="s">
         <v>12</v>
       </c>
     </row>
@@ -806,14 +818,14 @@
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="7" t="s">
         <v>23</v>
       </c>
     </row>
@@ -833,10 +845,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4DAA02D-4B80-49E4-98A1-4EF8777A053B}">
-  <dimension ref="A2:I51"/>
+  <dimension ref="A2:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -852,31 +864,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1057,6 +1069,9 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
       <c r="B14" t="s">
         <v>41</v>
       </c>
@@ -1070,6 +1085,9 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
       <c r="B15" t="s">
         <v>42</v>
       </c>
@@ -1083,6 +1101,9 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
       <c r="B16" t="s">
         <v>43</v>
       </c>
@@ -1096,6 +1117,9 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
       <c r="B17" t="s">
         <v>44</v>
       </c>
@@ -1125,6 +1149,9 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
       <c r="B19" t="s">
         <v>41</v>
       </c>
@@ -1138,6 +1165,9 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
       <c r="B20" t="s">
         <v>42</v>
       </c>
@@ -1151,6 +1181,9 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
       <c r="B21" t="s">
         <v>43</v>
       </c>
@@ -1164,6 +1197,9 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
       <c r="B22" t="s">
         <v>44</v>
       </c>
@@ -1193,21 +1229,33 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
       <c r="B24" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
       <c r="B25" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
       <c r="B26" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
       <c r="B27" t="s">
         <v>44</v>
       </c>
@@ -1221,21 +1269,33 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>25</v>
+      </c>
       <c r="B29" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
       <c r="B30" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>25</v>
+      </c>
       <c r="B31" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>25</v>
+      </c>
       <c r="B32" t="s">
         <v>44</v>
       </c>
@@ -1249,21 +1309,33 @@
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
       <c r="B34" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>31</v>
+      </c>
       <c r="B35" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>31</v>
+      </c>
       <c r="B36" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>31</v>
+      </c>
       <c r="B37" t="s">
         <v>44</v>
       </c>
@@ -1278,7 +1350,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B39" t="s">
         <v>41</v>
@@ -1286,7 +1358,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B40" t="s">
         <v>42</v>
@@ -1294,7 +1366,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B41" t="s">
         <v>43</v>
@@ -1302,7 +1374,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B42" t="s">
         <v>44</v>
@@ -1310,46 +1382,96 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="B43" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="B44" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>20</v>
+        <v>4</v>
+      </c>
+      <c r="B45" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>5</v>
+        <v>33</v>
+      </c>
+      <c r="B46" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>16</v>
+        <v>26</v>
+      </c>
+      <c r="B47" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>15</v>
+      </c>
+      <c r="B48" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>16</v>
+      </c>
+      <c r="B51" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="B52" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added results for config 2 on astar
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6481310-65DA-40F3-8865-EDE26DFB0DAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5F3B93-864D-40B9-AA32-86CF0F5334B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Benchmarks" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="50">
   <si>
     <t>Benchmark</t>
   </si>
@@ -160,9 +160,6 @@
     <t>SRRIP</t>
   </si>
   <si>
-    <t>SHIP</t>
-  </si>
-  <si>
     <t>Hawkeye</t>
   </si>
   <si>
@@ -176,6 +173,15 @@
   </si>
   <si>
     <t>Ours</t>
+  </si>
+  <si>
+    <t>Warmup</t>
+  </si>
+  <si>
+    <t>50 mil</t>
+  </si>
+  <si>
+    <t>Sim</t>
   </si>
 </sst>
 </file>
@@ -576,7 +582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7E4829A-9C93-4D4A-85F2-271118D8F455}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -588,7 +594,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -602,7 +608,7 @@
         <v>2017</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" s="8"/>
     </row>
@@ -845,10 +851,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4DAA02D-4B80-49E4-98A1-4EF8777A053B}">
-  <dimension ref="A2:I55"/>
+  <dimension ref="A2:K86"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -863,12 +869,12 @@
     <col min="8" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>34</v>
@@ -891,24 +897,51 @@
       <c r="I2" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
       <c r="B3" t="s">
         <v>40</v>
       </c>
-      <c r="H3" t="e">
+      <c r="C3">
+        <v>50000002</v>
+      </c>
+      <c r="D3">
+        <v>144370894</v>
+      </c>
+      <c r="E3">
+        <v>1363020</v>
+      </c>
+      <c r="F3">
+        <v>1245194</v>
+      </c>
+      <c r="G3">
+        <v>117826</v>
+      </c>
+      <c r="H3">
         <f>(C3/D3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I3" t="e">
+        <v>0.34633020974435469</v>
+      </c>
+      <c r="I3">
         <f>G3/(C3/1000)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2.3565199057392037</v>
+      </c>
+      <c r="J3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -916,15 +949,15 @@
         <v>41</v>
       </c>
       <c r="H4" t="e">
-        <f t="shared" ref="H4:H23" si="0">(C4/D4)</f>
+        <f t="shared" ref="H4:H67" si="0">(C4/D4)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I4" t="e">
-        <f t="shared" ref="I4:I23" si="1">G4/(C4/1000)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <f t="shared" ref="I4:I67" si="1">G4/(C4/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -940,7 +973,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -956,12 +989,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H7" t="e">
         <f t="shared" si="0"/>
@@ -972,12 +1005,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H8" t="e">
         <f t="shared" si="0"/>
@@ -988,12 +1021,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H9" t="e">
         <f t="shared" si="0"/>
@@ -1004,12 +1037,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H10" t="e">
         <f t="shared" si="0"/>
@@ -1020,12 +1053,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H11" t="e">
         <f t="shared" si="0"/>
@@ -1036,12 +1069,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H12" t="e">
         <f t="shared" si="0"/>
@@ -1052,12 +1085,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H13" t="e">
         <f t="shared" si="0"/>
@@ -1068,44 +1101,44 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
       <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I14" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I15" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
         <v>41</v>
-      </c>
-      <c r="H14" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I14" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" t="s">
-        <v>42</v>
-      </c>
-      <c r="H15" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I15" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" t="s">
-        <v>43</v>
       </c>
       <c r="H16" t="e">
         <f t="shared" si="0"/>
@@ -1118,10 +1151,10 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H17" t="e">
         <f t="shared" si="0"/>
@@ -1137,7 +1170,7 @@
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H18" t="e">
         <f t="shared" si="0"/>
@@ -1150,10 +1183,10 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H19" t="e">
         <f t="shared" si="0"/>
@@ -1166,10 +1199,10 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H20" t="e">
         <f t="shared" si="0"/>
@@ -1182,10 +1215,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H21" t="e">
         <f t="shared" si="0"/>
@@ -1198,10 +1231,10 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H22" t="e">
         <f t="shared" si="0"/>
@@ -1214,7 +1247,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
         <v>40</v>
@@ -1230,249 +1263,1010 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
         <v>41</v>
       </c>
+      <c r="H24" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I24" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
         <v>42</v>
       </c>
+      <c r="H25" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I25" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>43</v>
       </c>
+      <c r="H26" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I26" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="H27" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I27" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="H28" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I28" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="H29" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I29" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="H30" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I30" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>43</v>
+        <v>40</v>
+      </c>
+      <c r="H31" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I31" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="H32" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I32" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
+        <v>42</v>
+      </c>
+      <c r="H33" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I33" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>43</v>
+      </c>
+      <c r="H34" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I34" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>31</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="H35" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I35" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>31</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="H36" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I36" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>31</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="H37" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I37" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>31</v>
-      </c>
-      <c r="B37" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="H38" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I38" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>32</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="H39" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I39" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>32</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="H40" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I40" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>32</v>
-      </c>
-      <c r="B41" t="s">
+      <c r="H41" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I41" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>32</v>
-      </c>
-      <c r="B42" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="H42" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I42" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="B43" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="H43" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I43" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B44" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="H44" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I44" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>4</v>
       </c>
       <c r="B45" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="H45" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I45" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="B46" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="H46" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I46" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>33</v>
+      </c>
+      <c r="B47" t="s">
+        <v>40</v>
+      </c>
+      <c r="H47" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I47" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48" t="s">
+        <v>41</v>
+      </c>
+      <c r="H48" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I48" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>33</v>
+      </c>
+      <c r="B49" t="s">
+        <v>42</v>
+      </c>
+      <c r="H49" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I49" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>33</v>
+      </c>
+      <c r="B50" t="s">
+        <v>43</v>
+      </c>
+      <c r="H50" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I50" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>26</v>
       </c>
-      <c r="B47" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+      <c r="B51" t="s">
+        <v>40</v>
+      </c>
+      <c r="H51" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I51" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" t="s">
+        <v>41</v>
+      </c>
+      <c r="H52" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I52" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53" t="s">
+        <v>42</v>
+      </c>
+      <c r="H53" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I53" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" t="s">
+        <v>43</v>
+      </c>
+      <c r="H54" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I54" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>15</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B55" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="H55" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I55" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>15</v>
+      </c>
+      <c r="B56" t="s">
+        <v>41</v>
+      </c>
+      <c r="H56" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I56" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>15</v>
+      </c>
+      <c r="B57" t="s">
+        <v>42</v>
+      </c>
+      <c r="H57" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I57" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>15</v>
+      </c>
+      <c r="B58" t="s">
+        <v>43</v>
+      </c>
+      <c r="H58" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I58" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>20</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B59" t="s">
+        <v>40</v>
+      </c>
+      <c r="H59" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I59" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>20</v>
+      </c>
+      <c r="B60" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="H60" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I60" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>20</v>
+      </c>
+      <c r="B61" t="s">
+        <v>42</v>
+      </c>
+      <c r="H61" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I61" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>20</v>
+      </c>
+      <c r="B62" t="s">
+        <v>43</v>
+      </c>
+      <c r="H62" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I62" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
         <v>5</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B63" t="s">
+        <v>40</v>
+      </c>
+      <c r="H63" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I63" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" t="s">
+        <v>41</v>
+      </c>
+      <c r="H64" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I64" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>5</v>
+      </c>
+      <c r="B65" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+      <c r="H65" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I65" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66" t="s">
+        <v>43</v>
+      </c>
+      <c r="H66" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I66" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>16</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B67" t="s">
+        <v>40</v>
+      </c>
+      <c r="H67" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I67" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>16</v>
+      </c>
+      <c r="B68" t="s">
+        <v>41</v>
+      </c>
+      <c r="H68" t="e">
+        <f t="shared" ref="H68:H86" si="2">(C68/D68)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I68" t="e">
+        <f t="shared" ref="I68:I86" si="3">G68/(C68/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>16</v>
+      </c>
+      <c r="B69" t="s">
+        <v>42</v>
+      </c>
+      <c r="H69" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I69" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>16</v>
+      </c>
+      <c r="B70" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+      <c r="H70" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I70" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
         <v>19</v>
       </c>
-      <c r="B52" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+      <c r="B71" t="s">
+        <v>40</v>
+      </c>
+      <c r="H71" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I71" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>19</v>
+      </c>
+      <c r="B72" t="s">
+        <v>41</v>
+      </c>
+      <c r="H72" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I72" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>19</v>
+      </c>
+      <c r="B73" t="s">
+        <v>42</v>
+      </c>
+      <c r="H73" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I73" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>19</v>
+      </c>
+      <c r="B74" t="s">
+        <v>43</v>
+      </c>
+      <c r="H74" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I74" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+      <c r="B75" t="s">
+        <v>40</v>
+      </c>
+      <c r="H75" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I75" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>12</v>
+      </c>
+      <c r="B76" t="s">
+        <v>41</v>
+      </c>
+      <c r="H76" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I76" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>12</v>
+      </c>
+      <c r="B77" t="s">
+        <v>42</v>
+      </c>
+      <c r="H77" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I77" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>12</v>
+      </c>
+      <c r="B78" t="s">
+        <v>43</v>
+      </c>
+      <c r="H78" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I78" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+      <c r="B79" t="s">
+        <v>40</v>
+      </c>
+      <c r="H79" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I79" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>22</v>
+      </c>
+      <c r="B80" t="s">
+        <v>41</v>
+      </c>
+      <c r="H80" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I80" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>22</v>
+      </c>
+      <c r="B81" t="s">
+        <v>42</v>
+      </c>
+      <c r="H81" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I81" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>22</v>
+      </c>
+      <c r="B82" t="s">
+        <v>43</v>
+      </c>
+      <c r="H82" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I82" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
         <v>23</v>
+      </c>
+      <c r="B83" t="s">
+        <v>40</v>
+      </c>
+      <c r="H83" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I83" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>23</v>
+      </c>
+      <c r="B84" t="s">
+        <v>41</v>
+      </c>
+      <c r="H84" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I84" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>23</v>
+      </c>
+      <c r="B85" t="s">
+        <v>42</v>
+      </c>
+      <c r="H85" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I85" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>23</v>
+      </c>
+      <c r="B86" t="s">
+        <v>43</v>
+      </c>
+      <c r="H86" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I86" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added config1 for Hawkeye for astar
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5F3B93-864D-40B9-AA32-86CF0F5334B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F4BC6D-FB90-4B81-A769-2D92D0AED199}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="51">
   <si>
     <t>Benchmark</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t>Sim</t>
+  </si>
+  <si>
+    <t>Hit Rate</t>
   </si>
 </sst>
 </file>
@@ -851,25 +854,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4DAA02D-4B80-49E4-98A1-4EF8777A053B}">
-  <dimension ref="A2:K86"/>
+  <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -898,13 +903,16 @@
         <v>30</v>
       </c>
       <c r="J2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -934,62 +942,118 @@
         <f>G3/(C3/1000)</f>
         <v>2.3565199057392037</v>
       </c>
-      <c r="J3" t="s">
-        <v>48</v>
-      </c>
       <c r="K3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
       <c r="B4" t="s">
         <v>41</v>
       </c>
-      <c r="H4" t="e">
+      <c r="C4">
+        <v>50000002</v>
+      </c>
+      <c r="D4">
+        <v>144723077</v>
+      </c>
+      <c r="E4">
+        <v>1363019</v>
+      </c>
+      <c r="F4">
+        <v>1237390</v>
+      </c>
+      <c r="G4">
+        <v>125629</v>
+      </c>
+      <c r="H4">
         <f t="shared" ref="H4:H67" si="0">(C4/D4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I4" t="e">
-        <f t="shared" ref="I4:I67" si="1">G4/(C4/1000)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+        <v>0.34548741663363058</v>
+      </c>
+      <c r="I4">
+        <f>G4/(C4/1000)</f>
+        <v>2.5125798994968038</v>
+      </c>
+      <c r="K4" t="s">
+        <v>48</v>
+      </c>
+      <c r="L4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
       <c r="B5" t="s">
         <v>42</v>
       </c>
-      <c r="H5" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I5" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>50000002</v>
+      </c>
+      <c r="D5">
+        <v>144624545</v>
+      </c>
+      <c r="E5">
+        <v>1363017</v>
+      </c>
+      <c r="F5">
+        <v>1237373</v>
+      </c>
+      <c r="G5">
+        <v>125644</v>
+      </c>
+      <c r="H5">
+        <f>(C5/D5)</f>
+        <v>0.34572279553239044</v>
+      </c>
+      <c r="I5">
+        <f>G5/(C5/1000)</f>
+        <v>2.5128798994848038</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
       <c r="B6" t="s">
         <v>43</v>
       </c>
-      <c r="H6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I6" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>50000002</v>
+      </c>
+      <c r="D6">
+        <v>144624545</v>
+      </c>
+      <c r="E6">
+        <v>33711</v>
+      </c>
+      <c r="F6">
+        <v>30050</v>
+      </c>
+      <c r="G6">
+        <f>E6-F6</f>
+        <v>3661</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>0.34572279553239044</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ref="I6:I67" si="1">G6/(C6/1000)</f>
+        <v>7.321999707120011E-2</v>
+      </c>
+      <c r="J6">
+        <f>F6/E6</f>
+        <v>0.89140043309305572</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1005,7 +1069,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1021,7 +1085,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1037,7 +1101,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1053,7 +1117,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1069,7 +1133,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1085,7 +1149,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1101,7 +1165,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1117,7 +1181,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1133,7 +1197,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -2280,12 +2344,1439 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E5CF80-89BD-41BF-8339-D77E14018905}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:K86"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:G5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="4" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3">
+        <v>50000002</v>
+      </c>
+      <c r="D3">
+        <v>131275368</v>
+      </c>
+      <c r="E3">
+        <v>2517437</v>
+      </c>
+      <c r="F3">
+        <v>2379046</v>
+      </c>
+      <c r="G3">
+        <v>138391</v>
+      </c>
+      <c r="H3">
+        <f>(C3/D3)</f>
+        <v>0.38087877993988939</v>
+      </c>
+      <c r="I3">
+        <f>G3/(C3/1000)</f>
+        <v>2.7678198892872046</v>
+      </c>
+      <c r="J3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4">
+        <v>50000002</v>
+      </c>
+      <c r="D4">
+        <v>131351438</v>
+      </c>
+      <c r="E4">
+        <v>2517362</v>
+      </c>
+      <c r="F4">
+        <v>2372183</v>
+      </c>
+      <c r="G4">
+        <v>145179</v>
+      </c>
+      <c r="H4">
+        <f>(C4/D4)</f>
+        <v>0.3806582003312366</v>
+      </c>
+      <c r="I4">
+        <f>G4/(C4/1000)</f>
+        <v>2.9035798838568048</v>
+      </c>
+      <c r="J4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5">
+        <f>(Config1!C5/Config1!D5)</f>
+        <v>0.34572279553239044</v>
+      </c>
+      <c r="I5">
+        <f>Config1!G5/(Config1!C5/1000)</f>
+        <v>2.5128798994848038</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" t="e">
+        <f>(C6/D6)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I6" t="e">
+        <f>G6/(C6/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" t="e">
+        <f>(C7/D7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I7" t="e">
+        <f>G7/(C7/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" t="e">
+        <f>(C8/D8)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I8" t="e">
+        <f>G8/(C8/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" t="e">
+        <f>(C9/D9)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I9" t="e">
+        <f>G9/(C9/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" t="e">
+        <f>(C10/D10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I10" t="e">
+        <f>G10/(C10/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" t="e">
+        <f>(C11/D11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I11" t="e">
+        <f>G11/(C11/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" t="e">
+        <f>(C12/D12)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I12" t="e">
+        <f>G12/(C12/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" t="e">
+        <f>(C13/D13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I13" t="e">
+        <f>G13/(C13/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" t="e">
+        <f>(C14/D14)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I14" t="e">
+        <f>G14/(C14/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" t="e">
+        <f>(C15/D15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I15" t="e">
+        <f>G15/(C15/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" t="e">
+        <f>(C16/D16)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I16" t="e">
+        <f>G16/(C16/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" t="e">
+        <f>(C17/D17)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I17" t="e">
+        <f>G17/(C17/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="H18" t="e">
+        <f>(C18/D18)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I18" t="e">
+        <f>G18/(C18/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" t="e">
+        <f>(C19/D19)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I19" t="e">
+        <f>G19/(C19/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="H20" t="e">
+        <f>(C20/D20)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I20" t="e">
+        <f>G20/(C20/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="H21" t="e">
+        <f>(C21/D21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I21" t="e">
+        <f>G21/(C21/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="H22" t="e">
+        <f>(C22/D22)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I22" t="e">
+        <f>G22/(C22/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="H23" t="e">
+        <f>(C23/D23)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I23" t="e">
+        <f>G23/(C23/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="H24" t="e">
+        <f>(C24/D24)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I24" t="e">
+        <f>G24/(C24/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>42</v>
+      </c>
+      <c r="H25" t="e">
+        <f>(C25/D25)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I25" t="e">
+        <f>G25/(C25/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+      <c r="H26" t="e">
+        <f>(C26/D26)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I26" t="e">
+        <f>G26/(C26/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" t="s">
+        <v>40</v>
+      </c>
+      <c r="H27" t="e">
+        <f>(C27/D27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I27" t="e">
+        <f>G27/(C27/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="H28" t="e">
+        <f>(C28/D28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I28" t="e">
+        <f>G28/(C28/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" t="s">
+        <v>42</v>
+      </c>
+      <c r="H29" t="e">
+        <f>(C29/D29)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I29" t="e">
+        <f>G29/(C29/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>43</v>
+      </c>
+      <c r="H30" t="e">
+        <f>(C30/D30)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I30" t="e">
+        <f>G30/(C30/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" t="s">
+        <v>40</v>
+      </c>
+      <c r="H31" t="e">
+        <f>(C31/D31)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I31" t="e">
+        <f>G31/(C31/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>41</v>
+      </c>
+      <c r="H32" t="e">
+        <f>(C32/D32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I32" t="e">
+        <f>G32/(C32/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>42</v>
+      </c>
+      <c r="H33" t="e">
+        <f>(C33/D33)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I33" t="e">
+        <f>G33/(C33/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>43</v>
+      </c>
+      <c r="H34" t="e">
+        <f>(C34/D34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I34" t="e">
+        <f>G34/(C34/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" t="s">
+        <v>40</v>
+      </c>
+      <c r="H35" t="e">
+        <f>(C35/D35)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I35" t="e">
+        <f>G35/(C35/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36" t="s">
+        <v>41</v>
+      </c>
+      <c r="H36" t="e">
+        <f>(C36/D36)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I36" t="e">
+        <f>G36/(C36/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" t="s">
+        <v>42</v>
+      </c>
+      <c r="H37" t="e">
+        <f>(C37/D37)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I37" t="e">
+        <f>G37/(C37/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38" t="s">
+        <v>43</v>
+      </c>
+      <c r="H38" t="e">
+        <f>(C38/D38)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I38" t="e">
+        <f>G38/(C38/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" t="s">
+        <v>40</v>
+      </c>
+      <c r="H39" t="e">
+        <f>(C39/D39)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I39" t="e">
+        <f>G39/(C39/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" t="s">
+        <v>41</v>
+      </c>
+      <c r="H40" t="e">
+        <f>(C40/D40)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I40" t="e">
+        <f>G40/(C40/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" t="s">
+        <v>42</v>
+      </c>
+      <c r="H41" t="e">
+        <f>(C41/D41)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I41" t="e">
+        <f>G41/(C41/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" t="s">
+        <v>43</v>
+      </c>
+      <c r="H42" t="e">
+        <f>(C42/D42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I42" t="e">
+        <f>G42/(C42/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" t="s">
+        <v>40</v>
+      </c>
+      <c r="H43" t="e">
+        <f>(C43/D43)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I43" t="e">
+        <f>G43/(C43/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" t="s">
+        <v>41</v>
+      </c>
+      <c r="H44" t="e">
+        <f>(C44/D44)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I44" t="e">
+        <f>G44/(C44/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" t="s">
+        <v>42</v>
+      </c>
+      <c r="H45" t="e">
+        <f>(C45/D45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I45" t="e">
+        <f>G45/(C45/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" t="s">
+        <v>43</v>
+      </c>
+      <c r="H46" t="e">
+        <f>(C46/D46)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I46" t="e">
+        <f>G46/(C46/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>33</v>
+      </c>
+      <c r="B47" t="s">
+        <v>40</v>
+      </c>
+      <c r="H47" t="e">
+        <f>(C47/D47)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I47" t="e">
+        <f>G47/(C47/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48" t="s">
+        <v>41</v>
+      </c>
+      <c r="H48" t="e">
+        <f>(C48/D48)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I48" t="e">
+        <f>G48/(C48/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>33</v>
+      </c>
+      <c r="B49" t="s">
+        <v>42</v>
+      </c>
+      <c r="H49" t="e">
+        <f>(C49/D49)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I49" t="e">
+        <f>G49/(C49/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>33</v>
+      </c>
+      <c r="B50" t="s">
+        <v>43</v>
+      </c>
+      <c r="H50" t="e">
+        <f>(C50/D50)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I50" t="e">
+        <f>G50/(C50/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B51" t="s">
+        <v>40</v>
+      </c>
+      <c r="H51" t="e">
+        <f>(C51/D51)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I51" t="e">
+        <f>G51/(C51/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" t="s">
+        <v>41</v>
+      </c>
+      <c r="H52" t="e">
+        <f>(C52/D52)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I52" t="e">
+        <f>G52/(C52/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53" t="s">
+        <v>42</v>
+      </c>
+      <c r="H53" t="e">
+        <f>(C53/D53)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I53" t="e">
+        <f>G53/(C53/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" t="s">
+        <v>43</v>
+      </c>
+      <c r="H54" t="e">
+        <f>(C54/D54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I54" t="e">
+        <f>G54/(C54/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>15</v>
+      </c>
+      <c r="B55" t="s">
+        <v>40</v>
+      </c>
+      <c r="H55" t="e">
+        <f>(C55/D55)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I55" t="e">
+        <f>G55/(C55/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>15</v>
+      </c>
+      <c r="B56" t="s">
+        <v>41</v>
+      </c>
+      <c r="H56" t="e">
+        <f>(C56/D56)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I56" t="e">
+        <f>G56/(C56/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>15</v>
+      </c>
+      <c r="B57" t="s">
+        <v>42</v>
+      </c>
+      <c r="H57" t="e">
+        <f>(C57/D57)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I57" t="e">
+        <f>G57/(C57/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>15</v>
+      </c>
+      <c r="B58" t="s">
+        <v>43</v>
+      </c>
+      <c r="H58" t="e">
+        <f>(C58/D58)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I58" t="e">
+        <f>G58/(C58/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>20</v>
+      </c>
+      <c r="B59" t="s">
+        <v>40</v>
+      </c>
+      <c r="H59" t="e">
+        <f>(C59/D59)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I59" t="e">
+        <f>G59/(C59/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>20</v>
+      </c>
+      <c r="B60" t="s">
+        <v>41</v>
+      </c>
+      <c r="H60" t="e">
+        <f>(C60/D60)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I60" t="e">
+        <f>G60/(C60/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>20</v>
+      </c>
+      <c r="B61" t="s">
+        <v>42</v>
+      </c>
+      <c r="H61" t="e">
+        <f>(C61/D61)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I61" t="e">
+        <f>G61/(C61/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>20</v>
+      </c>
+      <c r="B62" t="s">
+        <v>43</v>
+      </c>
+      <c r="H62" t="e">
+        <f>(C62/D62)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I62" t="e">
+        <f>G62/(C62/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" t="s">
+        <v>40</v>
+      </c>
+      <c r="H63" t="e">
+        <f>(C63/D63)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I63" t="e">
+        <f>G63/(C63/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" t="s">
+        <v>41</v>
+      </c>
+      <c r="H64" t="e">
+        <f>(C64/D64)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I64" t="e">
+        <f>G64/(C64/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>5</v>
+      </c>
+      <c r="B65" t="s">
+        <v>42</v>
+      </c>
+      <c r="H65" t="e">
+        <f>(C65/D65)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I65" t="e">
+        <f>G65/(C65/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66" t="s">
+        <v>43</v>
+      </c>
+      <c r="H66" t="e">
+        <f>(C66/D66)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I66" t="e">
+        <f>G66/(C66/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>16</v>
+      </c>
+      <c r="B67" t="s">
+        <v>40</v>
+      </c>
+      <c r="H67" t="e">
+        <f>(C67/D67)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I67" t="e">
+        <f>G67/(C67/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>16</v>
+      </c>
+      <c r="B68" t="s">
+        <v>41</v>
+      </c>
+      <c r="H68" t="e">
+        <f t="shared" ref="H68:H86" si="0">(C68/D68)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I68" t="e">
+        <f t="shared" ref="I68:I86" si="1">G68/(C68/1000)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>16</v>
+      </c>
+      <c r="B69" t="s">
+        <v>42</v>
+      </c>
+      <c r="H69" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I69" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>16</v>
+      </c>
+      <c r="B70" t="s">
+        <v>43</v>
+      </c>
+      <c r="H70" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I70" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>19</v>
+      </c>
+      <c r="B71" t="s">
+        <v>40</v>
+      </c>
+      <c r="H71" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I71" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>19</v>
+      </c>
+      <c r="B72" t="s">
+        <v>41</v>
+      </c>
+      <c r="H72" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I72" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>19</v>
+      </c>
+      <c r="B73" t="s">
+        <v>42</v>
+      </c>
+      <c r="H73" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I73" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>19</v>
+      </c>
+      <c r="B74" t="s">
+        <v>43</v>
+      </c>
+      <c r="H74" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I74" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>12</v>
+      </c>
+      <c r="B75" t="s">
+        <v>40</v>
+      </c>
+      <c r="H75" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I75" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>12</v>
+      </c>
+      <c r="B76" t="s">
+        <v>41</v>
+      </c>
+      <c r="H76" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I76" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>12</v>
+      </c>
+      <c r="B77" t="s">
+        <v>42</v>
+      </c>
+      <c r="H77" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I77" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>12</v>
+      </c>
+      <c r="B78" t="s">
+        <v>43</v>
+      </c>
+      <c r="H78" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I78" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>22</v>
+      </c>
+      <c r="B79" t="s">
+        <v>40</v>
+      </c>
+      <c r="H79" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I79" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>22</v>
+      </c>
+      <c r="B80" t="s">
+        <v>41</v>
+      </c>
+      <c r="H80" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I80" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>22</v>
+      </c>
+      <c r="B81" t="s">
+        <v>42</v>
+      </c>
+      <c r="H81" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I81" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>22</v>
+      </c>
+      <c r="B82" t="s">
+        <v>43</v>
+      </c>
+      <c r="H82" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I82" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>23</v>
+      </c>
+      <c r="B83" t="s">
+        <v>40</v>
+      </c>
+      <c r="H83" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I83" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>23</v>
+      </c>
+      <c r="B84" t="s">
+        <v>41</v>
+      </c>
+      <c r="H84" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I84" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>23</v>
+      </c>
+      <c r="B85" t="s">
+        <v>42</v>
+      </c>
+      <c r="H85" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I85" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>23</v>
+      </c>
+      <c r="B86" t="s">
+        <v>43</v>
+      </c>
+      <c r="H86" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I86" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added config2 for Hawkeye
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F4BC6D-FB90-4B81-A769-2D92D0AED199}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F33A673-A843-4BB5-B82F-80AAA95BB8F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="48">
   <si>
     <t>Benchmark</t>
   </si>
@@ -173,15 +173,6 @@
   </si>
   <si>
     <t>Ours</t>
-  </si>
-  <si>
-    <t>Warmup</t>
-  </si>
-  <si>
-    <t>50 mil</t>
-  </si>
-  <si>
-    <t>Sim</t>
   </si>
   <si>
     <t>Hit Rate</t>
@@ -903,14 +894,10 @@
         <v>30</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="K2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>49</v>
-      </c>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -942,12 +929,6 @@
         <f>G3/(C3/1000)</f>
         <v>2.3565199057392037</v>
       </c>
-      <c r="K3" t="s">
-        <v>48</v>
-      </c>
-      <c r="L3" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -978,12 +959,6 @@
       <c r="I4">
         <f>G4/(C4/1000)</f>
         <v>2.5125798994968038</v>
-      </c>
-      <c r="K4" t="s">
-        <v>48</v>
-      </c>
-      <c r="L4" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -2344,10 +2319,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E5CF80-89BD-41BF-8339-D77E14018905}">
-  <dimension ref="A2:K86"/>
+  <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:G5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2355,7 +2330,7 @@
     <col min="3" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -2386,11 +2361,10 @@
       <c r="J2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -2420,14 +2394,8 @@
         <f>G3/(C3/1000)</f>
         <v>2.7678198892872046</v>
       </c>
-      <c r="J3" t="s">
-        <v>48</v>
-      </c>
-      <c r="K3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -2457,46 +2425,75 @@
         <f>G4/(C4/1000)</f>
         <v>2.9035798838568048</v>
       </c>
-      <c r="J4" t="s">
-        <v>48</v>
-      </c>
-      <c r="K4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
       <c r="B5" t="s">
         <v>42</v>
       </c>
+      <c r="C5">
+        <v>50000002</v>
+      </c>
+      <c r="D5">
+        <v>131405787</v>
+      </c>
+      <c r="E5">
+        <v>2517423</v>
+      </c>
+      <c r="F5">
+        <v>2374604</v>
+      </c>
+      <c r="G5">
+        <v>142819</v>
+      </c>
       <c r="H5">
-        <f>(Config1!C5/Config1!D5)</f>
-        <v>0.34572279553239044</v>
+        <f>(C5/D5)</f>
+        <v>0.38050076135535799</v>
       </c>
       <c r="I5">
-        <f>Config1!G5/(Config1!C5/1000)</f>
-        <v>2.5128798994848038</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <f>G5/(C5/1000)</f>
+        <v>2.8563798857448046</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
       <c r="B6" t="s">
         <v>43</v>
       </c>
-      <c r="H6" t="e">
+      <c r="C6">
+        <v>50000002</v>
+      </c>
+      <c r="D6">
+        <v>131405787</v>
+      </c>
+      <c r="E6">
+        <v>34143</v>
+      </c>
+      <c r="F6">
+        <v>43676</v>
+      </c>
+      <c r="G6">
+        <f>E6-F6</f>
+        <v>-9533</v>
+      </c>
+      <c r="H6">
         <f>(C6/D6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I6" t="e">
+        <v>0.38050076135535799</v>
+      </c>
+      <c r="I6">
         <f>G6/(C6/1000)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+        <v>-0.19065999237360029</v>
+      </c>
+      <c r="J6">
+        <f>F6/E6</f>
+        <v>1.2792080367864569</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -2512,7 +2509,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -2528,7 +2525,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -2544,7 +2541,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -2560,7 +2557,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -2576,7 +2573,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -2592,7 +2589,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -2608,7 +2605,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2624,7 +2621,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -2640,7 +2637,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Added simulation for LRU on bzip2
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519B9A94-A535-40A4-BAC7-4D58DF14469B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F608D3FD-6342-4168-81F8-77788D671EAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
@@ -258,9 +258,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -269,6 +266,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -596,24 +596,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
       <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="6">
+      <c r="A2" s="5">
         <v>2016</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>2017</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>48</v>
       </c>
     </row>
@@ -744,7 +744,7 @@
       <c r="B14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>33</v>
       </c>
     </row>
@@ -755,7 +755,7 @@
       <c r="B15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>26</v>
       </c>
     </row>
@@ -766,7 +766,7 @@
       <c r="B16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>15</v>
       </c>
     </row>
@@ -777,7 +777,7 @@
       <c r="B17" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -788,7 +788,7 @@
       <c r="B18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>5</v>
       </c>
     </row>
@@ -799,7 +799,7 @@
       <c r="B19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>16</v>
       </c>
     </row>
@@ -810,7 +810,7 @@
       <c r="B20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>19</v>
       </c>
     </row>
@@ -821,7 +821,7 @@
       <c r="B21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="7" t="s">
         <v>12</v>
       </c>
     </row>
@@ -832,14 +832,14 @@
       <c r="B22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>23</v>
       </c>
     </row>
@@ -862,7 +862,7 @@
   <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -880,38 +880,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -967,7 +967,7 @@
         <v>125629</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H67" si="0">(C4/D4)</f>
+        <f>(C4/D4)</f>
         <v>0.34548741663363058</v>
       </c>
       <c r="I4">
@@ -1030,11 +1030,11 @@
         <v>3661</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
+        <f>(C6/D6)</f>
         <v>0.34572279553239044</v>
       </c>
       <c r="I6">
-        <f t="shared" ref="I6:I67" si="1">G6/(C6/1000)</f>
+        <f>G6/(C6/1000)</f>
         <v>7.321999707120011E-2</v>
       </c>
       <c r="J6">
@@ -1049,13 +1049,28 @@
       <c r="B7" t="s">
         <v>40</v>
       </c>
-      <c r="H7" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I7" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C7">
+        <v>50000001</v>
+      </c>
+      <c r="D7">
+        <v>69489973</v>
+      </c>
+      <c r="E7">
+        <v>620421</v>
+      </c>
+      <c r="F7">
+        <v>547766</v>
+      </c>
+      <c r="G7">
+        <v>72655</v>
+      </c>
+      <c r="H7">
+        <f>(C7/D7)</f>
+        <v>0.71952828359855603</v>
+      </c>
+      <c r="I7">
+        <f>G7/(C7/1000)</f>
+        <v>1.4530999709380006</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -1066,11 +1081,11 @@
         <v>41</v>
       </c>
       <c r="H8" t="e">
-        <f t="shared" si="0"/>
+        <f>(C8/D8)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I8" t="e">
-        <f t="shared" si="1"/>
+        <f>G8/(C8/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1082,11 +1097,11 @@
         <v>42</v>
       </c>
       <c r="H9" t="e">
-        <f t="shared" si="0"/>
+        <f>(C9/D9)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I9" t="e">
-        <f t="shared" si="1"/>
+        <f>G9/(C9/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1098,11 +1113,11 @@
         <v>43</v>
       </c>
       <c r="H10" t="e">
-        <f t="shared" si="0"/>
+        <f>(C10/D10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I10" t="e">
-        <f t="shared" si="1"/>
+        <f>G10/(C10/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1114,11 +1129,11 @@
         <v>40</v>
       </c>
       <c r="H11" t="e">
-        <f t="shared" si="0"/>
+        <f>(C11/D11)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I11" t="e">
-        <f t="shared" si="1"/>
+        <f>G11/(C11/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1130,11 +1145,11 @@
         <v>41</v>
       </c>
       <c r="H12" t="e">
-        <f t="shared" si="0"/>
+        <f>(C12/D12)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I12" t="e">
-        <f t="shared" si="1"/>
+        <f>G12/(C12/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1146,11 +1161,11 @@
         <v>42</v>
       </c>
       <c r="H13" t="e">
-        <f t="shared" si="0"/>
+        <f>(C13/D13)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I13" t="e">
-        <f t="shared" si="1"/>
+        <f>G13/(C13/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1162,11 +1177,11 @@
         <v>43</v>
       </c>
       <c r="H14" t="e">
-        <f t="shared" si="0"/>
+        <f>(C14/D14)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I14" t="e">
-        <f t="shared" si="1"/>
+        <f>G14/(C14/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1178,11 +1193,11 @@
         <v>40</v>
       </c>
       <c r="H15" t="e">
-        <f t="shared" si="0"/>
+        <f>(C15/D15)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I15" t="e">
-        <f t="shared" si="1"/>
+        <f>G15/(C15/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1194,11 +1209,11 @@
         <v>41</v>
       </c>
       <c r="H16" t="e">
-        <f t="shared" si="0"/>
+        <f>(C16/D16)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I16" t="e">
-        <f t="shared" si="1"/>
+        <f>G16/(C16/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1210,11 +1225,11 @@
         <v>42</v>
       </c>
       <c r="H17" t="e">
-        <f t="shared" si="0"/>
+        <f>(C17/D17)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I17" t="e">
-        <f t="shared" si="1"/>
+        <f>G17/(C17/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1226,11 +1241,11 @@
         <v>43</v>
       </c>
       <c r="H18" t="e">
-        <f t="shared" si="0"/>
+        <f>(C18/D18)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I18" t="e">
-        <f t="shared" si="1"/>
+        <f>G18/(C18/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1242,11 +1257,11 @@
         <v>40</v>
       </c>
       <c r="H19" t="e">
-        <f t="shared" si="0"/>
+        <f>(C19/D19)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I19" t="e">
-        <f t="shared" si="1"/>
+        <f>G19/(C19/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1258,11 +1273,11 @@
         <v>41</v>
       </c>
       <c r="H20" t="e">
-        <f t="shared" si="0"/>
+        <f>(C20/D20)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I20" t="e">
-        <f t="shared" si="1"/>
+        <f>G20/(C20/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1274,11 +1289,11 @@
         <v>42</v>
       </c>
       <c r="H21" t="e">
-        <f t="shared" si="0"/>
+        <f>(C21/D21)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I21" t="e">
-        <f t="shared" si="1"/>
+        <f>G21/(C21/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1290,11 +1305,11 @@
         <v>43</v>
       </c>
       <c r="H22" t="e">
-        <f t="shared" si="0"/>
+        <f>(C22/D22)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I22" t="e">
-        <f t="shared" si="1"/>
+        <f>G22/(C22/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1306,11 +1321,11 @@
         <v>40</v>
       </c>
       <c r="H23" t="e">
-        <f t="shared" si="0"/>
+        <f>(C23/D23)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I23" t="e">
-        <f t="shared" si="1"/>
+        <f>G23/(C23/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1322,11 +1337,11 @@
         <v>41</v>
       </c>
       <c r="H24" t="e">
-        <f t="shared" si="0"/>
+        <f>(C24/D24)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I24" t="e">
-        <f t="shared" si="1"/>
+        <f>G24/(C24/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1338,11 +1353,11 @@
         <v>42</v>
       </c>
       <c r="H25" t="e">
-        <f t="shared" si="0"/>
+        <f>(C25/D25)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I25" t="e">
-        <f t="shared" si="1"/>
+        <f>G25/(C25/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1354,11 +1369,11 @@
         <v>43</v>
       </c>
       <c r="H26" t="e">
-        <f t="shared" si="0"/>
+        <f>(C26/D26)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I26" t="e">
-        <f t="shared" si="1"/>
+        <f>G26/(C26/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1370,11 +1385,11 @@
         <v>40</v>
       </c>
       <c r="H27" t="e">
-        <f t="shared" si="0"/>
+        <f>(C27/D27)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I27" t="e">
-        <f t="shared" si="1"/>
+        <f>G27/(C27/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1386,11 +1401,11 @@
         <v>41</v>
       </c>
       <c r="H28" t="e">
-        <f t="shared" si="0"/>
+        <f>(C28/D28)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I28" t="e">
-        <f t="shared" si="1"/>
+        <f>G28/(C28/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1402,11 +1417,11 @@
         <v>42</v>
       </c>
       <c r="H29" t="e">
-        <f t="shared" si="0"/>
+        <f>(C29/D29)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I29" t="e">
-        <f t="shared" si="1"/>
+        <f>G29/(C29/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1418,11 +1433,11 @@
         <v>43</v>
       </c>
       <c r="H30" t="e">
-        <f t="shared" si="0"/>
+        <f>(C30/D30)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I30" t="e">
-        <f t="shared" si="1"/>
+        <f>G30/(C30/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1434,11 +1449,11 @@
         <v>40</v>
       </c>
       <c r="H31" t="e">
-        <f t="shared" si="0"/>
+        <f>(C31/D31)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I31" t="e">
-        <f t="shared" si="1"/>
+        <f>G31/(C31/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1450,11 +1465,11 @@
         <v>41</v>
       </c>
       <c r="H32" t="e">
-        <f t="shared" si="0"/>
+        <f>(C32/D32)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I32" t="e">
-        <f t="shared" si="1"/>
+        <f>G32/(C32/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1466,11 +1481,11 @@
         <v>42</v>
       </c>
       <c r="H33" t="e">
-        <f t="shared" si="0"/>
+        <f>(C33/D33)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I33" t="e">
-        <f t="shared" si="1"/>
+        <f>G33/(C33/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1482,11 +1497,11 @@
         <v>43</v>
       </c>
       <c r="H34" t="e">
-        <f t="shared" si="0"/>
+        <f>(C34/D34)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I34" t="e">
-        <f t="shared" si="1"/>
+        <f>G34/(C34/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1498,11 +1513,11 @@
         <v>40</v>
       </c>
       <c r="H35" t="e">
-        <f t="shared" si="0"/>
+        <f>(C35/D35)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I35" t="e">
-        <f t="shared" si="1"/>
+        <f>G35/(C35/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1514,11 +1529,11 @@
         <v>41</v>
       </c>
       <c r="H36" t="e">
-        <f t="shared" si="0"/>
+        <f>(C36/D36)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I36" t="e">
-        <f t="shared" si="1"/>
+        <f>G36/(C36/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1530,11 +1545,11 @@
         <v>42</v>
       </c>
       <c r="H37" t="e">
-        <f t="shared" si="0"/>
+        <f>(C37/D37)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I37" t="e">
-        <f t="shared" si="1"/>
+        <f>G37/(C37/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1546,11 +1561,11 @@
         <v>43</v>
       </c>
       <c r="H38" t="e">
-        <f t="shared" si="0"/>
+        <f>(C38/D38)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I38" t="e">
-        <f t="shared" si="1"/>
+        <f>G38/(C38/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1562,11 +1577,11 @@
         <v>40</v>
       </c>
       <c r="H39" t="e">
-        <f t="shared" si="0"/>
+        <f>(C39/D39)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I39" t="e">
-        <f t="shared" si="1"/>
+        <f>G39/(C39/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1578,11 +1593,11 @@
         <v>41</v>
       </c>
       <c r="H40" t="e">
-        <f t="shared" si="0"/>
+        <f>(C40/D40)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I40" t="e">
-        <f t="shared" si="1"/>
+        <f>G40/(C40/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1594,11 +1609,11 @@
         <v>42</v>
       </c>
       <c r="H41" t="e">
-        <f t="shared" si="0"/>
+        <f>(C41/D41)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I41" t="e">
-        <f t="shared" si="1"/>
+        <f>G41/(C41/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1610,11 +1625,11 @@
         <v>43</v>
       </c>
       <c r="H42" t="e">
-        <f t="shared" si="0"/>
+        <f>(C42/D42)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I42" t="e">
-        <f t="shared" si="1"/>
+        <f>G42/(C42/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1626,11 +1641,11 @@
         <v>40</v>
       </c>
       <c r="H43" t="e">
-        <f t="shared" si="0"/>
+        <f>(C43/D43)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I43" t="e">
-        <f t="shared" si="1"/>
+        <f>G43/(C43/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1642,11 +1657,11 @@
         <v>41</v>
       </c>
       <c r="H44" t="e">
-        <f t="shared" si="0"/>
+        <f>(C44/D44)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I44" t="e">
-        <f t="shared" si="1"/>
+        <f>G44/(C44/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1658,11 +1673,11 @@
         <v>42</v>
       </c>
       <c r="H45" t="e">
-        <f t="shared" si="0"/>
+        <f>(C45/D45)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I45" t="e">
-        <f t="shared" si="1"/>
+        <f>G45/(C45/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1674,11 +1689,11 @@
         <v>43</v>
       </c>
       <c r="H46" t="e">
-        <f t="shared" si="0"/>
+        <f>(C46/D46)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I46" t="e">
-        <f t="shared" si="1"/>
+        <f>G46/(C46/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1690,11 +1705,11 @@
         <v>40</v>
       </c>
       <c r="H47" t="e">
-        <f t="shared" si="0"/>
+        <f>(C47/D47)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I47" t="e">
-        <f t="shared" si="1"/>
+        <f>G47/(C47/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1706,11 +1721,11 @@
         <v>41</v>
       </c>
       <c r="H48" t="e">
-        <f t="shared" si="0"/>
+        <f>(C48/D48)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I48" t="e">
-        <f t="shared" si="1"/>
+        <f>G48/(C48/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1722,11 +1737,11 @@
         <v>42</v>
       </c>
       <c r="H49" t="e">
-        <f t="shared" si="0"/>
+        <f>(C49/D49)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I49" t="e">
-        <f t="shared" si="1"/>
+        <f>G49/(C49/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1738,11 +1753,11 @@
         <v>43</v>
       </c>
       <c r="H50" t="e">
-        <f t="shared" si="0"/>
+        <f>(C50/D50)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I50" t="e">
-        <f t="shared" si="1"/>
+        <f>G50/(C50/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1754,11 +1769,11 @@
         <v>40</v>
       </c>
       <c r="H51" t="e">
-        <f t="shared" si="0"/>
+        <f>(C51/D51)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I51" t="e">
-        <f t="shared" si="1"/>
+        <f>G51/(C51/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1770,11 +1785,11 @@
         <v>41</v>
       </c>
       <c r="H52" t="e">
-        <f t="shared" si="0"/>
+        <f>(C52/D52)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I52" t="e">
-        <f t="shared" si="1"/>
+        <f>G52/(C52/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1786,11 +1801,11 @@
         <v>42</v>
       </c>
       <c r="H53" t="e">
-        <f t="shared" si="0"/>
+        <f>(C53/D53)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I53" t="e">
-        <f t="shared" si="1"/>
+        <f>G53/(C53/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1802,11 +1817,11 @@
         <v>43</v>
       </c>
       <c r="H54" t="e">
-        <f t="shared" si="0"/>
+        <f>(C54/D54)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I54" t="e">
-        <f t="shared" si="1"/>
+        <f>G54/(C54/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1818,11 +1833,11 @@
         <v>40</v>
       </c>
       <c r="H55" t="e">
-        <f t="shared" si="0"/>
+        <f>(C55/D55)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I55" t="e">
-        <f t="shared" si="1"/>
+        <f>G55/(C55/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1834,11 +1849,11 @@
         <v>41</v>
       </c>
       <c r="H56" t="e">
-        <f t="shared" si="0"/>
+        <f>(C56/D56)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I56" t="e">
-        <f t="shared" si="1"/>
+        <f>G56/(C56/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1850,11 +1865,11 @@
         <v>42</v>
       </c>
       <c r="H57" t="e">
-        <f t="shared" si="0"/>
+        <f>(C57/D57)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I57" t="e">
-        <f t="shared" si="1"/>
+        <f>G57/(C57/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1866,11 +1881,11 @@
         <v>43</v>
       </c>
       <c r="H58" t="e">
-        <f t="shared" si="0"/>
+        <f>(C58/D58)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I58" t="e">
-        <f t="shared" si="1"/>
+        <f>G58/(C58/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1882,11 +1897,11 @@
         <v>40</v>
       </c>
       <c r="H59" t="e">
-        <f t="shared" si="0"/>
+        <f>(C59/D59)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I59" t="e">
-        <f t="shared" si="1"/>
+        <f>G59/(C59/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1898,11 +1913,11 @@
         <v>41</v>
       </c>
       <c r="H60" t="e">
-        <f t="shared" si="0"/>
+        <f>(C60/D60)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I60" t="e">
-        <f t="shared" si="1"/>
+        <f>G60/(C60/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1914,11 +1929,11 @@
         <v>42</v>
       </c>
       <c r="H61" t="e">
-        <f t="shared" si="0"/>
+        <f>(C61/D61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I61" t="e">
-        <f t="shared" si="1"/>
+        <f>G61/(C61/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1930,11 +1945,11 @@
         <v>43</v>
       </c>
       <c r="H62" t="e">
-        <f t="shared" si="0"/>
+        <f>(C62/D62)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I62" t="e">
-        <f t="shared" si="1"/>
+        <f>G62/(C62/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1946,11 +1961,11 @@
         <v>40</v>
       </c>
       <c r="H63" t="e">
-        <f t="shared" si="0"/>
+        <f>(C63/D63)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I63" t="e">
-        <f t="shared" si="1"/>
+        <f>G63/(C63/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1962,11 +1977,11 @@
         <v>41</v>
       </c>
       <c r="H64" t="e">
-        <f t="shared" si="0"/>
+        <f>(C64/D64)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I64" t="e">
-        <f t="shared" si="1"/>
+        <f>G64/(C64/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1978,11 +1993,11 @@
         <v>42</v>
       </c>
       <c r="H65" t="e">
-        <f t="shared" si="0"/>
+        <f>(C65/D65)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I65" t="e">
-        <f t="shared" si="1"/>
+        <f>G65/(C65/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1994,11 +2009,11 @@
         <v>43</v>
       </c>
       <c r="H66" t="e">
-        <f t="shared" si="0"/>
+        <f>(C66/D66)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I66" t="e">
-        <f t="shared" si="1"/>
+        <f>G66/(C66/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2010,11 +2025,11 @@
         <v>40</v>
       </c>
       <c r="H67" t="e">
-        <f t="shared" si="0"/>
+        <f>(C67/D67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I67" t="e">
-        <f t="shared" si="1"/>
+        <f>G67/(C67/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2026,11 +2041,11 @@
         <v>41</v>
       </c>
       <c r="H68" t="e">
-        <f t="shared" ref="H68:H86" si="2">(C68/D68)</f>
+        <f t="shared" ref="H68:H86" si="0">(C68/D68)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I68" t="e">
-        <f t="shared" ref="I68:I86" si="3">G68/(C68/1000)</f>
+        <f t="shared" ref="I68:I86" si="1">G68/(C68/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2042,11 +2057,11 @@
         <v>42</v>
       </c>
       <c r="H69" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I69" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2058,11 +2073,11 @@
         <v>43</v>
       </c>
       <c r="H70" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I70" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2074,11 +2089,11 @@
         <v>40</v>
       </c>
       <c r="H71" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I71" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2090,11 +2105,11 @@
         <v>41</v>
       </c>
       <c r="H72" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I72" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2106,11 +2121,11 @@
         <v>42</v>
       </c>
       <c r="H73" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I73" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2122,11 +2137,11 @@
         <v>43</v>
       </c>
       <c r="H74" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I74" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2138,11 +2153,11 @@
         <v>40</v>
       </c>
       <c r="H75" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I75" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2154,11 +2169,11 @@
         <v>41</v>
       </c>
       <c r="H76" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I76" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2170,11 +2185,11 @@
         <v>42</v>
       </c>
       <c r="H77" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I77" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2186,11 +2201,11 @@
         <v>43</v>
       </c>
       <c r="H78" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I78" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2202,11 +2217,11 @@
         <v>40</v>
       </c>
       <c r="H79" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I79" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2218,11 +2233,11 @@
         <v>41</v>
       </c>
       <c r="H80" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I80" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2234,11 +2249,11 @@
         <v>42</v>
       </c>
       <c r="H81" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I81" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2250,11 +2265,11 @@
         <v>43</v>
       </c>
       <c r="H82" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I82" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2266,11 +2281,11 @@
         <v>40</v>
       </c>
       <c r="H83" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I83" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2282,11 +2297,11 @@
         <v>41</v>
       </c>
       <c r="H84" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I84" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2298,11 +2313,11 @@
         <v>42</v>
       </c>
       <c r="H85" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I85" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2314,11 +2329,11 @@
         <v>43</v>
       </c>
       <c r="H86" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I86" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2336,7 +2351,7 @@
   <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2353,38 +2368,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -2409,11 +2424,11 @@
         <v>138391</v>
       </c>
       <c r="H3">
-        <f>(C3/D3)</f>
+        <f t="shared" ref="H3:H34" si="0">(C3/D3)</f>
         <v>0.38087877993988939</v>
       </c>
       <c r="I3">
-        <f>G3/(C3/1000)</f>
+        <f t="shared" ref="I3:I34" si="1">G3/(C3/1000)</f>
         <v>2.7678198892872046</v>
       </c>
     </row>
@@ -2440,11 +2455,11 @@
         <v>145179</v>
       </c>
       <c r="H4">
-        <f>(C4/D4)</f>
+        <f t="shared" si="0"/>
         <v>0.3806582003312366</v>
       </c>
       <c r="I4">
-        <f>G4/(C4/1000)</f>
+        <f t="shared" si="1"/>
         <v>2.9035798838568048</v>
       </c>
     </row>
@@ -2471,11 +2486,11 @@
         <v>142819</v>
       </c>
       <c r="H5">
-        <f>(C5/D5)</f>
+        <f t="shared" si="0"/>
         <v>0.38050076135535799</v>
       </c>
       <c r="I5">
-        <f>G5/(C5/1000)</f>
+        <f t="shared" si="1"/>
         <v>2.8563798857448046</v>
       </c>
     </row>
@@ -2503,11 +2518,11 @@
         <v>-9533</v>
       </c>
       <c r="H6">
-        <f>(C6/D6)</f>
+        <f t="shared" si="0"/>
         <v>0.38050076135535799</v>
       </c>
       <c r="I6">
-        <f>G6/(C6/1000)</f>
+        <f t="shared" si="1"/>
         <v>-0.19065999237360029</v>
       </c>
       <c r="J6">
@@ -2522,13 +2537,28 @@
       <c r="B7" t="s">
         <v>40</v>
       </c>
-      <c r="H7" t="e">
+      <c r="C7">
+        <v>50000001</v>
+      </c>
+      <c r="D7">
+        <v>67484290</v>
+      </c>
+      <c r="E7">
+        <v>853737</v>
+      </c>
+      <c r="F7">
+        <v>774446</v>
+      </c>
+      <c r="G7">
+        <v>79291</v>
+      </c>
+      <c r="H7">
         <f>(C7/D7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I7" t="e">
+        <v>0.7409131962416734</v>
+      </c>
+      <c r="I7">
         <f>G7/(C7/1000)</f>
-        <v>#DIV/0!</v>
+        <v>1.5858199682836007</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -2539,11 +2569,11 @@
         <v>41</v>
       </c>
       <c r="H8" t="e">
-        <f>(C8/D8)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I8" t="e">
-        <f>G8/(C8/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2555,11 +2585,11 @@
         <v>42</v>
       </c>
       <c r="H9" t="e">
-        <f>(C9/D9)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I9" t="e">
-        <f>G9/(C9/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2571,11 +2601,11 @@
         <v>43</v>
       </c>
       <c r="H10" t="e">
-        <f>(C10/D10)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I10" t="e">
-        <f>G10/(C10/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2587,11 +2617,11 @@
         <v>40</v>
       </c>
       <c r="H11" t="e">
-        <f>(C11/D11)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I11" t="e">
-        <f>G11/(C11/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2603,11 +2633,11 @@
         <v>41</v>
       </c>
       <c r="H12" t="e">
-        <f>(C12/D12)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I12" t="e">
-        <f>G12/(C12/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2619,11 +2649,11 @@
         <v>42</v>
       </c>
       <c r="H13" t="e">
-        <f>(C13/D13)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I13" t="e">
-        <f>G13/(C13/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2635,11 +2665,11 @@
         <v>43</v>
       </c>
       <c r="H14" t="e">
-        <f>(C14/D14)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I14" t="e">
-        <f>G14/(C14/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2651,11 +2681,11 @@
         <v>40</v>
       </c>
       <c r="H15" t="e">
-        <f>(C15/D15)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I15" t="e">
-        <f>G15/(C15/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2667,11 +2697,11 @@
         <v>41</v>
       </c>
       <c r="H16" t="e">
-        <f>(C16/D16)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I16" t="e">
-        <f>G16/(C16/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2683,11 +2713,11 @@
         <v>42</v>
       </c>
       <c r="H17" t="e">
-        <f>(C17/D17)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I17" t="e">
-        <f>G17/(C17/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2699,11 +2729,11 @@
         <v>43</v>
       </c>
       <c r="H18" t="e">
-        <f>(C18/D18)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I18" t="e">
-        <f>G18/(C18/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2715,11 +2745,11 @@
         <v>40</v>
       </c>
       <c r="H19" t="e">
-        <f>(C19/D19)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I19" t="e">
-        <f>G19/(C19/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2731,11 +2761,11 @@
         <v>41</v>
       </c>
       <c r="H20" t="e">
-        <f>(C20/D20)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I20" t="e">
-        <f>G20/(C20/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2747,11 +2777,11 @@
         <v>42</v>
       </c>
       <c r="H21" t="e">
-        <f>(C21/D21)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I21" t="e">
-        <f>G21/(C21/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2763,11 +2793,11 @@
         <v>43</v>
       </c>
       <c r="H22" t="e">
-        <f>(C22/D22)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I22" t="e">
-        <f>G22/(C22/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2779,11 +2809,11 @@
         <v>40</v>
       </c>
       <c r="H23" t="e">
-        <f>(C23/D23)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I23" t="e">
-        <f>G23/(C23/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2795,11 +2825,11 @@
         <v>41</v>
       </c>
       <c r="H24" t="e">
-        <f>(C24/D24)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I24" t="e">
-        <f>G24/(C24/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2811,11 +2841,11 @@
         <v>42</v>
       </c>
       <c r="H25" t="e">
-        <f>(C25/D25)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I25" t="e">
-        <f>G25/(C25/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2827,11 +2857,11 @@
         <v>43</v>
       </c>
       <c r="H26" t="e">
-        <f>(C26/D26)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I26" t="e">
-        <f>G26/(C26/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2843,11 +2873,11 @@
         <v>40</v>
       </c>
       <c r="H27" t="e">
-        <f>(C27/D27)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I27" t="e">
-        <f>G27/(C27/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2859,11 +2889,11 @@
         <v>41</v>
       </c>
       <c r="H28" t="e">
-        <f>(C28/D28)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I28" t="e">
-        <f>G28/(C28/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2875,11 +2905,11 @@
         <v>42</v>
       </c>
       <c r="H29" t="e">
-        <f>(C29/D29)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I29" t="e">
-        <f>G29/(C29/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2891,11 +2921,11 @@
         <v>43</v>
       </c>
       <c r="H30" t="e">
-        <f>(C30/D30)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I30" t="e">
-        <f>G30/(C30/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2907,11 +2937,11 @@
         <v>40</v>
       </c>
       <c r="H31" t="e">
-        <f>(C31/D31)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I31" t="e">
-        <f>G31/(C31/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2923,11 +2953,11 @@
         <v>41</v>
       </c>
       <c r="H32" t="e">
-        <f>(C32/D32)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I32" t="e">
-        <f>G32/(C32/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2939,11 +2969,11 @@
         <v>42</v>
       </c>
       <c r="H33" t="e">
-        <f>(C33/D33)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I33" t="e">
-        <f>G33/(C33/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2955,11 +2985,11 @@
         <v>43</v>
       </c>
       <c r="H34" t="e">
-        <f>(C34/D34)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I34" t="e">
-        <f>G34/(C34/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2971,11 +3001,11 @@
         <v>40</v>
       </c>
       <c r="H35" t="e">
-        <f>(C35/D35)</f>
+        <f t="shared" ref="H35:H67" si="2">(C35/D35)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I35" t="e">
-        <f>G35/(C35/1000)</f>
+        <f t="shared" ref="I35:I67" si="3">G35/(C35/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2987,11 +3017,11 @@
         <v>41</v>
       </c>
       <c r="H36" t="e">
-        <f>(C36/D36)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I36" t="e">
-        <f>G36/(C36/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3003,11 +3033,11 @@
         <v>42</v>
       </c>
       <c r="H37" t="e">
-        <f>(C37/D37)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I37" t="e">
-        <f>G37/(C37/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3019,11 +3049,11 @@
         <v>43</v>
       </c>
       <c r="H38" t="e">
-        <f>(C38/D38)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I38" t="e">
-        <f>G38/(C38/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3035,11 +3065,11 @@
         <v>40</v>
       </c>
       <c r="H39" t="e">
-        <f>(C39/D39)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I39" t="e">
-        <f>G39/(C39/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3051,11 +3081,11 @@
         <v>41</v>
       </c>
       <c r="H40" t="e">
-        <f>(C40/D40)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I40" t="e">
-        <f>G40/(C40/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3067,11 +3097,11 @@
         <v>42</v>
       </c>
       <c r="H41" t="e">
-        <f>(C41/D41)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I41" t="e">
-        <f>G41/(C41/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3083,11 +3113,11 @@
         <v>43</v>
       </c>
       <c r="H42" t="e">
-        <f>(C42/D42)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I42" t="e">
-        <f>G42/(C42/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3099,11 +3129,11 @@
         <v>40</v>
       </c>
       <c r="H43" t="e">
-        <f>(C43/D43)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I43" t="e">
-        <f>G43/(C43/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3115,11 +3145,11 @@
         <v>41</v>
       </c>
       <c r="H44" t="e">
-        <f>(C44/D44)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I44" t="e">
-        <f>G44/(C44/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3131,11 +3161,11 @@
         <v>42</v>
       </c>
       <c r="H45" t="e">
-        <f>(C45/D45)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I45" t="e">
-        <f>G45/(C45/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3147,11 +3177,11 @@
         <v>43</v>
       </c>
       <c r="H46" t="e">
-        <f>(C46/D46)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I46" t="e">
-        <f>G46/(C46/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3163,11 +3193,11 @@
         <v>40</v>
       </c>
       <c r="H47" t="e">
-        <f>(C47/D47)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I47" t="e">
-        <f>G47/(C47/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3179,11 +3209,11 @@
         <v>41</v>
       </c>
       <c r="H48" t="e">
-        <f>(C48/D48)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I48" t="e">
-        <f>G48/(C48/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3195,11 +3225,11 @@
         <v>42</v>
       </c>
       <c r="H49" t="e">
-        <f>(C49/D49)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I49" t="e">
-        <f>G49/(C49/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3211,11 +3241,11 @@
         <v>43</v>
       </c>
       <c r="H50" t="e">
-        <f>(C50/D50)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I50" t="e">
-        <f>G50/(C50/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3227,11 +3257,11 @@
         <v>40</v>
       </c>
       <c r="H51" t="e">
-        <f>(C51/D51)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I51" t="e">
-        <f>G51/(C51/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3243,11 +3273,11 @@
         <v>41</v>
       </c>
       <c r="H52" t="e">
-        <f>(C52/D52)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I52" t="e">
-        <f>G52/(C52/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3259,11 +3289,11 @@
         <v>42</v>
       </c>
       <c r="H53" t="e">
-        <f>(C53/D53)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I53" t="e">
-        <f>G53/(C53/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3275,11 +3305,11 @@
         <v>43</v>
       </c>
       <c r="H54" t="e">
-        <f>(C54/D54)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I54" t="e">
-        <f>G54/(C54/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3291,11 +3321,11 @@
         <v>40</v>
       </c>
       <c r="H55" t="e">
-        <f>(C55/D55)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I55" t="e">
-        <f>G55/(C55/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3307,11 +3337,11 @@
         <v>41</v>
       </c>
       <c r="H56" t="e">
-        <f>(C56/D56)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I56" t="e">
-        <f>G56/(C56/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3323,11 +3353,11 @@
         <v>42</v>
       </c>
       <c r="H57" t="e">
-        <f>(C57/D57)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I57" t="e">
-        <f>G57/(C57/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3339,11 +3369,11 @@
         <v>43</v>
       </c>
       <c r="H58" t="e">
-        <f>(C58/D58)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I58" t="e">
-        <f>G58/(C58/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3355,11 +3385,11 @@
         <v>40</v>
       </c>
       <c r="H59" t="e">
-        <f>(C59/D59)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I59" t="e">
-        <f>G59/(C59/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3371,11 +3401,11 @@
         <v>41</v>
       </c>
       <c r="H60" t="e">
-        <f>(C60/D60)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I60" t="e">
-        <f>G60/(C60/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3387,11 +3417,11 @@
         <v>42</v>
       </c>
       <c r="H61" t="e">
-        <f>(C61/D61)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I61" t="e">
-        <f>G61/(C61/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3403,11 +3433,11 @@
         <v>43</v>
       </c>
       <c r="H62" t="e">
-        <f>(C62/D62)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I62" t="e">
-        <f>G62/(C62/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3419,11 +3449,11 @@
         <v>40</v>
       </c>
       <c r="H63" t="e">
-        <f>(C63/D63)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I63" t="e">
-        <f>G63/(C63/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3435,11 +3465,11 @@
         <v>41</v>
       </c>
       <c r="H64" t="e">
-        <f>(C64/D64)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I64" t="e">
-        <f>G64/(C64/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3451,11 +3481,11 @@
         <v>42</v>
       </c>
       <c r="H65" t="e">
-        <f>(C65/D65)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I65" t="e">
-        <f>G65/(C65/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3467,11 +3497,11 @@
         <v>43</v>
       </c>
       <c r="H66" t="e">
-        <f>(C66/D66)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I66" t="e">
-        <f>G66/(C66/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3483,11 +3513,11 @@
         <v>40</v>
       </c>
       <c r="H67" t="e">
-        <f>(C67/D67)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I67" t="e">
-        <f>G67/(C67/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3499,11 +3529,11 @@
         <v>41</v>
       </c>
       <c r="H68" t="e">
-        <f t="shared" ref="H68:H86" si="0">(C68/D68)</f>
+        <f t="shared" ref="H68:H86" si="4">(C68/D68)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I68" t="e">
-        <f t="shared" ref="I68:I86" si="1">G68/(C68/1000)</f>
+        <f t="shared" ref="I68:I86" si="5">G68/(C68/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3515,11 +3545,11 @@
         <v>42</v>
       </c>
       <c r="H69" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I69" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3531,11 +3561,11 @@
         <v>43</v>
       </c>
       <c r="H70" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I70" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3547,11 +3577,11 @@
         <v>40</v>
       </c>
       <c r="H71" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I71" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3563,11 +3593,11 @@
         <v>41</v>
       </c>
       <c r="H72" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I72" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3579,11 +3609,11 @@
         <v>42</v>
       </c>
       <c r="H73" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I73" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3595,11 +3625,11 @@
         <v>43</v>
       </c>
       <c r="H74" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I74" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3611,11 +3641,11 @@
         <v>40</v>
       </c>
       <c r="H75" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I75" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3627,11 +3657,11 @@
         <v>41</v>
       </c>
       <c r="H76" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I76" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3643,11 +3673,11 @@
         <v>42</v>
       </c>
       <c r="H77" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I77" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3659,11 +3689,11 @@
         <v>43</v>
       </c>
       <c r="H78" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I78" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3675,11 +3705,11 @@
         <v>40</v>
       </c>
       <c r="H79" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I79" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3691,11 +3721,11 @@
         <v>41</v>
       </c>
       <c r="H80" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I80" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3707,11 +3737,11 @@
         <v>42</v>
       </c>
       <c r="H81" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I81" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3723,11 +3753,11 @@
         <v>43</v>
       </c>
       <c r="H82" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I82" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3739,11 +3769,11 @@
         <v>40</v>
       </c>
       <c r="H83" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I83" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3755,11 +3785,11 @@
         <v>41</v>
       </c>
       <c r="H84" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I84" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3771,11 +3801,11 @@
         <v>42</v>
       </c>
       <c r="H85" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I85" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3787,11 +3817,11 @@
         <v>43</v>
       </c>
       <c r="H86" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I86" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added SRRIP for both configs using bzip2 benchmark
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F608D3FD-6342-4168-81F8-77788D671EAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65F35AA-EB2F-4177-8948-506DA409B6F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
@@ -862,7 +862,7 @@
   <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -936,11 +936,11 @@
         <v>117826</v>
       </c>
       <c r="H3">
-        <f>(C3/D3)</f>
+        <f t="shared" ref="H3:H34" si="0">(C3/D3)</f>
         <v>0.34633020974435469</v>
       </c>
       <c r="I3">
-        <f>G3/(C3/1000)</f>
+        <f t="shared" ref="I3:I34" si="1">G3/(C3/1000)</f>
         <v>2.3565199057392037</v>
       </c>
     </row>
@@ -967,11 +967,11 @@
         <v>125629</v>
       </c>
       <c r="H4">
-        <f>(C4/D4)</f>
+        <f t="shared" si="0"/>
         <v>0.34548741663363058</v>
       </c>
       <c r="I4">
-        <f>G4/(C4/1000)</f>
+        <f t="shared" si="1"/>
         <v>2.5125798994968038</v>
       </c>
     </row>
@@ -998,11 +998,11 @@
         <v>125644</v>
       </c>
       <c r="H5">
-        <f>(C5/D5)</f>
+        <f t="shared" si="0"/>
         <v>0.34572279553239044</v>
       </c>
       <c r="I5">
-        <f>G5/(C5/1000)</f>
+        <f t="shared" si="1"/>
         <v>2.5128798994848038</v>
       </c>
     </row>
@@ -1030,11 +1030,11 @@
         <v>3661</v>
       </c>
       <c r="H6">
-        <f>(C6/D6)</f>
+        <f t="shared" si="0"/>
         <v>0.34572279553239044</v>
       </c>
       <c r="I6">
-        <f>G6/(C6/1000)</f>
+        <f t="shared" si="1"/>
         <v>7.321999707120011E-2</v>
       </c>
       <c r="J6">
@@ -1065,11 +1065,11 @@
         <v>72655</v>
       </c>
       <c r="H7">
-        <f>(C7/D7)</f>
+        <f t="shared" si="0"/>
         <v>0.71952828359855603</v>
       </c>
       <c r="I7">
-        <f>G7/(C7/1000)</f>
+        <f t="shared" si="1"/>
         <v>1.4530999709380006</v>
       </c>
     </row>
@@ -1080,13 +1080,28 @@
       <c r="B8" t="s">
         <v>41</v>
       </c>
-      <c r="H8" t="e">
-        <f>(C8/D8)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I8" t="e">
-        <f>G8/(C8/1000)</f>
-        <v>#DIV/0!</v>
+      <c r="C8">
+        <v>50000001</v>
+      </c>
+      <c r="D8">
+        <v>70101084</v>
+      </c>
+      <c r="E8">
+        <v>620426</v>
+      </c>
+      <c r="F8">
+        <v>539473</v>
+      </c>
+      <c r="G8">
+        <v>80953</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0.71325574651598822</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>1.6190599676188007</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -1097,11 +1112,11 @@
         <v>42</v>
       </c>
       <c r="H9" t="e">
-        <f>(C9/D9)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I9" t="e">
-        <f>G9/(C9/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1113,11 +1128,11 @@
         <v>43</v>
       </c>
       <c r="H10" t="e">
-        <f>(C10/D10)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I10" t="e">
-        <f>G10/(C10/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1129,11 +1144,11 @@
         <v>40</v>
       </c>
       <c r="H11" t="e">
-        <f>(C11/D11)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I11" t="e">
-        <f>G11/(C11/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1145,11 +1160,11 @@
         <v>41</v>
       </c>
       <c r="H12" t="e">
-        <f>(C12/D12)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I12" t="e">
-        <f>G12/(C12/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1161,11 +1176,11 @@
         <v>42</v>
       </c>
       <c r="H13" t="e">
-        <f>(C13/D13)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I13" t="e">
-        <f>G13/(C13/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1177,11 +1192,11 @@
         <v>43</v>
       </c>
       <c r="H14" t="e">
-        <f>(C14/D14)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I14" t="e">
-        <f>G14/(C14/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1193,11 +1208,11 @@
         <v>40</v>
       </c>
       <c r="H15" t="e">
-        <f>(C15/D15)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I15" t="e">
-        <f>G15/(C15/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1209,11 +1224,11 @@
         <v>41</v>
       </c>
       <c r="H16" t="e">
-        <f>(C16/D16)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I16" t="e">
-        <f>G16/(C16/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1225,11 +1240,11 @@
         <v>42</v>
       </c>
       <c r="H17" t="e">
-        <f>(C17/D17)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I17" t="e">
-        <f>G17/(C17/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1241,11 +1256,11 @@
         <v>43</v>
       </c>
       <c r="H18" t="e">
-        <f>(C18/D18)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I18" t="e">
-        <f>G18/(C18/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1257,11 +1272,11 @@
         <v>40</v>
       </c>
       <c r="H19" t="e">
-        <f>(C19/D19)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I19" t="e">
-        <f>G19/(C19/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1273,11 +1288,11 @@
         <v>41</v>
       </c>
       <c r="H20" t="e">
-        <f>(C20/D20)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I20" t="e">
-        <f>G20/(C20/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1289,11 +1304,11 @@
         <v>42</v>
       </c>
       <c r="H21" t="e">
-        <f>(C21/D21)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I21" t="e">
-        <f>G21/(C21/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1305,11 +1320,11 @@
         <v>43</v>
       </c>
       <c r="H22" t="e">
-        <f>(C22/D22)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I22" t="e">
-        <f>G22/(C22/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1321,11 +1336,11 @@
         <v>40</v>
       </c>
       <c r="H23" t="e">
-        <f>(C23/D23)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I23" t="e">
-        <f>G23/(C23/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1337,11 +1352,11 @@
         <v>41</v>
       </c>
       <c r="H24" t="e">
-        <f>(C24/D24)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I24" t="e">
-        <f>G24/(C24/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1353,11 +1368,11 @@
         <v>42</v>
       </c>
       <c r="H25" t="e">
-        <f>(C25/D25)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I25" t="e">
-        <f>G25/(C25/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1369,11 +1384,11 @@
         <v>43</v>
       </c>
       <c r="H26" t="e">
-        <f>(C26/D26)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I26" t="e">
-        <f>G26/(C26/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1385,11 +1400,11 @@
         <v>40</v>
       </c>
       <c r="H27" t="e">
-        <f>(C27/D27)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I27" t="e">
-        <f>G27/(C27/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1401,11 +1416,11 @@
         <v>41</v>
       </c>
       <c r="H28" t="e">
-        <f>(C28/D28)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I28" t="e">
-        <f>G28/(C28/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1417,11 +1432,11 @@
         <v>42</v>
       </c>
       <c r="H29" t="e">
-        <f>(C29/D29)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I29" t="e">
-        <f>G29/(C29/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1433,11 +1448,11 @@
         <v>43</v>
       </c>
       <c r="H30" t="e">
-        <f>(C30/D30)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I30" t="e">
-        <f>G30/(C30/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1449,11 +1464,11 @@
         <v>40</v>
       </c>
       <c r="H31" t="e">
-        <f>(C31/D31)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I31" t="e">
-        <f>G31/(C31/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1465,11 +1480,11 @@
         <v>41</v>
       </c>
       <c r="H32" t="e">
-        <f>(C32/D32)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I32" t="e">
-        <f>G32/(C32/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1481,11 +1496,11 @@
         <v>42</v>
       </c>
       <c r="H33" t="e">
-        <f>(C33/D33)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I33" t="e">
-        <f>G33/(C33/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1497,11 +1512,11 @@
         <v>43</v>
       </c>
       <c r="H34" t="e">
-        <f>(C34/D34)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I34" t="e">
-        <f>G34/(C34/1000)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1513,11 +1528,11 @@
         <v>40</v>
       </c>
       <c r="H35" t="e">
-        <f>(C35/D35)</f>
+        <f t="shared" ref="H35:H67" si="2">(C35/D35)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I35" t="e">
-        <f>G35/(C35/1000)</f>
+        <f t="shared" ref="I35:I67" si="3">G35/(C35/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1529,11 +1544,11 @@
         <v>41</v>
       </c>
       <c r="H36" t="e">
-        <f>(C36/D36)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I36" t="e">
-        <f>G36/(C36/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1545,11 +1560,11 @@
         <v>42</v>
       </c>
       <c r="H37" t="e">
-        <f>(C37/D37)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I37" t="e">
-        <f>G37/(C37/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1561,11 +1576,11 @@
         <v>43</v>
       </c>
       <c r="H38" t="e">
-        <f>(C38/D38)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I38" t="e">
-        <f>G38/(C38/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1577,11 +1592,11 @@
         <v>40</v>
       </c>
       <c r="H39" t="e">
-        <f>(C39/D39)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I39" t="e">
-        <f>G39/(C39/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1593,11 +1608,11 @@
         <v>41</v>
       </c>
       <c r="H40" t="e">
-        <f>(C40/D40)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I40" t="e">
-        <f>G40/(C40/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1609,11 +1624,11 @@
         <v>42</v>
       </c>
       <c r="H41" t="e">
-        <f>(C41/D41)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I41" t="e">
-        <f>G41/(C41/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1625,11 +1640,11 @@
         <v>43</v>
       </c>
       <c r="H42" t="e">
-        <f>(C42/D42)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I42" t="e">
-        <f>G42/(C42/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1641,11 +1656,11 @@
         <v>40</v>
       </c>
       <c r="H43" t="e">
-        <f>(C43/D43)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I43" t="e">
-        <f>G43/(C43/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1657,11 +1672,11 @@
         <v>41</v>
       </c>
       <c r="H44" t="e">
-        <f>(C44/D44)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I44" t="e">
-        <f>G44/(C44/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1673,11 +1688,11 @@
         <v>42</v>
       </c>
       <c r="H45" t="e">
-        <f>(C45/D45)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I45" t="e">
-        <f>G45/(C45/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1689,11 +1704,11 @@
         <v>43</v>
       </c>
       <c r="H46" t="e">
-        <f>(C46/D46)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I46" t="e">
-        <f>G46/(C46/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1705,11 +1720,11 @@
         <v>40</v>
       </c>
       <c r="H47" t="e">
-        <f>(C47/D47)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I47" t="e">
-        <f>G47/(C47/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1721,11 +1736,11 @@
         <v>41</v>
       </c>
       <c r="H48" t="e">
-        <f>(C48/D48)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I48" t="e">
-        <f>G48/(C48/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1737,11 +1752,11 @@
         <v>42</v>
       </c>
       <c r="H49" t="e">
-        <f>(C49/D49)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I49" t="e">
-        <f>G49/(C49/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1753,11 +1768,11 @@
         <v>43</v>
       </c>
       <c r="H50" t="e">
-        <f>(C50/D50)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I50" t="e">
-        <f>G50/(C50/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1769,11 +1784,11 @@
         <v>40</v>
       </c>
       <c r="H51" t="e">
-        <f>(C51/D51)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I51" t="e">
-        <f>G51/(C51/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1785,11 +1800,11 @@
         <v>41</v>
       </c>
       <c r="H52" t="e">
-        <f>(C52/D52)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I52" t="e">
-        <f>G52/(C52/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1801,11 +1816,11 @@
         <v>42</v>
       </c>
       <c r="H53" t="e">
-        <f>(C53/D53)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I53" t="e">
-        <f>G53/(C53/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1817,11 +1832,11 @@
         <v>43</v>
       </c>
       <c r="H54" t="e">
-        <f>(C54/D54)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I54" t="e">
-        <f>G54/(C54/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1833,11 +1848,11 @@
         <v>40</v>
       </c>
       <c r="H55" t="e">
-        <f>(C55/D55)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I55" t="e">
-        <f>G55/(C55/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1849,11 +1864,11 @@
         <v>41</v>
       </c>
       <c r="H56" t="e">
-        <f>(C56/D56)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I56" t="e">
-        <f>G56/(C56/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1865,11 +1880,11 @@
         <v>42</v>
       </c>
       <c r="H57" t="e">
-        <f>(C57/D57)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I57" t="e">
-        <f>G57/(C57/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1881,11 +1896,11 @@
         <v>43</v>
       </c>
       <c r="H58" t="e">
-        <f>(C58/D58)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I58" t="e">
-        <f>G58/(C58/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1897,11 +1912,11 @@
         <v>40</v>
       </c>
       <c r="H59" t="e">
-        <f>(C59/D59)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I59" t="e">
-        <f>G59/(C59/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1913,11 +1928,11 @@
         <v>41</v>
       </c>
       <c r="H60" t="e">
-        <f>(C60/D60)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I60" t="e">
-        <f>G60/(C60/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1929,11 +1944,11 @@
         <v>42</v>
       </c>
       <c r="H61" t="e">
-        <f>(C61/D61)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I61" t="e">
-        <f>G61/(C61/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1945,11 +1960,11 @@
         <v>43</v>
       </c>
       <c r="H62" t="e">
-        <f>(C62/D62)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I62" t="e">
-        <f>G62/(C62/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1961,11 +1976,11 @@
         <v>40</v>
       </c>
       <c r="H63" t="e">
-        <f>(C63/D63)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I63" t="e">
-        <f>G63/(C63/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1977,11 +1992,11 @@
         <v>41</v>
       </c>
       <c r="H64" t="e">
-        <f>(C64/D64)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I64" t="e">
-        <f>G64/(C64/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1993,11 +2008,11 @@
         <v>42</v>
       </c>
       <c r="H65" t="e">
-        <f>(C65/D65)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I65" t="e">
-        <f>G65/(C65/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2009,11 +2024,11 @@
         <v>43</v>
       </c>
       <c r="H66" t="e">
-        <f>(C66/D66)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I66" t="e">
-        <f>G66/(C66/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2025,11 +2040,11 @@
         <v>40</v>
       </c>
       <c r="H67" t="e">
-        <f>(C67/D67)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I67" t="e">
-        <f>G67/(C67/1000)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2041,11 +2056,11 @@
         <v>41</v>
       </c>
       <c r="H68" t="e">
-        <f t="shared" ref="H68:H86" si="0">(C68/D68)</f>
+        <f t="shared" ref="H68:H86" si="4">(C68/D68)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I68" t="e">
-        <f t="shared" ref="I68:I86" si="1">G68/(C68/1000)</f>
+        <f t="shared" ref="I68:I86" si="5">G68/(C68/1000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2057,11 +2072,11 @@
         <v>42</v>
       </c>
       <c r="H69" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I69" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2073,11 +2088,11 @@
         <v>43</v>
       </c>
       <c r="H70" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I70" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2089,11 +2104,11 @@
         <v>40</v>
       </c>
       <c r="H71" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I71" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2105,11 +2120,11 @@
         <v>41</v>
       </c>
       <c r="H72" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I72" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2121,11 +2136,11 @@
         <v>42</v>
       </c>
       <c r="H73" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I73" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2137,11 +2152,11 @@
         <v>43</v>
       </c>
       <c r="H74" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I74" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2153,11 +2168,11 @@
         <v>40</v>
       </c>
       <c r="H75" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I75" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2169,11 +2184,11 @@
         <v>41</v>
       </c>
       <c r="H76" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I76" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2185,11 +2200,11 @@
         <v>42</v>
       </c>
       <c r="H77" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I77" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2201,11 +2216,11 @@
         <v>43</v>
       </c>
       <c r="H78" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I78" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2217,11 +2232,11 @@
         <v>40</v>
       </c>
       <c r="H79" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I79" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2233,11 +2248,11 @@
         <v>41</v>
       </c>
       <c r="H80" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I80" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2249,11 +2264,11 @@
         <v>42</v>
       </c>
       <c r="H81" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I81" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2265,11 +2280,11 @@
         <v>43</v>
       </c>
       <c r="H82" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I82" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2281,11 +2296,11 @@
         <v>40</v>
       </c>
       <c r="H83" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I83" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2297,11 +2312,11 @@
         <v>41</v>
       </c>
       <c r="H84" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I84" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2313,11 +2328,11 @@
         <v>42</v>
       </c>
       <c r="H85" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I85" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2329,11 +2344,11 @@
         <v>43</v>
       </c>
       <c r="H86" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I86" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2351,7 +2366,7 @@
   <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2568,13 +2583,28 @@
       <c r="B8" t="s">
         <v>41</v>
       </c>
-      <c r="H8" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I8" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C8">
+        <v>50000001</v>
+      </c>
+      <c r="D8">
+        <v>67777918</v>
+      </c>
+      <c r="E8">
+        <v>854509</v>
+      </c>
+      <c r="F8">
+        <v>766412</v>
+      </c>
+      <c r="G8">
+        <v>88097</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0.73770340658737854</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>1.7619399647612008</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added Hawkeye for both configs using bzip2 benchmark
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65F35AA-EB2F-4177-8948-506DA409B6F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C2BDF0-FAE0-489C-AD8B-877C0DC40C37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
@@ -862,7 +862,7 @@
   <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1111,13 +1111,28 @@
       <c r="B9" t="s">
         <v>42</v>
       </c>
-      <c r="H9" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I9" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C9">
+        <v>50000001</v>
+      </c>
+      <c r="D9">
+        <v>68593474</v>
+      </c>
+      <c r="E9">
+        <v>620418</v>
+      </c>
+      <c r="F9">
+        <v>560367</v>
+      </c>
+      <c r="G9">
+        <v>60051</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>0.72893233254230572</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>1.2010199759796005</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -1127,13 +1142,33 @@
       <c r="B10" t="s">
         <v>43</v>
       </c>
-      <c r="H10" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C10">
+        <v>50000001</v>
+      </c>
+      <c r="D10">
+        <v>68593474</v>
+      </c>
+      <c r="E10">
+        <v>12097</v>
+      </c>
+      <c r="F10">
+        <v>10446</v>
+      </c>
+      <c r="G10">
+        <f>E10-F10</f>
+        <v>1651</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>0.72893233254230572</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>3.3019999339600016E-2</v>
+      </c>
+      <c r="J10">
+        <f>F10/E10</f>
+        <v>0.86351988096222199</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -2366,7 +2401,7 @@
   <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2614,13 +2649,28 @@
       <c r="B9" t="s">
         <v>42</v>
       </c>
-      <c r="H9" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I9" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C9">
+        <v>50000001</v>
+      </c>
+      <c r="D9">
+        <v>66883100</v>
+      </c>
+      <c r="E9">
+        <v>853878</v>
+      </c>
+      <c r="F9">
+        <v>787833</v>
+      </c>
+      <c r="G9">
+        <v>66045</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>0.7475730191931893</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>1.3208999735820006</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -2630,13 +2680,33 @@
       <c r="B10" t="s">
         <v>43</v>
       </c>
-      <c r="H10" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C10">
+        <v>50000001</v>
+      </c>
+      <c r="D10">
+        <v>66883100</v>
+      </c>
+      <c r="E10">
+        <v>10725</v>
+      </c>
+      <c r="F10">
+        <v>12081</v>
+      </c>
+      <c r="G10">
+        <f>E10-F10</f>
+        <v>-1356</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>0.7475730191931893</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>-2.7119999457600012E-2</v>
+      </c>
+      <c r="J10">
+        <f>F10/E10</f>
+        <v>1.1264335664335665</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added LRU for both configs on calculix benchmark
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C2BDF0-FAE0-489C-AD8B-877C0DC40C37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4650AB7-12CA-4BEF-B9F0-E10BF0F12EEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
@@ -862,7 +862,7 @@
   <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1178,13 +1178,28 @@
       <c r="B11" t="s">
         <v>40</v>
       </c>
-      <c r="H11" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I11" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C11">
+        <v>50000001</v>
+      </c>
+      <c r="D11">
+        <v>31836870</v>
+      </c>
+      <c r="E11">
+        <v>405396</v>
+      </c>
+      <c r="F11">
+        <v>341068</v>
+      </c>
+      <c r="G11">
+        <v>64328</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>1.5705061772718236</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>1.2865599742688005</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -2401,7 +2416,7 @@
   <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2716,13 +2731,28 @@
       <c r="B11" t="s">
         <v>40</v>
       </c>
-      <c r="H11" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I11" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C11">
+        <v>50000000</v>
+      </c>
+      <c r="D11">
+        <v>24198526</v>
+      </c>
+      <c r="E11">
+        <v>425231</v>
+      </c>
+      <c r="F11">
+        <v>359739</v>
+      </c>
+      <c r="G11">
+        <v>65492</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>2.0662415553740754</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>1.3098399999999999</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added SRRIP results for both configs on calculix benchmark
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4650AB7-12CA-4BEF-B9F0-E10BF0F12EEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D347BD-DA9B-40DA-8D8C-BC7FC63BF598}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
@@ -862,7 +862,7 @@
   <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1209,13 +1209,28 @@
       <c r="B12" t="s">
         <v>41</v>
       </c>
-      <c r="H12" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I12" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C12">
+        <v>50000001</v>
+      </c>
+      <c r="D12">
+        <v>31741436</v>
+      </c>
+      <c r="E12">
+        <v>405396</v>
+      </c>
+      <c r="F12">
+        <v>351651</v>
+      </c>
+      <c r="G12">
+        <v>63745</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>1.5752280709669215</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>1.2748999745020007</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -2416,7 +2431,7 @@
   <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2762,13 +2777,28 @@
       <c r="B12" t="s">
         <v>41</v>
       </c>
-      <c r="H12" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I12" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C12">
+        <v>50000000</v>
+      </c>
+      <c r="D12">
+        <v>24173346</v>
+      </c>
+      <c r="E12">
+        <v>425232</v>
+      </c>
+      <c r="F12">
+        <v>360877</v>
+      </c>
+      <c r="G12">
+        <v>64355</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>2.0683938417131</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>1.2870999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added Hawkeye simulation results for both configs for calculix benchmark
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D347BD-DA9B-40DA-8D8C-BC7FC63BF598}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB98BF6C-B9CC-4F47-88F6-90AB56966FE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
@@ -862,7 +862,7 @@
   <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1178,29 +1178,6 @@
       <c r="B11" t="s">
         <v>40</v>
       </c>
-      <c r="C11">
-        <v>50000001</v>
-      </c>
-      <c r="D11">
-        <v>31836870</v>
-      </c>
-      <c r="E11">
-        <v>405396</v>
-      </c>
-      <c r="F11">
-        <v>341068</v>
-      </c>
-      <c r="G11">
-        <v>64328</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="0"/>
-        <v>1.5705061772718236</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="1"/>
-        <v>1.2865599742688005</v>
-      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -1209,29 +1186,6 @@
       <c r="B12" t="s">
         <v>41</v>
       </c>
-      <c r="C12">
-        <v>50000001</v>
-      </c>
-      <c r="D12">
-        <v>31741436</v>
-      </c>
-      <c r="E12">
-        <v>405396</v>
-      </c>
-      <c r="F12">
-        <v>351651</v>
-      </c>
-      <c r="G12">
-        <v>63745</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="0"/>
-        <v>1.5752280709669215</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="1"/>
-        <v>1.2748999745020007</v>
-      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -1240,14 +1194,6 @@
       <c r="B13" t="s">
         <v>42</v>
       </c>
-      <c r="H13" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I13" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -1256,14 +1202,6 @@
       <c r="B14" t="s">
         <v>43</v>
       </c>
-      <c r="H14" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I14" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -1272,13 +1210,28 @@
       <c r="B15" t="s">
         <v>40</v>
       </c>
-      <c r="H15" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I15" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C15">
+        <v>50000001</v>
+      </c>
+      <c r="D15">
+        <v>31836870</v>
+      </c>
+      <c r="E15">
+        <v>405396</v>
+      </c>
+      <c r="F15">
+        <v>341068</v>
+      </c>
+      <c r="G15">
+        <v>64328</v>
+      </c>
+      <c r="H15">
+        <f>(C15/D15)</f>
+        <v>1.5705061772718236</v>
+      </c>
+      <c r="I15">
+        <f>G15/(C15/1000)</f>
+        <v>1.2865599742688005</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -1288,48 +1241,98 @@
       <c r="B16" t="s">
         <v>41</v>
       </c>
-      <c r="H16" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I16" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>50000001</v>
+      </c>
+      <c r="D16">
+        <v>31741436</v>
+      </c>
+      <c r="E16">
+        <v>405396</v>
+      </c>
+      <c r="F16">
+        <v>351651</v>
+      </c>
+      <c r="G16">
+        <v>63745</v>
+      </c>
+      <c r="H16">
+        <f>(C16/D16)</f>
+        <v>1.5752280709669215</v>
+      </c>
+      <c r="I16">
+        <f>G16/(C16/1000)</f>
+        <v>1.2748999745020007</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>6</v>
       </c>
       <c r="B17" t="s">
         <v>42</v>
       </c>
-      <c r="H17" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I17" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>50000001</v>
+      </c>
+      <c r="D17">
+        <v>32754975</v>
+      </c>
+      <c r="E17">
+        <v>405396</v>
+      </c>
+      <c r="F17">
+        <v>326734</v>
+      </c>
+      <c r="G17">
+        <v>78662</v>
+      </c>
+      <c r="H17">
+        <f>(C17/D17)</f>
+        <v>1.5264857017903388</v>
+      </c>
+      <c r="I17">
+        <f>G17/(C17/1000)</f>
+        <v>1.5732399685352008</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>6</v>
       </c>
       <c r="B18" t="s">
         <v>43</v>
       </c>
-      <c r="H18" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I18" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>50000001</v>
+      </c>
+      <c r="D18">
+        <v>32754975</v>
+      </c>
+      <c r="E18">
+        <v>12640</v>
+      </c>
+      <c r="F18">
+        <v>10695</v>
+      </c>
+      <c r="G18">
+        <f>E18-F18</f>
+        <v>1945</v>
+      </c>
+      <c r="H18">
+        <f>(C18/D18)</f>
+        <v>1.5264857017903388</v>
+      </c>
+      <c r="I18">
+        <f>G18/(C18/1000)</f>
+        <v>3.889999922200002E-2</v>
+      </c>
+      <c r="J18">
+        <f>F18/E18</f>
+        <v>0.846123417721519</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1345,7 +1348,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1361,7 +1364,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1377,7 +1380,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1393,7 +1396,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1409,7 +1412,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1425,7 +1428,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1441,7 +1444,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1457,7 +1460,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1473,7 +1476,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -1489,7 +1492,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1505,7 +1508,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1521,7 +1524,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -1537,7 +1540,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -2431,7 +2434,7 @@
   <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2746,29 +2749,6 @@
       <c r="B11" t="s">
         <v>40</v>
       </c>
-      <c r="C11">
-        <v>50000000</v>
-      </c>
-      <c r="D11">
-        <v>24198526</v>
-      </c>
-      <c r="E11">
-        <v>425231</v>
-      </c>
-      <c r="F11">
-        <v>359739</v>
-      </c>
-      <c r="G11">
-        <v>65492</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="0"/>
-        <v>2.0662415553740754</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="1"/>
-        <v>1.3098399999999999</v>
-      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -2777,29 +2757,6 @@
       <c r="B12" t="s">
         <v>41</v>
       </c>
-      <c r="C12">
-        <v>50000000</v>
-      </c>
-      <c r="D12">
-        <v>24173346</v>
-      </c>
-      <c r="E12">
-        <v>425232</v>
-      </c>
-      <c r="F12">
-        <v>360877</v>
-      </c>
-      <c r="G12">
-        <v>64355</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="0"/>
-        <v>2.0683938417131</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="1"/>
-        <v>1.2870999999999999</v>
-      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -2808,14 +2765,6 @@
       <c r="B13" t="s">
         <v>42</v>
       </c>
-      <c r="H13" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I13" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -2824,14 +2773,6 @@
       <c r="B14" t="s">
         <v>43</v>
       </c>
-      <c r="H14" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I14" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -2840,13 +2781,28 @@
       <c r="B15" t="s">
         <v>40</v>
       </c>
-      <c r="H15" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I15" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C15">
+        <v>50000000</v>
+      </c>
+      <c r="D15">
+        <v>24198526</v>
+      </c>
+      <c r="E15">
+        <v>425231</v>
+      </c>
+      <c r="F15">
+        <v>359739</v>
+      </c>
+      <c r="G15">
+        <v>65492</v>
+      </c>
+      <c r="H15">
+        <f>(C15/D15)</f>
+        <v>2.0662415553740754</v>
+      </c>
+      <c r="I15">
+        <f>G15/(C15/1000)</f>
+        <v>1.3098399999999999</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -2856,48 +2812,98 @@
       <c r="B16" t="s">
         <v>41</v>
       </c>
-      <c r="H16" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I16" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>50000000</v>
+      </c>
+      <c r="D16">
+        <v>24173346</v>
+      </c>
+      <c r="E16">
+        <v>425232</v>
+      </c>
+      <c r="F16">
+        <v>360877</v>
+      </c>
+      <c r="G16">
+        <v>64355</v>
+      </c>
+      <c r="H16">
+        <f>(C16/D16)</f>
+        <v>2.0683938417131</v>
+      </c>
+      <c r="I16">
+        <f>G16/(C16/1000)</f>
+        <v>1.2870999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>6</v>
       </c>
       <c r="B17" t="s">
         <v>42</v>
       </c>
-      <c r="H17" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I17" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>50000000</v>
+      </c>
+      <c r="D17">
+        <v>24656481</v>
+      </c>
+      <c r="E17">
+        <v>425232</v>
+      </c>
+      <c r="F17">
+        <v>341733</v>
+      </c>
+      <c r="G17">
+        <v>83499</v>
+      </c>
+      <c r="H17">
+        <f>(C17/D17)</f>
+        <v>2.0278643980055384</v>
+      </c>
+      <c r="I17">
+        <f>G17/(C17/1000)</f>
+        <v>1.66998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>6</v>
       </c>
       <c r="B18" t="s">
         <v>43</v>
       </c>
-      <c r="H18" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I18" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>50000000</v>
+      </c>
+      <c r="D18">
+        <v>24656481</v>
+      </c>
+      <c r="E18">
+        <v>2148</v>
+      </c>
+      <c r="F18">
+        <v>7035</v>
+      </c>
+      <c r="G18">
+        <f>E18-F18</f>
+        <v>-4887</v>
+      </c>
+      <c r="H18">
+        <f>(C18/D18)</f>
+        <v>2.0278643980055384</v>
+      </c>
+      <c r="I18">
+        <f>G18/(C18/1000)</f>
+        <v>-9.7739999999999994E-2</v>
+      </c>
+      <c r="J18">
+        <f>F18/E18</f>
+        <v>3.2751396648044691</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -2913,7 +2919,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -2929,7 +2935,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -2945,7 +2951,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -2961,7 +2967,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -2977,7 +2983,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -2993,7 +2999,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -3009,7 +3015,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -3025,7 +3031,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -3041,7 +3047,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -3057,7 +3063,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -3073,7 +3079,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -3089,7 +3095,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -3105,7 +3111,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Added LRU results for both configs on gcc benchmark
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB98BF6C-B9CC-4F47-88F6-90AB56966FE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8449514-5054-46CC-9D19-DC65487C85BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Benchmarks" sheetId="2" r:id="rId1"/>
@@ -861,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4DAA02D-4B80-49E4-98A1-4EF8777A053B}">
   <dimension ref="A2:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1339,13 +1339,28 @@
       <c r="B19" t="s">
         <v>40</v>
       </c>
-      <c r="H19" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I19" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C19">
+        <v>50000000</v>
+      </c>
+      <c r="D19">
+        <v>183027013</v>
+      </c>
+      <c r="E19">
+        <v>249544</v>
+      </c>
+      <c r="F19">
+        <v>1811</v>
+      </c>
+      <c r="G19">
+        <v>247733</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>0.27318371851481837</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>4.9546599999999996</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -2433,8 +2448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E5CF80-89BD-41BF-8339-D77E14018905}">
   <dimension ref="A2:L86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2910,13 +2925,28 @@
       <c r="B19" t="s">
         <v>40</v>
       </c>
-      <c r="H19" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I19" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C19">
+        <v>50000000</v>
+      </c>
+      <c r="D19">
+        <v>178404939</v>
+      </c>
+      <c r="E19">
+        <v>388410</v>
+      </c>
+      <c r="F19">
+        <v>4081</v>
+      </c>
+      <c r="G19">
+        <v>384329</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>0.28026129926817778</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>7.6865800000000002</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added SRRIP results for both configs on gcc benchmark
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8449514-5054-46CC-9D19-DC65487C85BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5825709B-74EC-4C6B-BBCB-3F835CE7A5C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
@@ -862,7 +862,7 @@
   <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1370,13 +1370,28 @@
       <c r="B20" t="s">
         <v>41</v>
       </c>
-      <c r="H20" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I20" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C20">
+        <v>50000000</v>
+      </c>
+      <c r="D20">
+        <v>183028470</v>
+      </c>
+      <c r="E20">
+        <v>249544</v>
+      </c>
+      <c r="F20">
+        <v>2049</v>
+      </c>
+      <c r="G20">
+        <v>247495</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>0.2731815438330441</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>4.9499000000000004</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -2449,7 +2464,7 @@
   <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2956,13 +2971,28 @@
       <c r="B20" t="s">
         <v>41</v>
       </c>
-      <c r="H20" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I20" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C20">
+        <v>50000000</v>
+      </c>
+      <c r="D20">
+        <v>178389640</v>
+      </c>
+      <c r="E20">
+        <v>388410</v>
+      </c>
+      <c r="F20">
+        <v>4587</v>
+      </c>
+      <c r="G20">
+        <v>383823</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>0.28028533495555014</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>7.6764599999999996</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added Hawkeye simulation for both configs on gcc benchmark
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5825709B-74EC-4C6B-BBCB-3F835CE7A5C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9EC6DA-0233-494E-B4C5-5ABBC52D005D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
@@ -862,7 +862,7 @@
   <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1401,13 +1401,28 @@
       <c r="B21" t="s">
         <v>42</v>
       </c>
-      <c r="H21" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I21" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C21">
+        <v>50000000</v>
+      </c>
+      <c r="D21">
+        <v>181610645</v>
+      </c>
+      <c r="E21">
+        <v>249544</v>
+      </c>
+      <c r="F21">
+        <v>20244</v>
+      </c>
+      <c r="G21">
+        <v>229300</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>0.27531425814824895</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="1"/>
+        <v>4.5860000000000003</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -1417,13 +1432,33 @@
       <c r="B22" t="s">
         <v>43</v>
       </c>
-      <c r="H22" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I22" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C22">
+        <v>50000000</v>
+      </c>
+      <c r="D22">
+        <v>181610645</v>
+      </c>
+      <c r="E22">
+        <v>29056</v>
+      </c>
+      <c r="F22">
+        <v>4828</v>
+      </c>
+      <c r="G22">
+        <f>E22-F22</f>
+        <v>24228</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>0.27531425814824895</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="1"/>
+        <v>0.48455999999999999</v>
+      </c>
+      <c r="J22">
+        <f>F22/E22</f>
+        <v>0.16616189427312775</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -2463,8 +2498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E5CF80-89BD-41BF-8339-D77E14018905}">
   <dimension ref="A2:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3002,13 +3037,28 @@
       <c r="B21" t="s">
         <v>42</v>
       </c>
-      <c r="H21" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I21" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C21">
+        <v>50000000</v>
+      </c>
+      <c r="D21">
+        <v>177984613</v>
+      </c>
+      <c r="E21">
+        <v>388409</v>
+      </c>
+      <c r="F21">
+        <v>20202</v>
+      </c>
+      <c r="G21">
+        <v>368207</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>0.2809231604756755</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="1"/>
+        <v>7.3641399999999999</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -3018,13 +3068,33 @@
       <c r="B22" t="s">
         <v>43</v>
       </c>
-      <c r="H22" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I22" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C22">
+        <v>50000000</v>
+      </c>
+      <c r="D22">
+        <v>177984613</v>
+      </c>
+      <c r="E22">
+        <v>16566</v>
+      </c>
+      <c r="F22">
+        <v>2906</v>
+      </c>
+      <c r="G22">
+        <f>E22-F22</f>
+        <v>13660</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>0.2809231604756755</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="1"/>
+        <v>0.2732</v>
+      </c>
+      <c r="J22">
+        <f>F22/E22</f>
+        <v>0.17541953398527105</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added LRU simulation results to both configs for GemsFDTD
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9EC6DA-0233-494E-B4C5-5ABBC52D005D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BD1FF1-3098-4010-AE74-1908F0CFA4F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Benchmarks" sheetId="2" r:id="rId1"/>
@@ -861,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4DAA02D-4B80-49E4-98A1-4EF8777A053B}">
   <dimension ref="A2:L86"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1468,13 +1468,28 @@
       <c r="B23" t="s">
         <v>40</v>
       </c>
-      <c r="H23" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I23" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C23">
+        <v>50000001</v>
+      </c>
+      <c r="D23">
+        <v>176325149</v>
+      </c>
+      <c r="E23">
+        <v>2633224</v>
+      </c>
+      <c r="F23">
+        <v>743948</v>
+      </c>
+      <c r="G23">
+        <v>1889276</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>0.28356704238486141</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>37.785519244289617</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -2498,8 +2513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E5CF80-89BD-41BF-8339-D77E14018905}">
   <dimension ref="A2:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3104,13 +3119,28 @@
       <c r="B23" t="s">
         <v>40</v>
       </c>
-      <c r="H23" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I23" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C23">
+        <v>50000001</v>
+      </c>
+      <c r="D23">
+        <v>82264148</v>
+      </c>
+      <c r="E23">
+        <v>2703165</v>
+      </c>
+      <c r="F23">
+        <v>737636</v>
+      </c>
+      <c r="G23">
+        <v>1965529</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>0.60779819904048604</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>39.310579213788415</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added SRRIP simulation results for both configs for GemsFDTD
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BD1FF1-3098-4010-AE74-1908F0CFA4F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B6E077-B54A-4B5E-A0B9-DEEDEF4718F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
@@ -861,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4DAA02D-4B80-49E4-98A1-4EF8777A053B}">
   <dimension ref="A2:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1499,13 +1499,28 @@
       <c r="B24" t="s">
         <v>41</v>
       </c>
-      <c r="H24" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I24" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C24">
+        <v>50000001</v>
+      </c>
+      <c r="D24">
+        <v>177915746</v>
+      </c>
+      <c r="E24">
+        <v>2633224</v>
+      </c>
+      <c r="F24">
+        <v>716957</v>
+      </c>
+      <c r="G24">
+        <v>1916267</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>0.28103190484331836</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>38.325339233493217</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -2514,7 +2529,7 @@
   <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3150,13 +3165,28 @@
       <c r="B24" t="s">
         <v>41</v>
       </c>
-      <c r="H24" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I24" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C24">
+        <v>50000001</v>
+      </c>
+      <c r="D24">
+        <v>82957415</v>
+      </c>
+      <c r="E24">
+        <v>2703160</v>
+      </c>
+      <c r="F24">
+        <v>717098</v>
+      </c>
+      <c r="G24">
+        <v>1986062</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>0.6027188889624876</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>39.721239205575216</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Adding Hawkeye results for both configs of Gem
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B6E077-B54A-4B5E-A0B9-DEEDEF4718F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE65A1B-6BD0-4041-9E41-5C6FE2DB1121}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
@@ -862,7 +862,7 @@
   <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1530,13 +1530,28 @@
       <c r="B25" t="s">
         <v>42</v>
       </c>
-      <c r="H25" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I25" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C25">
+        <v>50000001</v>
+      </c>
+      <c r="D25">
+        <v>151789738</v>
+      </c>
+      <c r="E25">
+        <v>2633225</v>
+      </c>
+      <c r="F25">
+        <v>582227</v>
+      </c>
+      <c r="G25">
+        <v>2050998</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>0.32940303909082447</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="1"/>
+        <v>41.019959179600818</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -1546,13 +1561,33 @@
       <c r="B26" t="s">
         <v>43</v>
       </c>
-      <c r="H26" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I26" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C26">
+        <v>50000001</v>
+      </c>
+      <c r="D26">
+        <v>151789738</v>
+      </c>
+      <c r="E26">
+        <v>47832</v>
+      </c>
+      <c r="F26">
+        <v>12892</v>
+      </c>
+      <c r="G26">
+        <f>E26-F26</f>
+        <v>34940</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>0.32940303909082447</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="1"/>
+        <v>0.69879998602400029</v>
+      </c>
+      <c r="J26">
+        <f>F26/E26</f>
+        <v>0.26952667670178959</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -2529,7 +2564,7 @@
   <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3196,13 +3231,28 @@
       <c r="B25" t="s">
         <v>42</v>
       </c>
-      <c r="H25" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I25" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C25">
+        <v>50000001</v>
+      </c>
+      <c r="D25">
+        <v>80542122</v>
+      </c>
+      <c r="E25">
+        <v>2703163</v>
+      </c>
+      <c r="F25">
+        <v>101472</v>
+      </c>
+      <c r="G25">
+        <v>2601691</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>0.62079319191515714</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="1"/>
+        <v>52.033818959323625</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -3212,13 +3262,33 @@
       <c r="B26" t="s">
         <v>43</v>
       </c>
-      <c r="H26" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I26" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C26">
+        <v>50000001</v>
+      </c>
+      <c r="D26">
+        <v>80542122</v>
+      </c>
+      <c r="E26">
+        <v>9064</v>
+      </c>
+      <c r="F26">
+        <v>2963</v>
+      </c>
+      <c r="G26">
+        <f>E26-F26</f>
+        <v>6101</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>0.62079319191515714</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="1"/>
+        <v>0.12201999755960005</v>
+      </c>
+      <c r="J26">
+        <f>F26/E26</f>
+        <v>0.32689761694616065</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added LRU resutls for both configs on h264 benchmark
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE65A1B-6BD0-4041-9E41-5C6FE2DB1121}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0C4379-DA0E-4182-9BC2-B96F034387D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Benchmarks" sheetId="2" r:id="rId1"/>
@@ -861,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4DAA02D-4B80-49E4-98A1-4EF8777A053B}">
   <dimension ref="A2:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1725,13 +1725,28 @@
       <c r="B35" t="s">
         <v>40</v>
       </c>
-      <c r="H35" t="e">
+      <c r="C35">
+        <v>50000002</v>
+      </c>
+      <c r="D35">
+        <v>57664446</v>
+      </c>
+      <c r="E35">
+        <v>143904</v>
+      </c>
+      <c r="F35">
+        <v>109064</v>
+      </c>
+      <c r="G35">
+        <v>34840</v>
+      </c>
+      <c r="H35">
         <f t="shared" ref="H35:H67" si="2">(C35/D35)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I35" t="e">
+        <v>0.86708544811130239</v>
+      </c>
+      <c r="I35">
         <f t="shared" ref="I35:I67" si="3">G35/(C35/1000)</f>
-        <v>#DIV/0!</v>
+        <v>0.69679997212800115</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
@@ -2563,8 +2578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E5CF80-89BD-41BF-8339-D77E14018905}">
   <dimension ref="A2:L86"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3426,13 +3441,28 @@
       <c r="B35" t="s">
         <v>40</v>
       </c>
-      <c r="H35" t="e">
+      <c r="C35">
+        <v>50000002</v>
+      </c>
+      <c r="D35">
+        <v>56440725</v>
+      </c>
+      <c r="E35">
+        <v>156605</v>
+      </c>
+      <c r="F35">
+        <v>115024</v>
+      </c>
+      <c r="G35">
+        <v>41581</v>
+      </c>
+      <c r="H35">
         <f t="shared" ref="H35:H67" si="2">(C35/D35)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I35" t="e">
+        <v>0.8858851830836687</v>
+      </c>
+      <c r="I35">
         <f t="shared" ref="I35:I67" si="3">G35/(C35/1000)</f>
-        <v>#DIV/0!</v>
+        <v>0.83161996673520133</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added Hawkeye to both configs in h264 benchmarks
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0C4379-DA0E-4182-9BC2-B96F034387D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5DF131-77BC-4EDB-BC52-1CBF2F92D750}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
@@ -862,7 +862,7 @@
   <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1686,7 +1686,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>27</v>
       </c>
@@ -1749,55 +1749,105 @@
         <v>0.69679997212800115</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>27</v>
       </c>
       <c r="B36" t="s">
         <v>41</v>
       </c>
-      <c r="H36" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I36" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C36">
+        <v>50000002</v>
+      </c>
+      <c r="D36">
+        <v>57480184</v>
+      </c>
+      <c r="E36">
+        <v>143908</v>
+      </c>
+      <c r="F36">
+        <v>109219</v>
+      </c>
+      <c r="G36">
+        <v>34689</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="2"/>
+        <v>0.86986503035550478</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="3"/>
+        <v>0.69377997224880106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>27</v>
       </c>
       <c r="B37" t="s">
         <v>42</v>
       </c>
-      <c r="H37" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I37" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C37">
+        <v>50000002</v>
+      </c>
+      <c r="D37">
+        <v>57409774</v>
+      </c>
+      <c r="E37">
+        <v>143909</v>
+      </c>
+      <c r="F37">
+        <v>112112</v>
+      </c>
+      <c r="G37">
+        <v>31797</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="2"/>
+        <v>0.87093187302914654</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="3"/>
+        <v>0.63593997456240103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>27</v>
       </c>
       <c r="B38" t="s">
         <v>43</v>
       </c>
-      <c r="H38" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I38" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C38">
+        <v>50000002</v>
+      </c>
+      <c r="D38">
+        <v>57409774</v>
+      </c>
+      <c r="E38">
+        <v>3157</v>
+      </c>
+      <c r="F38">
+        <v>2153</v>
+      </c>
+      <c r="G38">
+        <f>E38-F38</f>
+        <v>1004</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="2"/>
+        <v>0.87093187302914654</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="3"/>
+        <v>2.0079999196800032E-2</v>
+      </c>
+      <c r="J38">
+        <f>F38/E38</f>
+        <v>0.68197656002534046</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -1813,7 +1863,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>13</v>
       </c>
@@ -1829,7 +1879,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>13</v>
       </c>
@@ -1845,7 +1895,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>13</v>
       </c>
@@ -1861,7 +1911,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -1877,7 +1927,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>4</v>
       </c>
@@ -1893,7 +1943,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>4</v>
       </c>
@@ -1909,7 +1959,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -1925,7 +1975,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>33</v>
       </c>
@@ -1941,7 +1991,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>33</v>
       </c>
@@ -2579,7 +2629,7 @@
   <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3402,7 +3452,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -3418,7 +3468,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -3434,7 +3484,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>27</v>
       </c>
@@ -3465,55 +3515,105 @@
         <v>0.83161996673520133</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>27</v>
       </c>
       <c r="B36" t="s">
         <v>41</v>
       </c>
-      <c r="H36" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I36" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C36">
+        <v>50000002</v>
+      </c>
+      <c r="D36">
+        <v>56323779</v>
+      </c>
+      <c r="E36">
+        <v>156650</v>
+      </c>
+      <c r="F36">
+        <v>115510</v>
+      </c>
+      <c r="G36">
+        <v>41140</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="2"/>
+        <v>0.88772456123727073</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="3"/>
+        <v>0.82279996708800129</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>27</v>
       </c>
       <c r="B37" t="s">
         <v>42</v>
       </c>
-      <c r="H37" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I37" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C37">
+        <v>50000002</v>
+      </c>
+      <c r="D37">
+        <v>56144630</v>
+      </c>
+      <c r="E37">
+        <v>156527</v>
+      </c>
+      <c r="F37">
+        <v>115863</v>
+      </c>
+      <c r="G37">
+        <v>40664</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="2"/>
+        <v>0.89055715568879878</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="3"/>
+        <v>0.81327996746880127</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>27</v>
       </c>
       <c r="B38" t="s">
         <v>43</v>
       </c>
-      <c r="H38" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I38" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C38">
+        <v>50000002</v>
+      </c>
+      <c r="D38">
+        <v>56144630</v>
+      </c>
+      <c r="E38">
+        <v>1922</v>
+      </c>
+      <c r="F38">
+        <v>1576</v>
+      </c>
+      <c r="G38">
+        <f>E38-F38</f>
+        <v>346</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="2"/>
+        <v>0.89055715568879878</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="3"/>
+        <v>6.9199997232000108E-3</v>
+      </c>
+      <c r="J38">
+        <f>F38/E38</f>
+        <v>0.81997918834547345</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -3529,7 +3629,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>13</v>
       </c>
@@ -3545,7 +3645,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>13</v>
       </c>
@@ -3561,7 +3661,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>13</v>
       </c>
@@ -3577,7 +3677,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -3593,7 +3693,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>4</v>
       </c>
@@ -3609,7 +3709,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>4</v>
       </c>
@@ -3625,7 +3725,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -3641,7 +3741,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>33</v>
       </c>
@@ -3657,7 +3757,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
Added LRU for both configs on hmmer benchmark
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5DF131-77BC-4EDB-BC52-1CBF2F92D750}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF870594-2F98-4079-8CAC-B25AD3FFFA70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Benchmarks" sheetId="2" r:id="rId1"/>
@@ -861,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4DAA02D-4B80-49E4-98A1-4EF8777A053B}">
   <dimension ref="A2:L86"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1854,13 +1854,28 @@
       <c r="B39" t="s">
         <v>40</v>
       </c>
-      <c r="H39" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I39" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C39">
+        <v>50000000</v>
+      </c>
+      <c r="D39">
+        <v>44994000</v>
+      </c>
+      <c r="E39">
+        <v>328305</v>
+      </c>
+      <c r="F39">
+        <v>306380</v>
+      </c>
+      <c r="G39">
+        <v>21925</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="2"/>
+        <v>1.1112592790149798</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="3"/>
+        <v>0.4385</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
@@ -2628,8 +2643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E5CF80-89BD-41BF-8339-D77E14018905}">
   <dimension ref="A2:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3620,13 +3635,28 @@
       <c r="B39" t="s">
         <v>40</v>
       </c>
-      <c r="H39" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I39" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C39">
+        <v>50000000</v>
+      </c>
+      <c r="D39">
+        <v>43489442</v>
+      </c>
+      <c r="E39">
+        <v>331371</v>
+      </c>
+      <c r="F39">
+        <v>309182</v>
+      </c>
+      <c r="G39">
+        <v>22189</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="2"/>
+        <v>1.1497043351349507</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="3"/>
+        <v>0.44378000000000001</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added SRRIP to both configs on hmmer benchmark
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF870594-2F98-4079-8CAC-B25AD3FFFA70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A4A901B-3FA3-4E81-89AD-EE5ADC13EDFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
@@ -862,7 +862,7 @@
   <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1885,13 +1885,28 @@
       <c r="B40" t="s">
         <v>41</v>
       </c>
-      <c r="H40" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I40" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C40">
+        <v>50000000</v>
+      </c>
+      <c r="D40">
+        <v>44965903</v>
+      </c>
+      <c r="E40">
+        <v>328306</v>
+      </c>
+      <c r="F40">
+        <v>307235</v>
+      </c>
+      <c r="G40">
+        <v>21071</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="2"/>
+        <v>1.1119536507473229</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="3"/>
+        <v>0.42142000000000002</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
@@ -2644,7 +2659,7 @@
   <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3666,13 +3681,28 @@
       <c r="B40" t="s">
         <v>41</v>
       </c>
-      <c r="H40" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I40" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C40">
+        <v>50000000</v>
+      </c>
+      <c r="D40">
+        <v>43492624</v>
+      </c>
+      <c r="E40">
+        <v>331371</v>
+      </c>
+      <c r="F40">
+        <v>310122</v>
+      </c>
+      <c r="G40">
+        <v>21249</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="2"/>
+        <v>1.1496202206608643</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="3"/>
+        <v>0.42498000000000002</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added LRU for both configs for lbm benchmark
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A4A901B-3FA3-4E81-89AD-EE5ADC13EDFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D72027-7327-4E93-A408-05E170AB5AD4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
@@ -586,7 +586,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -861,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4DAA02D-4B80-49E4-98A1-4EF8777A053B}">
   <dimension ref="A2:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1916,13 +1916,28 @@
       <c r="B41" t="s">
         <v>42</v>
       </c>
-      <c r="H41" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I41" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C41">
+        <v>50000000</v>
+      </c>
+      <c r="D41">
+        <v>44574971</v>
+      </c>
+      <c r="E41">
+        <v>328304</v>
+      </c>
+      <c r="F41">
+        <v>318182</v>
+      </c>
+      <c r="G41">
+        <v>10122</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="2"/>
+        <v>1.1217057213564985</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="3"/>
+        <v>0.20244000000000001</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
@@ -1932,13 +1947,33 @@
       <c r="B42" t="s">
         <v>43</v>
       </c>
-      <c r="H42" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I42" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C42">
+        <v>50000000</v>
+      </c>
+      <c r="D42">
+        <v>44574971</v>
+      </c>
+      <c r="E42">
+        <v>5252</v>
+      </c>
+      <c r="F42">
+        <v>3689</v>
+      </c>
+      <c r="G42">
+        <f>E42-F42</f>
+        <v>1563</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="2"/>
+        <v>1.1217057213564985</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="3"/>
+        <v>3.1260000000000003E-2</v>
+      </c>
+      <c r="J42">
+        <f>F42/E42</f>
+        <v>0.70239908606245238</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
@@ -1948,13 +1983,28 @@
       <c r="B43" t="s">
         <v>40</v>
       </c>
-      <c r="H43" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I43" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C43">
+        <v>50000000</v>
+      </c>
+      <c r="D43">
+        <v>93261366</v>
+      </c>
+      <c r="E43">
+        <v>2641894</v>
+      </c>
+      <c r="F43">
+        <v>1161101</v>
+      </c>
+      <c r="G43">
+        <v>1480793</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="2"/>
+        <v>0.53612768228164276</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="3"/>
+        <v>29.615860000000001</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
@@ -2659,7 +2709,7 @@
   <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3712,13 +3762,28 @@
       <c r="B41" t="s">
         <v>42</v>
       </c>
-      <c r="H41" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I41" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C41">
+        <v>50000000</v>
+      </c>
+      <c r="D41">
+        <v>43537224</v>
+      </c>
+      <c r="E41">
+        <v>33170</v>
+      </c>
+      <c r="F41">
+        <v>270148</v>
+      </c>
+      <c r="G41">
+        <v>61222</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="2"/>
+        <v>1.1484425373560794</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="3"/>
+        <v>1.22444</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
@@ -3728,13 +3793,32 @@
       <c r="B42" t="s">
         <v>43</v>
       </c>
-      <c r="H42" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I42" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C42">
+        <v>50000000</v>
+      </c>
+      <c r="D42">
+        <v>43537224</v>
+      </c>
+      <c r="E42">
+        <v>1797</v>
+      </c>
+      <c r="F42">
+        <v>1620</v>
+      </c>
+      <c r="G42">
+        <v>177</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="2"/>
+        <v>1.1484425373560794</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="3"/>
+        <v>3.5400000000000002E-3</v>
+      </c>
+      <c r="J42">
+        <f>F42/E42</f>
+        <v>0.90150250417362265</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
@@ -3744,13 +3828,28 @@
       <c r="B43" t="s">
         <v>40</v>
       </c>
-      <c r="H43" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I43" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C43">
+        <v>50000000</v>
+      </c>
+      <c r="D43">
+        <v>80458099</v>
+      </c>
+      <c r="E43">
+        <v>2664603</v>
+      </c>
+      <c r="F43">
+        <v>1183779</v>
+      </c>
+      <c r="G43">
+        <v>1480824</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="2"/>
+        <v>0.6214414785017478</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="3"/>
+        <v>29.616479999999999</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added SRRIP for lbm benchmark
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D72027-7327-4E93-A408-05E170AB5AD4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADEE08D1-7733-4E3D-89FE-D493AF28AA71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
@@ -586,7 +586,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -821,7 +821,7 @@
       <c r="B21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -832,14 +832,14 @@
       <c r="B22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -862,7 +862,7 @@
   <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2014,13 +2014,28 @@
       <c r="B44" t="s">
         <v>41</v>
       </c>
-      <c r="H44" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I44" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C44">
+        <v>50000000</v>
+      </c>
+      <c r="D44">
+        <v>94566590</v>
+      </c>
+      <c r="E44">
+        <v>2641896</v>
+      </c>
+      <c r="F44">
+        <v>1099626</v>
+      </c>
+      <c r="G44">
+        <v>1542270</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="2"/>
+        <v>0.52872795772798831</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="3"/>
+        <v>30.845400000000001</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
@@ -2709,7 +2724,7 @@
   <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3859,13 +3874,28 @@
       <c r="B44" t="s">
         <v>41</v>
       </c>
-      <c r="H44" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I44" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C44">
+        <v>50000000</v>
+      </c>
+      <c r="D44">
+        <v>81755589</v>
+      </c>
+      <c r="E44">
+        <v>2664853</v>
+      </c>
+      <c r="F44">
+        <v>1118717</v>
+      </c>
+      <c r="G44">
+        <v>1546136</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="2"/>
+        <v>0.61157898330351457</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="3"/>
+        <v>30.922720000000002</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added Hawkeye for lbm benchmark
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADEE08D1-7733-4E3D-89FE-D493AF28AA71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6422A19C-B568-4FEE-9A6A-E2769B7E46FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
@@ -862,7 +862,7 @@
   <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2045,13 +2045,28 @@
       <c r="B45" t="s">
         <v>42</v>
       </c>
-      <c r="H45" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I45" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C45">
+        <v>50000000</v>
+      </c>
+      <c r="D45">
+        <v>82429919</v>
+      </c>
+      <c r="E45">
+        <v>2641903</v>
+      </c>
+      <c r="F45">
+        <v>883205</v>
+      </c>
+      <c r="G45">
+        <v>1758698</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="2"/>
+        <v>0.60657587204471231</v>
+      </c>
+      <c r="I45">
+        <f>F45/(C45/1000)</f>
+        <v>17.664100000000001</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
@@ -2061,13 +2076,33 @@
       <c r="B46" t="s">
         <v>43</v>
       </c>
-      <c r="H46" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I46" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C46">
+        <v>50000000</v>
+      </c>
+      <c r="D46">
+        <v>82429919</v>
+      </c>
+      <c r="E46">
+        <v>49369</v>
+      </c>
+      <c r="F46">
+        <v>13788</v>
+      </c>
+      <c r="G46">
+        <f>E46-F46</f>
+        <v>35581</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="2"/>
+        <v>0.60657587204471231</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="3"/>
+        <v>0.71162000000000003</v>
+      </c>
+      <c r="J46">
+        <f>F46/E46</f>
+        <v>0.27928457128967571</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
@@ -2724,7 +2759,7 @@
   <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3905,13 +3940,28 @@
       <c r="B45" t="s">
         <v>42</v>
       </c>
-      <c r="H45" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I45" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C45">
+        <v>50000000</v>
+      </c>
+      <c r="D45">
+        <v>71437360</v>
+      </c>
+      <c r="E45">
+        <v>2656558</v>
+      </c>
+      <c r="F45">
+        <v>867959</v>
+      </c>
+      <c r="G45">
+        <v>1788599</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="2"/>
+        <v>0.69991388259588538</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="3"/>
+        <v>35.771979999999999</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
@@ -3921,13 +3971,33 @@
       <c r="B46" t="s">
         <v>43</v>
       </c>
-      <c r="H46" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I46" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C46">
+        <v>50000000</v>
+      </c>
+      <c r="D46">
+        <v>71437360</v>
+      </c>
+      <c r="E46">
+        <v>42802</v>
+      </c>
+      <c r="F46">
+        <v>13968</v>
+      </c>
+      <c r="G46">
+        <f>E46-F46</f>
+        <v>28834</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="2"/>
+        <v>0.69991388259588538</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="3"/>
+        <v>0.57667999999999997</v>
+      </c>
+      <c r="J46">
+        <f>F46/E46</f>
+        <v>0.32633989065931501</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added LRU for leslie benchmark
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6422A19C-B568-4FEE-9A6A-E2769B7E46FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7752EB-F380-4A68-8A4E-8B4E1DAD6884}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Benchmarks" sheetId="2" r:id="rId1"/>
@@ -861,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4DAA02D-4B80-49E4-98A1-4EF8777A053B}">
   <dimension ref="A2:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2112,13 +2112,28 @@
       <c r="B47" t="s">
         <v>40</v>
       </c>
-      <c r="H47" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I47" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C47">
+        <v>50000000</v>
+      </c>
+      <c r="D47">
+        <v>106886860</v>
+      </c>
+      <c r="E47">
+        <v>2036037</v>
+      </c>
+      <c r="F47">
+        <v>850017</v>
+      </c>
+      <c r="G47">
+        <v>1186020</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="2"/>
+        <v>0.46778434692533771</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="3"/>
+        <v>23.720400000000001</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
@@ -2758,8 +2773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E5CF80-89BD-41BF-8339-D77E14018905}">
   <dimension ref="A2:L86"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4007,13 +4022,28 @@
       <c r="B47" t="s">
         <v>40</v>
       </c>
-      <c r="H47" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I47" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C47">
+        <v>50000000</v>
+      </c>
+      <c r="D47">
+        <v>76809653</v>
+      </c>
+      <c r="E47">
+        <v>2122055</v>
+      </c>
+      <c r="F47">
+        <v>912378</v>
+      </c>
+      <c r="G47">
+        <v>1209677</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="2"/>
+        <v>0.65095984745563162</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="3"/>
+        <v>24.193539999999999</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added LRU results to both configs for xalancbmk benchmark
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA5343C-755F-45D9-875B-595EC1C3516F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9875D049-3758-4970-9FBA-134D83A95801}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Benchmarks" sheetId="2" r:id="rId1"/>
@@ -871,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4DAA02D-4B80-49E4-98A1-4EF8777A053B}">
   <dimension ref="A2:L86"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2796,13 +2796,28 @@
       <c r="B79" t="s">
         <v>40</v>
       </c>
-      <c r="H79" t="e">
+      <c r="C79">
+        <v>50000000</v>
+      </c>
+      <c r="D79">
+        <v>243557965</v>
+      </c>
+      <c r="E79">
+        <v>1587557</v>
+      </c>
+      <c r="F79">
+        <v>134788</v>
+      </c>
+      <c r="G79">
+        <v>1452769</v>
+      </c>
+      <c r="H79">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I79" t="e">
+        <v>0.20528993991225045</v>
+      </c>
+      <c r="I79">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>29.05538</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
@@ -2930,8 +2945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E5CF80-89BD-41BF-8339-D77E14018905}">
   <dimension ref="A2:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4821,13 +4836,28 @@
       <c r="B79" t="s">
         <v>40</v>
       </c>
-      <c r="H79" t="e">
+      <c r="C79">
+        <v>50000000</v>
+      </c>
+      <c r="D79">
+        <v>193897645</v>
+      </c>
+      <c r="E79">
+        <v>2168988</v>
+      </c>
+      <c r="F79">
+        <v>129839</v>
+      </c>
+      <c r="G79">
+        <v>2039149</v>
+      </c>
+      <c r="H79">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I79" t="e">
+        <v>0.25786801072287391</v>
+      </c>
+      <c r="I79">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>40.782980000000002</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added SRRIP results to both configs for xalancbmk benchmark
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9875D049-3758-4970-9FBA-134D83A95801}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FD856A-D94A-4BB0-A577-0E5446A12A43}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
@@ -871,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4DAA02D-4B80-49E4-98A1-4EF8777A053B}">
   <dimension ref="A2:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2827,64 +2827,129 @@
       <c r="B80" t="s">
         <v>41</v>
       </c>
-      <c r="H80" t="e">
+      <c r="C80">
+        <v>50000000</v>
+      </c>
+      <c r="D80">
+        <v>241354593</v>
+      </c>
+      <c r="E80">
+        <v>1587556</v>
+      </c>
+      <c r="F80">
+        <v>162379</v>
+      </c>
+      <c r="G80">
+        <v>1425177</v>
+      </c>
+      <c r="H80">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I80" t="e">
+        <v>0.207164070832495</v>
+      </c>
+      <c r="I80">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+        <v>28.503540000000001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>22</v>
       </c>
       <c r="B81" t="s">
         <v>42</v>
       </c>
-      <c r="H81" t="e">
+      <c r="C81">
+        <v>50000000</v>
+      </c>
+      <c r="D81">
+        <v>228028533</v>
+      </c>
+      <c r="E81">
+        <v>1587556</v>
+      </c>
+      <c r="F81">
+        <v>363341</v>
+      </c>
+      <c r="G81">
+        <v>1224215</v>
+      </c>
+      <c r="H81">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I81" t="e">
+        <v>0.21927080502684285</v>
+      </c>
+      <c r="I81">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+        <v>24.484300000000001</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>22</v>
       </c>
       <c r="B82" t="s">
         <v>43</v>
       </c>
-      <c r="H82" t="e">
+      <c r="C82">
+        <v>50000000</v>
+      </c>
+      <c r="D82">
+        <v>228028533</v>
+      </c>
+      <c r="E82">
+        <v>47204</v>
+      </c>
+      <c r="F82">
+        <v>16412</v>
+      </c>
+      <c r="G82">
+        <f>E82-F82</f>
+        <v>30792</v>
+      </c>
+      <c r="H82">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I82" t="e">
+        <v>0.21927080502684285</v>
+      </c>
+      <c r="I82">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.61584000000000005</v>
+      </c>
+      <c r="J82">
+        <f>F82/E82</f>
+        <v>0.34768239979662741</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>23</v>
       </c>
       <c r="B83" t="s">
         <v>40</v>
       </c>
-      <c r="H83" t="e">
+      <c r="C83">
+        <v>50000000</v>
+      </c>
+      <c r="D83">
+        <v>43611395</v>
+      </c>
+      <c r="E83">
+        <v>402709</v>
+      </c>
+      <c r="F83">
+        <v>151183</v>
+      </c>
+      <c r="G83">
+        <v>251526</v>
+      </c>
+      <c r="H83">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I83" t="e">
+        <v>1.1464893521521153</v>
+      </c>
+      <c r="I83">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+        <v>5.0305200000000001</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>23</v>
       </c>
@@ -2900,7 +2965,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>23</v>
       </c>
@@ -2916,7 +2981,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>23</v>
       </c>
@@ -2945,8 +3010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E5CF80-89BD-41BF-8339-D77E14018905}">
   <dimension ref="A2:L86"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4867,64 +4932,129 @@
       <c r="B80" t="s">
         <v>41</v>
       </c>
-      <c r="H80" t="e">
+      <c r="C80">
+        <v>50000000</v>
+      </c>
+      <c r="D80">
+        <v>192694662</v>
+      </c>
+      <c r="E80">
+        <v>2168997</v>
+      </c>
+      <c r="F80">
+        <v>161045</v>
+      </c>
+      <c r="G80">
+        <v>2007952</v>
+      </c>
+      <c r="H80">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I80" t="e">
+        <v>0.25947786763288749</v>
+      </c>
+      <c r="I80">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40.159039999999997</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>22</v>
       </c>
       <c r="B81" t="s">
         <v>42</v>
       </c>
-      <c r="H81" t="e">
+      <c r="C81">
+        <v>50000000</v>
+      </c>
+      <c r="D81">
+        <v>186495428</v>
+      </c>
+      <c r="E81">
+        <v>2168866</v>
+      </c>
+      <c r="F81">
+        <v>334605</v>
+      </c>
+      <c r="G81">
+        <v>1834261</v>
+      </c>
+      <c r="H81">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I81" t="e">
+        <v>0.268103087224208</v>
+      </c>
+      <c r="I81">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+        <v>36.685220000000001</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>22</v>
       </c>
       <c r="B82" t="s">
         <v>43</v>
       </c>
-      <c r="H82" t="e">
+      <c r="C82">
+        <v>50000000</v>
+      </c>
+      <c r="D82">
+        <v>186495428</v>
+      </c>
+      <c r="E82">
+        <v>27979</v>
+      </c>
+      <c r="F82">
+        <v>14942</v>
+      </c>
+      <c r="G82">
+        <f>E82-F82</f>
+        <v>13037</v>
+      </c>
+      <c r="H82">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I82" t="e">
+        <v>0.268103087224208</v>
+      </c>
+      <c r="I82">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.26074000000000003</v>
+      </c>
+      <c r="J82">
+        <f>F82/E82</f>
+        <v>0.53404338968512099</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>23</v>
       </c>
       <c r="B83" t="s">
         <v>40</v>
       </c>
-      <c r="H83" t="e">
+      <c r="C83">
+        <v>50000001</v>
+      </c>
+      <c r="D83">
+        <v>34327145</v>
+      </c>
+      <c r="E83">
+        <v>409177</v>
+      </c>
+      <c r="F83">
+        <v>157503</v>
+      </c>
+      <c r="G83">
+        <v>251674</v>
+      </c>
+      <c r="H83">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I83" t="e">
+        <v>1.4565732454592422</v>
+      </c>
+      <c r="I83">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+        <v>5.033479899330402</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>23</v>
       </c>
@@ -4940,7 +5070,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>23</v>
       </c>
@@ -4956,7 +5086,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Finished tonto simulation results
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FD856A-D94A-4BB0-A577-0E5446A12A43}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306E491E-8862-419B-93AE-1123E030D233}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
@@ -220,18 +220,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -252,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -268,14 +262,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -596,7 +587,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -606,11 +597,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
       <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -623,7 +614,7 @@
       <c r="C2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>48</v>
       </c>
     </row>
@@ -754,7 +745,7 @@
       <c r="B14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="8" t="s">
         <v>33</v>
       </c>
     </row>
@@ -765,7 +756,7 @@
       <c r="B15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>26</v>
       </c>
     </row>
@@ -776,7 +767,7 @@
       <c r="B16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="8" t="s">
         <v>15</v>
       </c>
     </row>
@@ -787,7 +778,7 @@
       <c r="B17" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -798,7 +789,7 @@
       <c r="B18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -809,7 +800,7 @@
       <c r="B19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="8" t="s">
         <v>16</v>
       </c>
     </row>
@@ -820,7 +811,7 @@
       <c r="B20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -871,8 +862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4DAA02D-4B80-49E4-98A1-4EF8777A053B}">
   <dimension ref="A2:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1188,14 +1179,14 @@
       <c r="B11" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -1204,14 +1195,14 @@
       <c r="B12" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -1220,14 +1211,14 @@
       <c r="B13" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -1236,14 +1227,14 @@
       <c r="B14" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -2565,7 +2556,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>5</v>
       </c>
@@ -2581,7 +2572,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>5</v>
       </c>
@@ -2597,7 +2588,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>16</v>
       </c>
@@ -2613,7 +2604,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>16</v>
       </c>
@@ -2629,7 +2620,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>16</v>
       </c>
@@ -2645,7 +2636,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>16</v>
       </c>
@@ -2661,7 +2652,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>19</v>
       </c>
@@ -2677,7 +2668,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>19</v>
       </c>
@@ -2693,7 +2684,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>19</v>
       </c>
@@ -2709,7 +2700,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>19</v>
       </c>
@@ -2725,71 +2716,136 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>12</v>
       </c>
       <c r="B75" t="s">
         <v>40</v>
       </c>
-      <c r="H75" t="e">
+      <c r="C75">
+        <v>50000000</v>
+      </c>
+      <c r="D75">
+        <v>80146024</v>
+      </c>
+      <c r="E75">
+        <v>1156983</v>
+      </c>
+      <c r="F75">
+        <v>952546</v>
+      </c>
+      <c r="G75">
+        <v>204437</v>
+      </c>
+      <c r="H75">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I75" t="e">
+        <v>0.62386126603111336</v>
+      </c>
+      <c r="I75">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.0887399999999996</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>12</v>
       </c>
       <c r="B76" t="s">
         <v>41</v>
       </c>
-      <c r="H76" t="e">
+      <c r="C76">
+        <v>50000000</v>
+      </c>
+      <c r="D76">
+        <v>79992046</v>
+      </c>
+      <c r="E76">
+        <v>1156995</v>
+      </c>
+      <c r="F76">
+        <v>950307</v>
+      </c>
+      <c r="G76">
+        <v>206688</v>
+      </c>
+      <c r="H76">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I76" t="e">
+        <v>0.62506214680394601</v>
+      </c>
+      <c r="I76">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.1337599999999997</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>12</v>
       </c>
       <c r="B77" t="s">
         <v>42</v>
       </c>
-      <c r="H77" t="e">
+      <c r="C77">
+        <v>50000000</v>
+      </c>
+      <c r="D77">
+        <v>72566733</v>
+      </c>
+      <c r="E77">
+        <v>1157014</v>
+      </c>
+      <c r="F77">
+        <v>1034064</v>
+      </c>
+      <c r="G77">
+        <v>122950</v>
+      </c>
+      <c r="H77">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I77" t="e">
+        <v>0.68902095950771269</v>
+      </c>
+      <c r="I77">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2.4590000000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>12</v>
       </c>
       <c r="B78" t="s">
         <v>43</v>
       </c>
-      <c r="H78" t="e">
+      <c r="C78">
+        <v>50000000</v>
+      </c>
+      <c r="D78">
+        <v>72566733</v>
+      </c>
+      <c r="E78">
+        <v>15854</v>
+      </c>
+      <c r="F78">
+        <v>13224</v>
+      </c>
+      <c r="G78">
+        <f>E78-F78</f>
+        <v>2630</v>
+      </c>
+      <c r="H78">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I78" t="e">
+        <v>0.68902095950771269</v>
+      </c>
+      <c r="I78">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+        <v>5.2600000000000001E-2</v>
+      </c>
+      <c r="J78">
+        <f>F78/E78</f>
+        <v>0.83411126529582436</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>22</v>
       </c>
@@ -2820,7 +2876,7 @@
         <v>29.05538</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>22</v>
       </c>
@@ -2956,13 +3012,28 @@
       <c r="B84" t="s">
         <v>41</v>
       </c>
-      <c r="H84" t="e">
+      <c r="C84">
+        <v>50000000</v>
+      </c>
+      <c r="D84">
+        <v>43906336</v>
+      </c>
+      <c r="E84">
+        <v>402713</v>
+      </c>
+      <c r="F84">
+        <v>136242</v>
+      </c>
+      <c r="G84">
+        <v>266471</v>
+      </c>
+      <c r="H84">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I84" t="e">
+        <v>1.1387878050220359</v>
+      </c>
+      <c r="I84">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>5.3294199999999998</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.3">
@@ -2972,13 +3043,28 @@
       <c r="B85" t="s">
         <v>42</v>
       </c>
-      <c r="H85" t="e">
+      <c r="C85">
+        <v>50000000</v>
+      </c>
+      <c r="D85">
+        <v>43567981</v>
+      </c>
+      <c r="E85">
+        <v>402702</v>
+      </c>
+      <c r="F85">
+        <v>74335</v>
+      </c>
+      <c r="G85">
+        <v>328367</v>
+      </c>
+      <c r="H85">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I85" t="e">
+        <v>1.1476317895015609</v>
+      </c>
+      <c r="I85">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>6.5673399999999997</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.3">
@@ -2988,13 +3074,33 @@
       <c r="B86" t="s">
         <v>43</v>
       </c>
-      <c r="H86" t="e">
+      <c r="C86">
+        <v>50000000</v>
+      </c>
+      <c r="D86">
+        <v>43567981</v>
+      </c>
+      <c r="E86">
+        <v>8977</v>
+      </c>
+      <c r="F86">
+        <v>1537</v>
+      </c>
+      <c r="G86">
+        <f>E86-F86</f>
+        <v>7440</v>
+      </c>
+      <c r="H86">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I86" t="e">
+        <v>1.1476317895015609</v>
+      </c>
+      <c r="I86">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.14879999999999999</v>
+      </c>
+      <c r="J86">
+        <f>F86/E86</f>
+        <v>0.1712153280605993</v>
       </c>
     </row>
   </sheetData>
@@ -3010,8 +3116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E5CF80-89BD-41BF-8339-D77E14018905}">
   <dimension ref="A2:L86"/>
   <sheetViews>
-    <sheetView topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4670,7 +4776,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>5</v>
       </c>
@@ -4686,7 +4792,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>5</v>
       </c>
@@ -4702,7 +4808,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>16</v>
       </c>
@@ -4718,7 +4824,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>16</v>
       </c>
@@ -4734,7 +4840,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>16</v>
       </c>
@@ -4750,7 +4856,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>16</v>
       </c>
@@ -4766,7 +4872,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>19</v>
       </c>
@@ -4782,7 +4888,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>19</v>
       </c>
@@ -4798,7 +4904,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>19</v>
       </c>
@@ -4814,7 +4920,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>19</v>
       </c>
@@ -4830,71 +4936,136 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>12</v>
       </c>
       <c r="B75" t="s">
         <v>40</v>
       </c>
-      <c r="H75" t="e">
+      <c r="C75">
+        <v>50000000</v>
+      </c>
+      <c r="D75">
+        <v>60439277</v>
+      </c>
+      <c r="E75">
+        <v>1159127</v>
+      </c>
+      <c r="F75">
+        <v>953758</v>
+      </c>
+      <c r="G75">
+        <v>205369</v>
+      </c>
+      <c r="H75">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I75" t="e">
+        <v>0.82727660689918581</v>
+      </c>
+      <c r="I75">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.10738</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>12</v>
       </c>
       <c r="B76" t="s">
         <v>41</v>
       </c>
-      <c r="H76" t="e">
+      <c r="C76">
+        <v>50000000</v>
+      </c>
+      <c r="D76">
+        <v>60012199</v>
+      </c>
+      <c r="E76">
+        <v>1159433</v>
+      </c>
+      <c r="F76">
+        <v>952495</v>
+      </c>
+      <c r="G76">
+        <v>206938</v>
+      </c>
+      <c r="H76">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I76" t="e">
+        <v>0.83316393721883109</v>
+      </c>
+      <c r="I76">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.1387600000000004</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>12</v>
       </c>
       <c r="B77" t="s">
         <v>42</v>
       </c>
-      <c r="H77" t="e">
+      <c r="C77">
+        <v>50000000</v>
+      </c>
+      <c r="D77">
+        <v>57829181</v>
+      </c>
+      <c r="E77">
+        <v>1159116</v>
+      </c>
+      <c r="F77">
+        <v>1020555</v>
+      </c>
+      <c r="G77">
+        <v>138561</v>
+      </c>
+      <c r="H77">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I77" t="e">
+        <v>0.86461539201117166</v>
+      </c>
+      <c r="I77">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2.77122</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>12</v>
       </c>
       <c r="B78" t="s">
         <v>43</v>
       </c>
-      <c r="H78" t="e">
+      <c r="C78">
+        <v>50000000</v>
+      </c>
+      <c r="D78">
+        <v>57829181</v>
+      </c>
+      <c r="E78">
+        <v>6647</v>
+      </c>
+      <c r="F78">
+        <v>7023</v>
+      </c>
+      <c r="G78">
+        <f>E78-F78</f>
+        <v>-376</v>
+      </c>
+      <c r="H78">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I78" t="e">
+        <v>0.86461539201117166</v>
+      </c>
+      <c r="I78">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+        <v>-7.5199999999999998E-3</v>
+      </c>
+      <c r="J78">
+        <f>F78/E78</f>
+        <v>1.056566872273206</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>22</v>
       </c>
@@ -4925,7 +5096,7 @@
         <v>40.782980000000002</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>22</v>
       </c>
@@ -5061,13 +5232,28 @@
       <c r="B84" t="s">
         <v>41</v>
       </c>
-      <c r="H84" t="e">
+      <c r="C84">
+        <v>50000002</v>
+      </c>
+      <c r="D84">
+        <v>34548685</v>
+      </c>
+      <c r="E84">
+        <v>409084</v>
+      </c>
+      <c r="F84">
+        <v>142267</v>
+      </c>
+      <c r="G84">
+        <v>266817</v>
+      </c>
+      <c r="H84">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I84" t="e">
+        <v>1.4472331436058998</v>
+      </c>
+      <c r="I84">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>5.3363397865464082</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.3">
@@ -5077,13 +5263,28 @@
       <c r="B85" t="s">
         <v>42</v>
       </c>
-      <c r="H85" t="e">
+      <c r="C85">
+        <v>50000001</v>
+      </c>
+      <c r="D85">
+        <v>34401098</v>
+      </c>
+      <c r="E85">
+        <v>409461</v>
+      </c>
+      <c r="F85">
+        <v>76807</v>
+      </c>
+      <c r="G85">
+        <v>332654</v>
+      </c>
+      <c r="H85">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I85" t="e">
+        <v>1.4534420093219118</v>
+      </c>
+      <c r="I85">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>6.6530798669384028</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.3">
@@ -5093,13 +5294,33 @@
       <c r="B86" t="s">
         <v>43</v>
       </c>
-      <c r="H86" t="e">
+      <c r="C86">
+        <v>50000001</v>
+      </c>
+      <c r="D86">
+        <v>34401098</v>
+      </c>
+      <c r="E86">
+        <v>3649</v>
+      </c>
+      <c r="F86">
+        <v>1206</v>
+      </c>
+      <c r="G86">
+        <f>E86-F86</f>
+        <v>2443</v>
+      </c>
+      <c r="H86">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I86" t="e">
+        <v>1.4534420093219118</v>
+      </c>
+      <c r="I86">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>4.885999902280002E-2</v>
+      </c>
+      <c r="J86">
+        <f>F86/E86</f>
+        <v>0.33050150726226363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Simulation for sphinx3 added
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306E491E-8862-419B-93AE-1123E030D233}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3892066D-3B59-48F1-9697-871440C6705D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Benchmarks" sheetId="2" r:id="rId1"/>
@@ -862,8 +862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4DAA02D-4B80-49E4-98A1-4EF8777A053B}">
   <dimension ref="A2:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2659,13 +2659,28 @@
       <c r="B71" t="s">
         <v>40</v>
       </c>
-      <c r="H71" t="e">
+      <c r="C71">
+        <v>50000000</v>
+      </c>
+      <c r="D71">
+        <v>92768345</v>
+      </c>
+      <c r="E71">
+        <v>754197</v>
+      </c>
+      <c r="F71">
+        <v>160196</v>
+      </c>
+      <c r="G71">
+        <v>594001</v>
+      </c>
+      <c r="H71">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I71" t="e">
+        <v>0.53897695383053346</v>
+      </c>
+      <c r="I71">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>11.88002</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
@@ -2675,13 +2690,28 @@
       <c r="B72" t="s">
         <v>41</v>
       </c>
-      <c r="H72" t="e">
+      <c r="C72">
+        <v>50000000</v>
+      </c>
+      <c r="D72">
+        <v>89747896</v>
+      </c>
+      <c r="E72">
+        <v>754200</v>
+      </c>
+      <c r="F72">
+        <v>215084</v>
+      </c>
+      <c r="G72">
+        <v>539116</v>
+      </c>
+      <c r="H72">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I72" t="e">
+        <v>0.55711612448273995</v>
+      </c>
+      <c r="I72">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>10.78232</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
@@ -2691,13 +2721,28 @@
       <c r="B73" t="s">
         <v>42</v>
       </c>
-      <c r="H73" t="e">
+      <c r="C73">
+        <v>50000000</v>
+      </c>
+      <c r="D73">
+        <v>78116641</v>
+      </c>
+      <c r="E73">
+        <v>754196</v>
+      </c>
+      <c r="F73">
+        <v>376654</v>
+      </c>
+      <c r="G73">
+        <v>377542</v>
+      </c>
+      <c r="H73">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I73" t="e">
+        <v>0.64006848425548657</v>
+      </c>
+      <c r="I73">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>7.55084</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
@@ -2707,13 +2752,33 @@
       <c r="B74" t="s">
         <v>43</v>
       </c>
-      <c r="H74" t="e">
+      <c r="C74">
+        <v>50000000</v>
+      </c>
+      <c r="D74">
+        <v>78116641</v>
+      </c>
+      <c r="E74">
+        <v>22436</v>
+      </c>
+      <c r="F74">
+        <v>11343</v>
+      </c>
+      <c r="G74">
+        <f>E74-F74</f>
+        <v>11093</v>
+      </c>
+      <c r="H74">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I74" t="e">
+        <v>0.64006848425548657</v>
+      </c>
+      <c r="I74">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.22186</v>
+      </c>
+      <c r="J74">
+        <f>F74/E74</f>
+        <v>0.5055714031021572</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
@@ -3116,8 +3181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E5CF80-89BD-41BF-8339-D77E14018905}">
   <dimension ref="A2:L86"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4879,13 +4944,28 @@
       <c r="B71" t="s">
         <v>40</v>
       </c>
-      <c r="H71" t="e">
+      <c r="C71">
+        <v>50000000</v>
+      </c>
+      <c r="D71">
+        <v>60373750</v>
+      </c>
+      <c r="E71">
+        <v>836292</v>
+      </c>
+      <c r="F71">
+        <v>153218</v>
+      </c>
+      <c r="G71">
+        <v>683074</v>
+      </c>
+      <c r="H71">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I71" t="e">
+        <v>0.82817449636638441</v>
+      </c>
+      <c r="I71">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>13.661479999999999</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
@@ -4895,13 +4975,28 @@
       <c r="B72" t="s">
         <v>41</v>
       </c>
-      <c r="H72" t="e">
+      <c r="C72">
+        <v>50000000</v>
+      </c>
+      <c r="D72">
+        <v>58442276</v>
+      </c>
+      <c r="E72">
+        <v>836345</v>
+      </c>
+      <c r="F72">
+        <v>215632</v>
+      </c>
+      <c r="G72">
+        <v>620713</v>
+      </c>
+      <c r="H72">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I72" t="e">
+        <v>0.85554505098329847</v>
+      </c>
+      <c r="I72">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>12.414260000000001</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
@@ -4911,13 +5006,28 @@
       <c r="B73" t="s">
         <v>42</v>
       </c>
-      <c r="H73" t="e">
+      <c r="C73">
+        <v>50000000</v>
+      </c>
+      <c r="D73">
+        <v>53262804</v>
+      </c>
+      <c r="E73">
+        <v>836625</v>
+      </c>
+      <c r="F73">
+        <v>309808</v>
+      </c>
+      <c r="G73">
+        <v>526817</v>
+      </c>
+      <c r="H73">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I73" t="e">
+        <v>0.9387414151158846</v>
+      </c>
+      <c r="I73">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>10.536339999999999</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
@@ -4927,13 +5037,33 @@
       <c r="B74" t="s">
         <v>43</v>
       </c>
-      <c r="H74" t="e">
+      <c r="C74">
+        <v>50000000</v>
+      </c>
+      <c r="D74">
+        <v>53262804</v>
+      </c>
+      <c r="E74">
+        <v>6303</v>
+      </c>
+      <c r="F74">
+        <v>5767</v>
+      </c>
+      <c r="G74">
+        <f>E74-F74</f>
+        <v>536</v>
+      </c>
+      <c r="H74">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I74" t="e">
+        <v>0.9387414151158846</v>
+      </c>
+      <c r="I74">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>1.072E-2</v>
+      </c>
+      <c r="J74">
+        <f>F74/E74</f>
+        <v>0.91496112962081544</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added LRU for soplex benchmark
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3892066D-3B59-48F1-9697-871440C6705D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88424FC-0808-46F2-AC71-5F49874C6B51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
@@ -863,7 +863,7 @@
   <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2595,13 +2595,28 @@
       <c r="B67" t="s">
         <v>40</v>
       </c>
-      <c r="H67" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I67" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C67">
+        <v>50000000</v>
+      </c>
+      <c r="D67">
+        <v>167531010</v>
+      </c>
+      <c r="E67">
+        <v>2732037</v>
+      </c>
+      <c r="F67">
+        <v>1413371</v>
+      </c>
+      <c r="G67">
+        <v>1318666</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="2"/>
+        <v>0.29845220893731855</v>
+      </c>
+      <c r="I67">
+        <f t="shared" si="3"/>
+        <v>26.37332</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
@@ -3182,7 +3197,7 @@
   <dimension ref="A2:L86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="E75" sqref="E75"/>
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4880,13 +4895,28 @@
       <c r="B67" t="s">
         <v>40</v>
       </c>
-      <c r="H67" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I67" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C67">
+        <v>50000000</v>
+      </c>
+      <c r="D67">
+        <v>126869636</v>
+      </c>
+      <c r="E67">
+        <v>3398940</v>
+      </c>
+      <c r="F67">
+        <v>1742705</v>
+      </c>
+      <c r="G67">
+        <v>1656235</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="2"/>
+        <v>0.39410533186995195</v>
+      </c>
+      <c r="I67">
+        <f t="shared" si="3"/>
+        <v>33.124699999999997</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added soplex simulation results
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88424FC-0808-46F2-AC71-5F49874C6B51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408E0FB9-F4D7-4A4B-BA13-BFB55887645C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Benchmarks" sheetId="2" r:id="rId1"/>
@@ -862,8 +862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4DAA02D-4B80-49E4-98A1-4EF8777A053B}">
   <dimension ref="A2:L86"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2626,13 +2626,28 @@
       <c r="B68" t="s">
         <v>41</v>
       </c>
-      <c r="H68" t="e">
+      <c r="C68">
+        <v>50000000</v>
+      </c>
+      <c r="D68">
+        <v>162827847</v>
+      </c>
+      <c r="E68">
+        <v>2732027</v>
+      </c>
+      <c r="F68">
+        <v>1497017</v>
+      </c>
+      <c r="G68">
+        <v>1235010</v>
+      </c>
+      <c r="H68">
         <f t="shared" ref="H68:H86" si="4">(C68/D68)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I68" t="e">
+        <v>0.30707278221273787</v>
+      </c>
+      <c r="I68">
         <f t="shared" ref="I68:I86" si="5">G68/(C68/1000)</f>
-        <v>#DIV/0!</v>
+        <v>24.700199999999999</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
@@ -2642,13 +2657,28 @@
       <c r="B69" t="s">
         <v>42</v>
       </c>
-      <c r="H69" t="e">
+      <c r="C69">
+        <v>50000000</v>
+      </c>
+      <c r="D69">
+        <v>156923926</v>
+      </c>
+      <c r="E69">
+        <v>2731976</v>
+      </c>
+      <c r="F69">
+        <v>1490724</v>
+      </c>
+      <c r="G69">
+        <v>1241252</v>
+      </c>
+      <c r="H69">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I69" t="e">
+        <v>0.31862572696530672</v>
+      </c>
+      <c r="I69">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>24.825040000000001</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
@@ -2658,13 +2688,33 @@
       <c r="B70" t="s">
         <v>43</v>
       </c>
-      <c r="H70" t="e">
+      <c r="C70">
+        <v>50000000</v>
+      </c>
+      <c r="D70">
+        <v>156923926</v>
+      </c>
+      <c r="E70">
+        <v>59591</v>
+      </c>
+      <c r="F70">
+        <v>31306</v>
+      </c>
+      <c r="G70">
+        <f>E70-F70</f>
+        <v>28285</v>
+      </c>
+      <c r="H70">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I70" t="e">
+        <v>0.31862572696530672</v>
+      </c>
+      <c r="I70">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.56569999999999998</v>
+      </c>
+      <c r="J70">
+        <f>F70/E70</f>
+        <v>0.52534778741756305</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
@@ -3196,8 +3246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E5CF80-89BD-41BF-8339-D77E14018905}">
   <dimension ref="A2:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4926,13 +4976,28 @@
       <c r="B68" t="s">
         <v>41</v>
       </c>
-      <c r="H68" t="e">
+      <c r="C68">
+        <v>50000000</v>
+      </c>
+      <c r="D68">
+        <v>124990062</v>
+      </c>
+      <c r="E68">
+        <v>3394940</v>
+      </c>
+      <c r="F68">
+        <v>1837023</v>
+      </c>
+      <c r="G68">
+        <v>1557917</v>
+      </c>
+      <c r="H68">
         <f t="shared" ref="H68:H86" si="4">(C68/D68)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I68" t="e">
+        <v>0.40003180412855543</v>
+      </c>
+      <c r="I68">
         <f t="shared" ref="I68:I86" si="5">G68/(C68/1000)</f>
-        <v>#DIV/0!</v>
+        <v>31.158339999999999</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added simulation results for omentpp
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408E0FB9-F4D7-4A4B-BA13-BFB55887645C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC77194-63A7-4F3D-8987-2908DF9F7ED3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Benchmarks" sheetId="2" r:id="rId1"/>
@@ -862,8 +862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4DAA02D-4B80-49E4-98A1-4EF8777A053B}">
   <dimension ref="A2:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2531,13 +2531,28 @@
       <c r="B63" t="s">
         <v>40</v>
       </c>
-      <c r="H63" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I63" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C63">
+        <v>50000001</v>
+      </c>
+      <c r="D63">
+        <v>141601931</v>
+      </c>
+      <c r="E63">
+        <v>1310666</v>
+      </c>
+      <c r="F63">
+        <v>968952</v>
+      </c>
+      <c r="G63">
+        <v>341714</v>
+      </c>
+      <c r="H63">
+        <f t="shared" si="2"/>
+        <v>0.35310253643363099</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="3"/>
+        <v>6.8342798633144035</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
@@ -2547,13 +2562,28 @@
       <c r="B64" t="s">
         <v>41</v>
       </c>
-      <c r="H64" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I64" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C64">
+        <v>50000001</v>
+      </c>
+      <c r="D64">
+        <v>138403519</v>
+      </c>
+      <c r="E64">
+        <v>1310668</v>
+      </c>
+      <c r="F64">
+        <v>1056307</v>
+      </c>
+      <c r="G64">
+        <v>254361</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="2"/>
+        <v>0.36126249795715093</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="3"/>
+        <v>5.0872198982556025</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
@@ -2563,13 +2593,28 @@
       <c r="B65" t="s">
         <v>42</v>
       </c>
-      <c r="H65" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I65" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C65">
+        <v>50000001</v>
+      </c>
+      <c r="D65">
+        <v>139982052</v>
+      </c>
+      <c r="E65">
+        <v>1310668</v>
+      </c>
+      <c r="F65">
+        <v>1044826</v>
+      </c>
+      <c r="G65">
+        <v>265842</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="2"/>
+        <v>0.35718865587139698</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="3"/>
+        <v>5.3168398936632029</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
@@ -2579,13 +2624,33 @@
       <c r="B66" t="s">
         <v>43</v>
       </c>
-      <c r="H66" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I66" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C66">
+        <v>50000001</v>
+      </c>
+      <c r="D66">
+        <v>139982052</v>
+      </c>
+      <c r="E66">
+        <v>39348</v>
+      </c>
+      <c r="F66">
+        <v>36263</v>
+      </c>
+      <c r="G66">
+        <f>E66-F66</f>
+        <v>3085</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="2"/>
+        <v>0.35718865587139698</v>
+      </c>
+      <c r="I66">
+        <f t="shared" si="3"/>
+        <v>6.1699998766000026E-2</v>
+      </c>
+      <c r="J66">
+        <f>F66/E66</f>
+        <v>0.92159703161532991</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
@@ -3246,8 +3311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E5CF80-89BD-41BF-8339-D77E14018905}">
   <dimension ref="A2:L86"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3562,6 +3627,14 @@
       <c r="B11" t="s">
         <v>40</v>
       </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -3570,6 +3643,14 @@
       <c r="B12" t="s">
         <v>41</v>
       </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -3578,6 +3659,14 @@
       <c r="B13" t="s">
         <v>42</v>
       </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -3586,6 +3675,14 @@
       <c r="B14" t="s">
         <v>43</v>
       </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -4881,13 +4978,28 @@
       <c r="B63" t="s">
         <v>40</v>
       </c>
-      <c r="H63" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I63" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C63">
+        <v>50000001</v>
+      </c>
+      <c r="D63">
+        <v>151477865</v>
+      </c>
+      <c r="E63">
+        <v>2348023</v>
+      </c>
+      <c r="F63">
+        <v>148199</v>
+      </c>
+      <c r="G63">
+        <v>2199824</v>
+      </c>
+      <c r="H63">
+        <f t="shared" si="2"/>
+        <v>0.33008123662160144</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="3"/>
+        <v>43.996479120070418</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
@@ -4897,13 +5009,28 @@
       <c r="B64" t="s">
         <v>41</v>
       </c>
-      <c r="H64" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I64" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C64">
+        <v>50000001</v>
+      </c>
+      <c r="D64">
+        <v>147254171</v>
+      </c>
+      <c r="E64">
+        <v>2346295</v>
+      </c>
+      <c r="F64">
+        <v>331469</v>
+      </c>
+      <c r="G64">
+        <v>2014826</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="2"/>
+        <v>0.33954896258931777</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="3"/>
+        <v>40.296519194069617</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
@@ -4913,13 +5040,28 @@
       <c r="B65" t="s">
         <v>42</v>
       </c>
-      <c r="H65" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I65" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C65">
+        <v>50000001</v>
+      </c>
+      <c r="D65">
+        <v>137716883</v>
+      </c>
+      <c r="E65">
+        <v>2342866</v>
+      </c>
+      <c r="F65">
+        <v>1035700</v>
+      </c>
+      <c r="G65">
+        <v>1307166</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="2"/>
+        <v>0.36306369931419374</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="3"/>
+        <v>26.143319477133613</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
@@ -4929,13 +5071,33 @@
       <c r="B66" t="s">
         <v>43</v>
       </c>
-      <c r="H66" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I66" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C66">
+        <v>50000001</v>
+      </c>
+      <c r="D66">
+        <v>137716883</v>
+      </c>
+      <c r="E66">
+        <v>34072</v>
+      </c>
+      <c r="F66">
+        <v>32791</v>
+      </c>
+      <c r="G66">
+        <f>E66-F66</f>
+        <v>1281</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="2"/>
+        <v>0.36306369931419374</v>
+      </c>
+      <c r="I66">
+        <f t="shared" si="3"/>
+        <v>2.5619999487600013E-2</v>
+      </c>
+      <c r="J66">
+        <f>F66/E66</f>
+        <v>0.96240314627846912</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
@@ -5007,13 +5169,28 @@
       <c r="B69" t="s">
         <v>42</v>
       </c>
-      <c r="H69" t="e">
+      <c r="C69">
+        <v>50000000</v>
+      </c>
+      <c r="D69">
+        <v>123879806</v>
+      </c>
+      <c r="E69">
+        <v>3389424</v>
+      </c>
+      <c r="F69">
+        <v>1788128</v>
+      </c>
+      <c r="G69">
+        <v>1601296</v>
+      </c>
+      <c r="H69">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I69" t="e">
+        <v>0.4036170350476655</v>
+      </c>
+      <c r="I69">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>32.025919999999999</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
@@ -5023,13 +5200,33 @@
       <c r="B70" t="s">
         <v>43</v>
       </c>
-      <c r="H70" t="e">
+      <c r="C70">
+        <v>50000000</v>
+      </c>
+      <c r="D70">
+        <v>123879806</v>
+      </c>
+      <c r="E70">
+        <v>34096</v>
+      </c>
+      <c r="F70">
+        <v>24461</v>
+      </c>
+      <c r="G70">
+        <f>E70-F70</f>
+        <v>9635</v>
+      </c>
+      <c r="H70">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I70" t="e">
+        <v>0.4036170350476655</v>
+      </c>
+      <c r="I70">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.19270000000000001</v>
+      </c>
+      <c r="J70">
+        <f>F70/E70</f>
+        <v>0.71741553261379631</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added LRU results for mcf
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC77194-63A7-4F3D-8987-2908DF9F7ED3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81315FE-B8C7-4563-8B0A-57BDC2F886A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Benchmarks" sheetId="2" r:id="rId1"/>
@@ -862,8 +862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4DAA02D-4B80-49E4-98A1-4EF8777A053B}">
   <dimension ref="A2:L86"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2403,13 +2403,28 @@
       <c r="B55" t="s">
         <v>40</v>
       </c>
-      <c r="H55" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I55" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C55">
+        <v>50000001</v>
+      </c>
+      <c r="D55">
+        <v>505789892</v>
+      </c>
+      <c r="E55">
+        <v>5694538</v>
+      </c>
+      <c r="F55">
+        <v>2113376</v>
+      </c>
+      <c r="G55">
+        <v>3581162</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="2"/>
+        <v>9.8855279219379893E-2</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="3"/>
+        <v>71.623238567535239</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
@@ -2467,13 +2482,28 @@
       <c r="B59" t="s">
         <v>40</v>
       </c>
-      <c r="H59" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I59" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C59">
+        <v>50000002</v>
+      </c>
+      <c r="D59">
+        <v>121522048</v>
+      </c>
+      <c r="E59">
+        <v>1510289</v>
+      </c>
+      <c r="F59">
+        <v>325673</v>
+      </c>
+      <c r="G59">
+        <v>1184616</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="2"/>
+        <v>0.41144798678837274</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="3"/>
+        <v>23.692319052307237</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
@@ -2483,13 +2513,28 @@
       <c r="B60" t="s">
         <v>41</v>
       </c>
-      <c r="H60" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I60" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C60">
+        <v>50000002</v>
+      </c>
+      <c r="D60">
+        <v>122348912</v>
+      </c>
+      <c r="E60">
+        <v>1510289</v>
+      </c>
+      <c r="F60">
+        <v>299898</v>
+      </c>
+      <c r="G60">
+        <v>1210391</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="2"/>
+        <v>0.40866732022921465</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="3"/>
+        <v>24.20781903168724</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
@@ -2499,13 +2544,28 @@
       <c r="B61" t="s">
         <v>42</v>
       </c>
-      <c r="H61" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I61" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C61">
+        <v>50000002</v>
+      </c>
+      <c r="D61">
+        <v>120220593</v>
+      </c>
+      <c r="E61">
+        <v>1510289</v>
+      </c>
+      <c r="F61">
+        <v>38749</v>
+      </c>
+      <c r="G61">
+        <v>1471540</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="2"/>
+        <v>0.4159021408254075</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="3"/>
+        <v>29.430798822768047</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
@@ -2515,13 +2575,33 @@
       <c r="B62" t="s">
         <v>43</v>
       </c>
-      <c r="H62" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I62" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C62">
+        <v>50000002</v>
+      </c>
+      <c r="D62">
+        <v>120220593</v>
+      </c>
+      <c r="E62">
+        <v>32737</v>
+      </c>
+      <c r="F62">
+        <v>571</v>
+      </c>
+      <c r="G62">
+        <f>E62-F62</f>
+        <v>32166</v>
+      </c>
+      <c r="H62">
+        <f t="shared" si="2"/>
+        <v>0.4159021408254075</v>
+      </c>
+      <c r="I62">
+        <f t="shared" si="3"/>
+        <v>0.643319974267201</v>
+      </c>
+      <c r="J62">
+        <f>F62/E62</f>
+        <v>1.7442038060909673E-2</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
@@ -3311,8 +3391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E5CF80-89BD-41BF-8339-D77E14018905}">
   <dimension ref="A2:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4850,13 +4930,28 @@
       <c r="B55" t="s">
         <v>40</v>
       </c>
-      <c r="H55" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I55" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C55">
+        <v>50000000</v>
+      </c>
+      <c r="D55">
+        <v>437451603</v>
+      </c>
+      <c r="E55">
+        <v>9525395</v>
+      </c>
+      <c r="F55">
+        <v>4305218</v>
+      </c>
+      <c r="G55">
+        <v>5220177</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="2"/>
+        <v>0.11429835816603466</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="3"/>
+        <v>104.40354000000001</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
@@ -4914,13 +5009,28 @@
       <c r="B59" t="s">
         <v>40</v>
       </c>
-      <c r="H59" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I59" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C59">
+        <v>50000002</v>
+      </c>
+      <c r="D59">
+        <v>93003755</v>
+      </c>
+      <c r="E59">
+        <v>1856592</v>
+      </c>
+      <c r="F59">
+        <v>325679</v>
+      </c>
+      <c r="G59">
+        <v>1530913</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="2"/>
+        <v>0.53761272327122711</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="3"/>
+        <v>30.618258775269648</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
@@ -4930,13 +5040,28 @@
       <c r="B60" t="s">
         <v>41</v>
       </c>
-      <c r="H60" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I60" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C60">
+        <v>50000002</v>
+      </c>
+      <c r="D60">
+        <v>93552246</v>
+      </c>
+      <c r="E60">
+        <v>1856586</v>
+      </c>
+      <c r="F60">
+        <v>300007</v>
+      </c>
+      <c r="G60">
+        <v>1556579</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="2"/>
+        <v>0.53446073331045418</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="3"/>
+        <v>31.13157875473685</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
@@ -4946,13 +5071,28 @@
       <c r="B61" t="s">
         <v>42</v>
       </c>
-      <c r="H61" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I61" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C61">
+        <v>50000002</v>
+      </c>
+      <c r="D61">
+        <v>92679825</v>
+      </c>
+      <c r="E61">
+        <v>1856587</v>
+      </c>
+      <c r="F61">
+        <v>32820</v>
+      </c>
+      <c r="G61">
+        <v>1823767</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="2"/>
+        <v>0.53949176101702823</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="3"/>
+        <v>36.475338540986456</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
@@ -4962,13 +5102,33 @@
       <c r="B62" t="s">
         <v>43</v>
       </c>
-      <c r="H62" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I62" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C62">
+        <v>50000002</v>
+      </c>
+      <c r="D62">
+        <v>92679825</v>
+      </c>
+      <c r="E62">
+        <v>17406</v>
+      </c>
+      <c r="F62">
+        <v>170</v>
+      </c>
+      <c r="G62">
+        <f>E62-F62</f>
+        <v>17236</v>
+      </c>
+      <c r="H62">
+        <f t="shared" si="2"/>
+        <v>0.53949176101702823</v>
+      </c>
+      <c r="I62">
+        <f t="shared" si="3"/>
+        <v>0.34471998621120054</v>
+      </c>
+      <c r="J62">
+        <f>F62/E62</f>
+        <v>9.7667470987015965E-3</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added SRRIP simulations for gromacs benchmark
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C508F26-57A2-4774-9B7E-C8071BCAEE36}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED070278-18E0-4D22-85FB-8CC06AD4074E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Benchmarks" sheetId="2" r:id="rId1"/>
@@ -585,7 +585,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -856,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4DAA02D-4B80-49E4-98A1-4EF8777A053B}">
   <dimension ref="A2:L82"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1591,13 +1591,28 @@
       <c r="B24" t="s">
         <v>41</v>
       </c>
-      <c r="H24" t="e">
+      <c r="C24">
+        <v>50000000</v>
+      </c>
+      <c r="D24">
+        <v>116980411</v>
+      </c>
+      <c r="E24">
+        <v>31351</v>
+      </c>
+      <c r="F24">
+        <v>19240</v>
+      </c>
+      <c r="G24">
+        <v>12111</v>
+      </c>
+      <c r="H24">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I24" t="e">
+        <v>0.42742198948164067</v>
+      </c>
+      <c r="I24">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.24221999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -1607,13 +1622,28 @@
       <c r="B25" t="s">
         <v>42</v>
       </c>
-      <c r="H25" t="e">
+      <c r="C25">
+        <v>50000000</v>
+      </c>
+      <c r="D25">
+        <v>117019326</v>
+      </c>
+      <c r="E25">
+        <v>31351</v>
+      </c>
+      <c r="F25">
+        <v>17616</v>
+      </c>
+      <c r="G25">
+        <v>13735</v>
+      </c>
+      <c r="H25">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I25" t="e">
+        <v>0.42727984948400743</v>
+      </c>
+      <c r="I25">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.2747</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -1623,13 +1653,33 @@
       <c r="B26" t="s">
         <v>43</v>
       </c>
-      <c r="H26" t="e">
+      <c r="C26">
+        <v>50000000</v>
+      </c>
+      <c r="D26">
+        <v>117019326</v>
+      </c>
+      <c r="E26">
+        <v>1411</v>
+      </c>
+      <c r="F26">
+        <v>859</v>
+      </c>
+      <c r="G26">
+        <f>E26-F26</f>
+        <v>552</v>
+      </c>
+      <c r="H26">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I26" t="e">
+        <v>0.42727984948400743</v>
+      </c>
+      <c r="I26">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>1.1039999999999999E-2</v>
+      </c>
+      <c r="J26">
+        <f>F26/E26</f>
+        <v>0.60878809355067331</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -1639,13 +1689,28 @@
       <c r="B27" t="s">
         <v>40</v>
       </c>
-      <c r="H27" t="e">
+      <c r="C27">
+        <v>50000001</v>
+      </c>
+      <c r="D27">
+        <v>124667669</v>
+      </c>
+      <c r="E27">
+        <v>30089</v>
+      </c>
+      <c r="F27">
+        <v>15882</v>
+      </c>
+      <c r="G27">
+        <v>14207</v>
+      </c>
+      <c r="H27">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I27" t="e">
+        <v>0.40106630212200406</v>
+      </c>
+      <c r="I27">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.28413999431720011</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -1655,13 +1720,28 @@
       <c r="B28" t="s">
         <v>41</v>
       </c>
-      <c r="H28" t="e">
+      <c r="C28">
+        <v>50000001</v>
+      </c>
+      <c r="D28">
+        <v>124667669</v>
+      </c>
+      <c r="E28">
+        <v>30089</v>
+      </c>
+      <c r="F28">
+        <v>15632</v>
+      </c>
+      <c r="G28">
+        <v>14457</v>
+      </c>
+      <c r="H28">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I28" t="e">
+        <v>0.40106630212200406</v>
+      </c>
+      <c r="I28">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.28913999421720016</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -3386,8 +3466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E5CF80-89BD-41BF-8339-D77E14018905}">
   <dimension ref="A2:L82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4120,13 +4200,28 @@
       <c r="B24" t="s">
         <v>41</v>
       </c>
-      <c r="H24" t="e">
+      <c r="C24">
+        <v>50000000</v>
+      </c>
+      <c r="D24">
+        <v>116540663</v>
+      </c>
+      <c r="E24">
+        <v>46889</v>
+      </c>
+      <c r="F24">
+        <v>28912</v>
+      </c>
+      <c r="G24">
+        <v>17977</v>
+      </c>
+      <c r="H24">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I24" t="e">
+        <v>0.42903479963898955</v>
+      </c>
+      <c r="I24">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.35954000000000003</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -4136,13 +4231,28 @@
       <c r="B25" t="s">
         <v>42</v>
       </c>
-      <c r="H25" t="e">
+      <c r="C25">
+        <v>50000000</v>
+      </c>
+      <c r="D25">
+        <v>116557215</v>
+      </c>
+      <c r="E25">
+        <v>46888</v>
+      </c>
+      <c r="F25">
+        <v>25562</v>
+      </c>
+      <c r="G25">
+        <v>21326</v>
+      </c>
+      <c r="H25">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I25" t="e">
+        <v>0.42897387347492816</v>
+      </c>
+      <c r="I25">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.42652000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -4152,13 +4262,33 @@
       <c r="B26" t="s">
         <v>43</v>
       </c>
-      <c r="H26" t="e">
+      <c r="C26">
+        <v>50000000</v>
+      </c>
+      <c r="D26">
+        <v>116557215</v>
+      </c>
+      <c r="E26">
+        <v>1167</v>
+      </c>
+      <c r="F26">
+        <v>1035</v>
+      </c>
+      <c r="G26">
+        <f>E26-F26</f>
+        <v>132</v>
+      </c>
+      <c r="H26">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I26" t="e">
+        <v>0.42897387347492816</v>
+      </c>
+      <c r="I26">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>2.64E-3</v>
+      </c>
+      <c r="J26">
+        <f>F26/E26</f>
+        <v>0.88688946015424164</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -4168,13 +4298,28 @@
       <c r="B27" t="s">
         <v>40</v>
       </c>
-      <c r="H27" t="e">
+      <c r="C27">
+        <v>50000001</v>
+      </c>
+      <c r="D27">
+        <v>124666538</v>
+      </c>
+      <c r="E27">
+        <v>30134</v>
+      </c>
+      <c r="F27">
+        <v>15919</v>
+      </c>
+      <c r="G27">
+        <v>14215</v>
+      </c>
+      <c r="H27">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I27" t="e">
+        <v>0.40106994067646284</v>
+      </c>
+      <c r="I27">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.28429999431400016</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -4184,13 +4329,28 @@
       <c r="B28" t="s">
         <v>41</v>
       </c>
-      <c r="H28" t="e">
+      <c r="C28">
+        <v>50000001</v>
+      </c>
+      <c r="D28">
+        <v>124666582</v>
+      </c>
+      <c r="E28">
+        <v>30134</v>
+      </c>
+      <c r="F28">
+        <v>15661</v>
+      </c>
+      <c r="G28">
+        <v>14473</v>
+      </c>
+      <c r="H28">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I28" t="e">
+        <v>0.40106979912226998</v>
+      </c>
+      <c r="I28">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.28945999421080015</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added simulation resutls for hawkeye for gromacs benchmark
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED070278-18E0-4D22-85FB-8CC06AD4074E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265970FD-677D-4E7C-BDAF-C852BF89C42C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Benchmarks" sheetId="2" r:id="rId1"/>
@@ -856,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4DAA02D-4B80-49E4-98A1-4EF8777A053B}">
   <dimension ref="A2:L82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1751,13 +1751,28 @@
       <c r="B29" t="s">
         <v>42</v>
       </c>
-      <c r="H29" t="e">
+      <c r="C29">
+        <v>50000001</v>
+      </c>
+      <c r="D29">
+        <v>124667969</v>
+      </c>
+      <c r="E29">
+        <v>30089</v>
+      </c>
+      <c r="F29">
+        <v>15881</v>
+      </c>
+      <c r="G29">
+        <v>14208</v>
+      </c>
+      <c r="H29">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I29" t="e">
+        <v>0.40106533699927366</v>
+      </c>
+      <c r="I29">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.28415999431680011</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
@@ -1767,13 +1782,33 @@
       <c r="B30" t="s">
         <v>43</v>
       </c>
-      <c r="H30" t="e">
+      <c r="C30">
+        <v>50000001</v>
+      </c>
+      <c r="D30">
+        <v>124667969</v>
+      </c>
+      <c r="E30">
+        <v>441</v>
+      </c>
+      <c r="F30">
+        <v>19</v>
+      </c>
+      <c r="G30">
+        <f>E30-F30</f>
+        <v>422</v>
+      </c>
+      <c r="H30">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I30" t="e">
+        <v>0.40106533699927366</v>
+      </c>
+      <c r="I30">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>8.4399998312000048E-3</v>
+      </c>
+      <c r="J30">
+        <f>F30/E30</f>
+        <v>4.3083900226757371E-2</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
@@ -3466,8 +3501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E5CF80-89BD-41BF-8339-D77E14018905}">
   <dimension ref="A2:L82"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3540,11 +3575,11 @@
         <v>138391</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H10" si="0">(C3/D3)</f>
+        <f>(C3/D3)</f>
         <v>0.38087877993988939</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I10" si="1">G3/(C3/1000)</f>
+        <f>G3/(C3/1000)</f>
         <v>2.7678198892872046</v>
       </c>
     </row>
@@ -3571,11 +3606,11 @@
         <v>145179</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="H4:H67" si="0">(C4/D4)</f>
         <v>0.3806582003312366</v>
       </c>
       <c r="I4">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="I4:I67" si="1">G4/(C4/1000)</f>
         <v>2.9035798838568048</v>
       </c>
     </row>
@@ -3669,11 +3704,11 @@
         <v>79291</v>
       </c>
       <c r="H7">
-        <f>(C7/D7)</f>
+        <f t="shared" si="0"/>
         <v>0.7409131962416734</v>
       </c>
       <c r="I7">
-        <f>G7/(C7/1000)</f>
+        <f t="shared" si="1"/>
         <v>1.5858199682836007</v>
       </c>
     </row>
@@ -3798,11 +3833,11 @@
         <v>65492</v>
       </c>
       <c r="H11">
-        <f t="shared" ref="H11:H30" si="2">(C11/D11)</f>
+        <f t="shared" si="0"/>
         <v>2.0662415553740754</v>
       </c>
       <c r="I11">
-        <f t="shared" ref="I11:I30" si="3">G11/(C11/1000)</f>
+        <f t="shared" si="1"/>
         <v>1.3098399999999999</v>
       </c>
     </row>
@@ -3829,11 +3864,11 @@
         <v>64355</v>
       </c>
       <c r="H12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2.0683938417131</v>
       </c>
       <c r="I12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1.2870999999999999</v>
       </c>
     </row>
@@ -3860,11 +3895,11 @@
         <v>83499</v>
       </c>
       <c r="H13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2.0278643980055384</v>
       </c>
       <c r="I13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1.66998</v>
       </c>
     </row>
@@ -3892,11 +3927,11 @@
         <v>-4887</v>
       </c>
       <c r="H14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2.0278643980055384</v>
       </c>
       <c r="I14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-9.7739999999999994E-2</v>
       </c>
       <c r="J14">
@@ -3927,11 +3962,11 @@
         <v>384329</v>
       </c>
       <c r="H15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.28026129926817778</v>
       </c>
       <c r="I15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>7.6865800000000002</v>
       </c>
     </row>
@@ -3958,11 +3993,11 @@
         <v>383823</v>
       </c>
       <c r="H16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.28028533495555014</v>
       </c>
       <c r="I16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>7.6764599999999996</v>
       </c>
     </row>
@@ -3989,11 +4024,11 @@
         <v>368207</v>
       </c>
       <c r="H17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.2809231604756755</v>
       </c>
       <c r="I17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>7.3641399999999999</v>
       </c>
     </row>
@@ -4021,11 +4056,11 @@
         <v>13660</v>
       </c>
       <c r="H18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.2809231604756755</v>
       </c>
       <c r="I18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.2732</v>
       </c>
       <c r="J18">
@@ -4056,11 +4091,11 @@
         <v>1965529</v>
       </c>
       <c r="H19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.60779819904048604</v>
       </c>
       <c r="I19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>39.310579213788415</v>
       </c>
     </row>
@@ -4087,11 +4122,11 @@
         <v>1986062</v>
       </c>
       <c r="H20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.6027188889624876</v>
       </c>
       <c r="I20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>39.721239205575216</v>
       </c>
     </row>
@@ -4118,11 +4153,11 @@
         <v>2601691</v>
       </c>
       <c r="H21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.62079319191515714</v>
       </c>
       <c r="I21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>52.033818959323625</v>
       </c>
     </row>
@@ -4150,11 +4185,11 @@
         <v>6101</v>
       </c>
       <c r="H22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.62079319191515714</v>
       </c>
       <c r="I22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.12201999755960005</v>
       </c>
       <c r="J22">
@@ -4185,11 +4220,11 @@
         <v>17742</v>
       </c>
       <c r="H23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.42905280620614933</v>
       </c>
       <c r="I23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.35483999999999999</v>
       </c>
     </row>
@@ -4216,11 +4251,11 @@
         <v>17977</v>
       </c>
       <c r="H24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.42903479963898955</v>
       </c>
       <c r="I24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.35954000000000003</v>
       </c>
     </row>
@@ -4247,11 +4282,11 @@
         <v>21326</v>
       </c>
       <c r="H25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.42897387347492816</v>
       </c>
       <c r="I25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.42652000000000001</v>
       </c>
     </row>
@@ -4279,11 +4314,11 @@
         <v>132</v>
       </c>
       <c r="H26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.42897387347492816</v>
       </c>
       <c r="I26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>2.64E-3</v>
       </c>
       <c r="J26">
@@ -4314,11 +4349,11 @@
         <v>14215</v>
       </c>
       <c r="H27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.40106994067646284</v>
       </c>
       <c r="I27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.28429999431400016</v>
       </c>
     </row>
@@ -4345,11 +4380,11 @@
         <v>14473</v>
       </c>
       <c r="H28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.40106979912226998</v>
       </c>
       <c r="I28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.28945999421080015</v>
       </c>
     </row>
@@ -4360,13 +4395,28 @@
       <c r="B29" t="s">
         <v>42</v>
       </c>
-      <c r="H29" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I29" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C29">
+        <v>50000001</v>
+      </c>
+      <c r="D29">
+        <v>124667224</v>
+      </c>
+      <c r="E29">
+        <v>30134</v>
+      </c>
+      <c r="F29">
+        <v>15919</v>
+      </c>
+      <c r="G29">
+        <v>14215</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="0"/>
+        <v>0.40106773372927595</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="1"/>
+        <v>0.28429999431400016</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
@@ -4376,13 +4426,33 @@
       <c r="B30" t="s">
         <v>43</v>
       </c>
-      <c r="H30" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I30" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="C30">
+        <v>50000001</v>
+      </c>
+      <c r="D30">
+        <v>124667224</v>
+      </c>
+      <c r="E30">
+        <v>216</v>
+      </c>
+      <c r="F30">
+        <v>18</v>
+      </c>
+      <c r="G30">
+        <f>E30-F30</f>
+        <v>198</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="0"/>
+        <v>0.40106773372927595</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="1"/>
+        <v>3.9599999208000019E-3</v>
+      </c>
+      <c r="J30">
+        <f>F30/E30</f>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
@@ -4408,11 +4478,11 @@
         <v>41581</v>
       </c>
       <c r="H31">
-        <f t="shared" ref="H31:H63" si="4">(C31/D31)</f>
+        <f t="shared" si="0"/>
         <v>0.8858851830836687</v>
       </c>
       <c r="I31">
-        <f t="shared" ref="I31:I63" si="5">G31/(C31/1000)</f>
+        <f t="shared" si="1"/>
         <v>0.83161996673520133</v>
       </c>
     </row>
@@ -4439,11 +4509,11 @@
         <v>41140</v>
       </c>
       <c r="H32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0.88772456123727073</v>
       </c>
       <c r="I32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.82279996708800129</v>
       </c>
     </row>
@@ -4470,11 +4540,11 @@
         <v>40664</v>
       </c>
       <c r="H33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0.89055715568879878</v>
       </c>
       <c r="I33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.81327996746880127</v>
       </c>
     </row>
@@ -4502,11 +4572,11 @@
         <v>346</v>
       </c>
       <c r="H34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0.89055715568879878</v>
       </c>
       <c r="I34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>6.9199997232000108E-3</v>
       </c>
       <c r="J34">
@@ -4537,11 +4607,11 @@
         <v>22189</v>
       </c>
       <c r="H35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1.1497043351349507</v>
       </c>
       <c r="I35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.44378000000000001</v>
       </c>
     </row>
@@ -4568,11 +4638,11 @@
         <v>21249</v>
       </c>
       <c r="H36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1.1496202206608643</v>
       </c>
       <c r="I36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.42498000000000002</v>
       </c>
     </row>
@@ -4599,11 +4669,11 @@
         <v>61222</v>
       </c>
       <c r="H37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1.1484425373560794</v>
       </c>
       <c r="I37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>1.22444</v>
       </c>
     </row>
@@ -4630,11 +4700,11 @@
         <v>177</v>
       </c>
       <c r="H38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1.1484425373560794</v>
       </c>
       <c r="I38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>3.5400000000000002E-3</v>
       </c>
       <c r="J38">
@@ -4665,11 +4735,11 @@
         <v>1480824</v>
       </c>
       <c r="H39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0.6214414785017478</v>
       </c>
       <c r="I39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>29.616479999999999</v>
       </c>
     </row>
@@ -4696,11 +4766,11 @@
         <v>1546136</v>
       </c>
       <c r="H40">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0.61157898330351457</v>
       </c>
       <c r="I40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>30.922720000000002</v>
       </c>
     </row>
@@ -4727,11 +4797,11 @@
         <v>1788599</v>
       </c>
       <c r="H41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0.69991388259588538</v>
       </c>
       <c r="I41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>35.771979999999999</v>
       </c>
     </row>
@@ -4759,11 +4829,11 @@
         <v>28834</v>
       </c>
       <c r="H42">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0.69991388259588538</v>
       </c>
       <c r="I42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.57667999999999997</v>
       </c>
       <c r="J42">
@@ -4794,11 +4864,11 @@
         <v>1209677</v>
       </c>
       <c r="H43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0.65095984745563162</v>
       </c>
       <c r="I43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>24.193539999999999</v>
       </c>
     </row>
@@ -4825,11 +4895,11 @@
         <v>1208797</v>
       </c>
       <c r="H44">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0.65126816043355495</v>
       </c>
       <c r="I44">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>24.175940000000001</v>
       </c>
     </row>
@@ -4856,11 +4926,11 @@
         <v>1552962</v>
       </c>
       <c r="H45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0.64921824255479121</v>
       </c>
       <c r="I45">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>31.059239999999999</v>
       </c>
     </row>
@@ -4888,11 +4958,11 @@
         <v>5966</v>
       </c>
       <c r="H46">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0.64921824255479121</v>
       </c>
       <c r="I46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.11932</v>
       </c>
       <c r="J46">
@@ -4923,11 +4993,11 @@
         <v>1617795</v>
       </c>
       <c r="H47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0.55068272322386758</v>
       </c>
       <c r="I47">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>32.355899999999998</v>
       </c>
     </row>
@@ -4954,11 +5024,11 @@
         <v>1700034</v>
       </c>
       <c r="H48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0.53845072305747654</v>
       </c>
       <c r="I48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>34.000680000000003</v>
       </c>
     </row>
@@ -4985,11 +5055,11 @@
         <v>2080940</v>
       </c>
       <c r="H49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0.5809985538481196</v>
       </c>
       <c r="I49">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>41.6188</v>
       </c>
     </row>
@@ -5017,11 +5087,11 @@
         <v>9374</v>
       </c>
       <c r="H50">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0.5809985538481196</v>
       </c>
       <c r="I50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.18748000000000001</v>
       </c>
       <c r="J50">
@@ -5052,11 +5122,11 @@
         <v>5220177</v>
       </c>
       <c r="H51">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0.11429835816603466</v>
       </c>
       <c r="I51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>104.40354000000001</v>
       </c>
     </row>
@@ -5083,11 +5153,11 @@
         <v>5220397</v>
       </c>
       <c r="H52">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0.11339835312161432</v>
       </c>
       <c r="I52">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>104.40794</v>
       </c>
     </row>
@@ -5114,11 +5184,11 @@
         <v>5234215</v>
       </c>
       <c r="H53">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0.12027532860524762</v>
       </c>
       <c r="I53">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>104.68429999999999</v>
       </c>
     </row>
@@ -5146,11 +5216,11 @@
         <v>33432</v>
       </c>
       <c r="H54">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0.12027532860524762</v>
       </c>
       <c r="I54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.66864000000000001</v>
       </c>
       <c r="J54">
@@ -5181,11 +5251,11 @@
         <v>1530913</v>
       </c>
       <c r="H55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0.53761272327122711</v>
       </c>
       <c r="I55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>30.618258775269648</v>
       </c>
     </row>
@@ -5212,11 +5282,11 @@
         <v>1556579</v>
       </c>
       <c r="H56">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0.53446073331045418</v>
       </c>
       <c r="I56">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>31.13157875473685</v>
       </c>
     </row>
@@ -5243,11 +5313,11 @@
         <v>1823767</v>
       </c>
       <c r="H57">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0.53949176101702823</v>
       </c>
       <c r="I57">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>36.475338540986456</v>
       </c>
     </row>
@@ -5275,11 +5345,11 @@
         <v>17236</v>
       </c>
       <c r="H58">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0.53949176101702823</v>
       </c>
       <c r="I58">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>0.34471998621120054</v>
       </c>
       <c r="J58">
@@ -5310,11 +5380,11 @@
         <v>2199824</v>
       </c>
       <c r="H59">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0.33008123662160144</v>
       </c>
       <c r="I59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>43.996479120070418</v>
       </c>
     </row>
@@ -5341,11 +5411,11 @@
         <v>2014826</v>
       </c>
       <c r="H60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0.33954896258931777</v>
       </c>
       <c r="I60">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>40.296519194069617</v>
       </c>
     </row>
@@ -5372,11 +5442,11 @@
         <v>1307166</v>
       </c>
       <c r="H61">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0.36306369931419374</v>
       </c>
       <c r="I61">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>26.143319477133613</v>
       </c>
     </row>
@@ -5404,11 +5474,11 @@
         <v>1281</v>
       </c>
       <c r="H62">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0.36306369931419374</v>
       </c>
       <c r="I62">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>2.5619999487600013E-2</v>
       </c>
       <c r="J62">
@@ -5439,11 +5509,11 @@
         <v>1656235</v>
       </c>
       <c r="H63">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0.39410533186995195</v>
       </c>
       <c r="I63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>33.124699999999997</v>
       </c>
     </row>
@@ -5470,11 +5540,11 @@
         <v>1557917</v>
       </c>
       <c r="H64">
-        <f t="shared" ref="H64:H82" si="6">(C64/D64)</f>
+        <f t="shared" si="0"/>
         <v>0.40003180412855543</v>
       </c>
       <c r="I64">
-        <f t="shared" ref="I64:I82" si="7">G64/(C64/1000)</f>
+        <f t="shared" si="1"/>
         <v>31.158339999999999</v>
       </c>
     </row>
@@ -5501,11 +5571,11 @@
         <v>1601296</v>
       </c>
       <c r="H65">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>0.4036170350476655</v>
       </c>
       <c r="I65">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>32.025919999999999</v>
       </c>
     </row>
@@ -5533,11 +5603,11 @@
         <v>9635</v>
       </c>
       <c r="H66">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>0.4036170350476655</v>
       </c>
       <c r="I66">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>0.19270000000000001</v>
       </c>
       <c r="J66">
@@ -5568,11 +5638,11 @@
         <v>683074</v>
       </c>
       <c r="H67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>0.82817449636638441</v>
       </c>
       <c r="I67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>13.661479999999999</v>
       </c>
     </row>
@@ -5599,11 +5669,11 @@
         <v>620713</v>
       </c>
       <c r="H68">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="H68:H82" si="2">(C68/D68)</f>
         <v>0.85554505098329847</v>
       </c>
       <c r="I68">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="I68:I82" si="3">G68/(C68/1000)</f>
         <v>12.414260000000001</v>
       </c>
     </row>
@@ -5630,11 +5700,11 @@
         <v>526817</v>
       </c>
       <c r="H69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0.9387414151158846</v>
       </c>
       <c r="I69">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>10.536339999999999</v>
       </c>
     </row>
@@ -5662,11 +5732,11 @@
         <v>536</v>
       </c>
       <c r="H70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0.9387414151158846</v>
       </c>
       <c r="I70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>1.072E-2</v>
       </c>
       <c r="J70">
@@ -5697,11 +5767,11 @@
         <v>205369</v>
       </c>
       <c r="H71">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0.82727660689918581</v>
       </c>
       <c r="I71">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>4.10738</v>
       </c>
     </row>
@@ -5728,11 +5798,11 @@
         <v>206938</v>
       </c>
       <c r="H72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0.83316393721883109</v>
       </c>
       <c r="I72">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>4.1387600000000004</v>
       </c>
     </row>
@@ -5759,11 +5829,11 @@
         <v>138561</v>
       </c>
       <c r="H73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0.86461539201117166</v>
       </c>
       <c r="I73">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>2.77122</v>
       </c>
     </row>
@@ -5791,11 +5861,11 @@
         <v>-376</v>
       </c>
       <c r="H74">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0.86461539201117166</v>
       </c>
       <c r="I74">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>-7.5199999999999998E-3</v>
       </c>
       <c r="J74">
@@ -5826,11 +5896,11 @@
         <v>2039149</v>
       </c>
       <c r="H75">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0.25786801072287391</v>
       </c>
       <c r="I75">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>40.782980000000002</v>
       </c>
     </row>
@@ -5857,11 +5927,11 @@
         <v>2007952</v>
       </c>
       <c r="H76">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0.25947786763288749</v>
       </c>
       <c r="I76">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>40.159039999999997</v>
       </c>
     </row>
@@ -5888,11 +5958,11 @@
         <v>1834261</v>
       </c>
       <c r="H77">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0.268103087224208</v>
       </c>
       <c r="I77">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>36.685220000000001</v>
       </c>
     </row>
@@ -5920,11 +5990,11 @@
         <v>13037</v>
       </c>
       <c r="H78">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0.268103087224208</v>
       </c>
       <c r="I78">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>0.26074000000000003</v>
       </c>
       <c r="J78">
@@ -5955,11 +6025,11 @@
         <v>251674</v>
       </c>
       <c r="H79">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>1.4565732454592422</v>
       </c>
       <c r="I79">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>5.033479899330402</v>
       </c>
     </row>
@@ -5986,11 +6056,11 @@
         <v>266817</v>
       </c>
       <c r="H80">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>1.4472331436058998</v>
       </c>
       <c r="I80">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>5.3363397865464082</v>
       </c>
     </row>
@@ -6017,11 +6087,11 @@
         <v>332654</v>
       </c>
       <c r="H81">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>1.4534420093219118</v>
       </c>
       <c r="I81">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>6.6530798669384028</v>
       </c>
     </row>
@@ -6049,11 +6119,11 @@
         <v>2443</v>
       </c>
       <c r="H82">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>1.4534420093219118</v>
       </c>
       <c r="I82">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>4.885999902280002E-2</v>
       </c>
       <c r="J82">

</xml_diff>

<commit_message>
Fixed IPC to percentage
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265970FD-677D-4E7C-BDAF-C852BF89C42C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7251149A-CDB5-4E97-8717-BF6944BBA6E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="49">
   <si>
     <t>Benchmark</t>
   </si>
@@ -151,9 +151,6 @@
     <t>Total Miss</t>
   </si>
   <si>
-    <t>IPC</t>
-  </si>
-  <si>
     <t>LRU</t>
   </si>
   <si>
@@ -176,6 +173,12 @@
   </si>
   <si>
     <t>Hit Rate</t>
+  </si>
+  <si>
+    <t>IPC (%)</t>
+  </si>
+  <si>
+    <t>IPC(%)</t>
   </si>
 </sst>
 </file>
@@ -242,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -267,6 +270,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -585,7 +591,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -596,7 +602,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -610,7 +616,7 @@
         <v>2017</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" s="7"/>
     </row>
@@ -739,7 +745,7 @@
       <c r="B14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="11" t="s">
         <v>33</v>
       </c>
     </row>
@@ -750,7 +756,7 @@
       <c r="B15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="11" t="s">
         <v>26</v>
       </c>
     </row>
@@ -856,8 +862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4DAA02D-4B80-49E4-98A1-4EF8777A053B}">
   <dimension ref="A2:L82"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -879,7 +885,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>34</v>
@@ -897,13 +903,13 @@
         <v>38</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
@@ -913,7 +919,7 @@
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3">
         <v>50000002</v>
@@ -931,11 +937,11 @@
         <v>117826</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H10" si="0">(C3/D3)</f>
-        <v>0.34633020974435469</v>
+        <f>(C3/D3)*100</f>
+        <v>34.633020974435468</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I10" si="1">G3/(C3/1000)</f>
+        <f t="shared" ref="I3:I10" si="0">G3/(C3/1000)</f>
         <v>2.3565199057392037</v>
       </c>
     </row>
@@ -944,7 +950,7 @@
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4">
         <v>50000002</v>
@@ -962,11 +968,11 @@
         <v>125629</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
-        <v>0.34548741663363058</v>
+        <f t="shared" ref="H4:H67" si="1">(C4/D4)*100</f>
+        <v>34.54874166336306</v>
       </c>
       <c r="I4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.5125798994968038</v>
       </c>
     </row>
@@ -975,7 +981,7 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5">
         <v>50000002</v>
@@ -993,11 +999,11 @@
         <v>125644</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
-        <v>0.34572279553239044</v>
+        <f t="shared" si="1"/>
+        <v>34.572279553239042</v>
       </c>
       <c r="I5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.5128798994848038</v>
       </c>
     </row>
@@ -1006,7 +1012,7 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6">
         <v>50000002</v>
@@ -1025,11 +1031,11 @@
         <v>3661</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
-        <v>0.34572279553239044</v>
+        <f t="shared" si="1"/>
+        <v>34.572279553239042</v>
       </c>
       <c r="I6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7.321999707120011E-2</v>
       </c>
       <c r="J6">
@@ -1042,7 +1048,7 @@
         <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7">
         <v>50000001</v>
@@ -1060,11 +1066,11 @@
         <v>72655</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
-        <v>0.71952828359855603</v>
+        <f t="shared" si="1"/>
+        <v>71.952828359855602</v>
       </c>
       <c r="I7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.4530999709380006</v>
       </c>
     </row>
@@ -1073,7 +1079,7 @@
         <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8">
         <v>50000001</v>
@@ -1091,11 +1097,11 @@
         <v>80953</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
-        <v>0.71325574651598822</v>
+        <f t="shared" si="1"/>
+        <v>71.325574651598828</v>
       </c>
       <c r="I8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.6190599676188007</v>
       </c>
     </row>
@@ -1104,7 +1110,7 @@
         <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9">
         <v>50000001</v>
@@ -1122,11 +1128,11 @@
         <v>60051</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
-        <v>0.72893233254230572</v>
+        <f t="shared" si="1"/>
+        <v>72.893233254230566</v>
       </c>
       <c r="I9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.2010199759796005</v>
       </c>
     </row>
@@ -1135,7 +1141,7 @@
         <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10">
         <v>50000001</v>
@@ -1154,11 +1160,11 @@
         <v>1651</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
-        <v>0.72893233254230572</v>
+        <f t="shared" si="1"/>
+        <v>72.893233254230566</v>
       </c>
       <c r="I10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.3019999339600016E-2</v>
       </c>
       <c r="J10">
@@ -1171,7 +1177,7 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11">
         <v>50000001</v>
@@ -1189,11 +1195,11 @@
         <v>64328</v>
       </c>
       <c r="H11">
-        <f t="shared" ref="H11:H30" si="2">(C11/D11)</f>
-        <v>1.5705061772718236</v>
+        <f t="shared" si="1"/>
+        <v>157.05061772718236</v>
       </c>
       <c r="I11">
-        <f t="shared" ref="I11:I30" si="3">G11/(C11/1000)</f>
+        <f t="shared" ref="I11:I30" si="2">G11/(C11/1000)</f>
         <v>1.2865599742688005</v>
       </c>
     </row>
@@ -1202,7 +1208,7 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12">
         <v>50000001</v>
@@ -1220,11 +1226,11 @@
         <v>63745</v>
       </c>
       <c r="H12">
+        <f t="shared" si="1"/>
+        <v>157.52280709669216</v>
+      </c>
+      <c r="I12">
         <f t="shared" si="2"/>
-        <v>1.5752280709669215</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="3"/>
         <v>1.2748999745020007</v>
       </c>
     </row>
@@ -1233,7 +1239,7 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13">
         <v>50000001</v>
@@ -1251,11 +1257,11 @@
         <v>78662</v>
       </c>
       <c r="H13">
+        <f t="shared" si="1"/>
+        <v>152.64857017903387</v>
+      </c>
+      <c r="I13">
         <f t="shared" si="2"/>
-        <v>1.5264857017903388</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="3"/>
         <v>1.5732399685352008</v>
       </c>
     </row>
@@ -1264,7 +1270,7 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14">
         <v>50000001</v>
@@ -1283,11 +1289,11 @@
         <v>1945</v>
       </c>
       <c r="H14">
+        <f t="shared" si="1"/>
+        <v>152.64857017903387</v>
+      </c>
+      <c r="I14">
         <f t="shared" si="2"/>
-        <v>1.5264857017903388</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="3"/>
         <v>3.889999922200002E-2</v>
       </c>
       <c r="J14">
@@ -1300,7 +1306,7 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15">
         <v>50000000</v>
@@ -1318,11 +1324,11 @@
         <v>247733</v>
       </c>
       <c r="H15">
+        <f t="shared" si="1"/>
+        <v>27.318371851481839</v>
+      </c>
+      <c r="I15">
         <f t="shared" si="2"/>
-        <v>0.27318371851481837</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="3"/>
         <v>4.9546599999999996</v>
       </c>
     </row>
@@ -1331,7 +1337,7 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16">
         <v>50000000</v>
@@ -1349,11 +1355,11 @@
         <v>247495</v>
       </c>
       <c r="H16">
+        <f t="shared" si="1"/>
+        <v>27.31815438330441</v>
+      </c>
+      <c r="I16">
         <f t="shared" si="2"/>
-        <v>0.2731815438330441</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="3"/>
         <v>4.9499000000000004</v>
       </c>
     </row>
@@ -1362,7 +1368,7 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17">
         <v>50000000</v>
@@ -1380,11 +1386,11 @@
         <v>229300</v>
       </c>
       <c r="H17">
+        <f t="shared" si="1"/>
+        <v>27.531425814824896</v>
+      </c>
+      <c r="I17">
         <f t="shared" si="2"/>
-        <v>0.27531425814824895</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="3"/>
         <v>4.5860000000000003</v>
       </c>
     </row>
@@ -1393,7 +1399,7 @@
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18">
         <v>50000000</v>
@@ -1412,11 +1418,11 @@
         <v>24228</v>
       </c>
       <c r="H18">
+        <f t="shared" si="1"/>
+        <v>27.531425814824896</v>
+      </c>
+      <c r="I18">
         <f t="shared" si="2"/>
-        <v>0.27531425814824895</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="3"/>
         <v>0.48455999999999999</v>
       </c>
       <c r="J18">
@@ -1429,7 +1435,7 @@
         <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19">
         <v>50000001</v>
@@ -1447,11 +1453,11 @@
         <v>1889276</v>
       </c>
       <c r="H19">
+        <f t="shared" si="1"/>
+        <v>28.356704238486142</v>
+      </c>
+      <c r="I19">
         <f t="shared" si="2"/>
-        <v>0.28356704238486141</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="3"/>
         <v>37.785519244289617</v>
       </c>
     </row>
@@ -1460,7 +1466,7 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20">
         <v>50000001</v>
@@ -1478,11 +1484,11 @@
         <v>1916267</v>
       </c>
       <c r="H20">
+        <f t="shared" si="1"/>
+        <v>28.103190484331837</v>
+      </c>
+      <c r="I20">
         <f t="shared" si="2"/>
-        <v>0.28103190484331836</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="3"/>
         <v>38.325339233493217</v>
       </c>
     </row>
@@ -1491,7 +1497,7 @@
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C21">
         <v>50000001</v>
@@ -1509,11 +1515,11 @@
         <v>2050998</v>
       </c>
       <c r="H21">
+        <f t="shared" si="1"/>
+        <v>32.940303909082445</v>
+      </c>
+      <c r="I21">
         <f t="shared" si="2"/>
-        <v>0.32940303909082447</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="3"/>
         <v>41.019959179600818</v>
       </c>
     </row>
@@ -1522,7 +1528,7 @@
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C22">
         <v>50000001</v>
@@ -1541,11 +1547,11 @@
         <v>34940</v>
       </c>
       <c r="H22">
+        <f t="shared" si="1"/>
+        <v>32.940303909082445</v>
+      </c>
+      <c r="I22">
         <f t="shared" si="2"/>
-        <v>0.32940303909082447</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="3"/>
         <v>0.69879998602400029</v>
       </c>
       <c r="J22">
@@ -1558,7 +1564,7 @@
         <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23">
         <v>50000000</v>
@@ -1576,11 +1582,11 @@
         <v>11702</v>
       </c>
       <c r="H23">
+        <f t="shared" si="1"/>
+        <v>42.737122608343007</v>
+      </c>
+      <c r="I23">
         <f t="shared" si="2"/>
-        <v>0.42737122608343009</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="3"/>
         <v>0.23404</v>
       </c>
     </row>
@@ -1589,7 +1595,7 @@
         <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C24">
         <v>50000000</v>
@@ -1607,11 +1613,11 @@
         <v>12111</v>
       </c>
       <c r="H24">
+        <f t="shared" si="1"/>
+        <v>42.742198948164067</v>
+      </c>
+      <c r="I24">
         <f t="shared" si="2"/>
-        <v>0.42742198948164067</v>
-      </c>
-      <c r="I24">
-        <f t="shared" si="3"/>
         <v>0.24221999999999999</v>
       </c>
     </row>
@@ -1620,7 +1626,7 @@
         <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C25">
         <v>50000000</v>
@@ -1638,11 +1644,11 @@
         <v>13735</v>
       </c>
       <c r="H25">
+        <f t="shared" si="1"/>
+        <v>42.727984948400746</v>
+      </c>
+      <c r="I25">
         <f t="shared" si="2"/>
-        <v>0.42727984948400743</v>
-      </c>
-      <c r="I25">
-        <f t="shared" si="3"/>
         <v>0.2747</v>
       </c>
     </row>
@@ -1651,7 +1657,7 @@
         <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C26">
         <v>50000000</v>
@@ -1670,11 +1676,11 @@
         <v>552</v>
       </c>
       <c r="H26">
+        <f t="shared" si="1"/>
+        <v>42.727984948400746</v>
+      </c>
+      <c r="I26">
         <f t="shared" si="2"/>
-        <v>0.42727984948400743</v>
-      </c>
-      <c r="I26">
-        <f t="shared" si="3"/>
         <v>1.1039999999999999E-2</v>
       </c>
       <c r="J26">
@@ -1687,7 +1693,7 @@
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C27">
         <v>50000001</v>
@@ -1705,11 +1711,11 @@
         <v>14207</v>
       </c>
       <c r="H27">
+        <f t="shared" si="1"/>
+        <v>40.106630212200407</v>
+      </c>
+      <c r="I27">
         <f t="shared" si="2"/>
-        <v>0.40106630212200406</v>
-      </c>
-      <c r="I27">
-        <f t="shared" si="3"/>
         <v>0.28413999431720011</v>
       </c>
     </row>
@@ -1718,7 +1724,7 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C28">
         <v>50000001</v>
@@ -1736,11 +1742,11 @@
         <v>14457</v>
       </c>
       <c r="H28">
+        <f t="shared" si="1"/>
+        <v>40.106630212200407</v>
+      </c>
+      <c r="I28">
         <f t="shared" si="2"/>
-        <v>0.40106630212200406</v>
-      </c>
-      <c r="I28">
-        <f t="shared" si="3"/>
         <v>0.28913999421720016</v>
       </c>
     </row>
@@ -1749,7 +1755,7 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C29">
         <v>50000001</v>
@@ -1767,11 +1773,11 @@
         <v>14208</v>
       </c>
       <c r="H29">
+        <f t="shared" si="1"/>
+        <v>40.106533699927368</v>
+      </c>
+      <c r="I29">
         <f t="shared" si="2"/>
-        <v>0.40106533699927366</v>
-      </c>
-      <c r="I29">
-        <f t="shared" si="3"/>
         <v>0.28415999431680011</v>
       </c>
     </row>
@@ -1780,7 +1786,7 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C30">
         <v>50000001</v>
@@ -1799,11 +1805,11 @@
         <v>422</v>
       </c>
       <c r="H30">
+        <f t="shared" si="1"/>
+        <v>40.106533699927368</v>
+      </c>
+      <c r="I30">
         <f t="shared" si="2"/>
-        <v>0.40106533699927366</v>
-      </c>
-      <c r="I30">
-        <f t="shared" si="3"/>
         <v>8.4399998312000048E-3</v>
       </c>
       <c r="J30">
@@ -1816,7 +1822,7 @@
         <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C31">
         <v>50000002</v>
@@ -1834,11 +1840,11 @@
         <v>34840</v>
       </c>
       <c r="H31">
-        <f t="shared" ref="H31:H63" si="4">(C31/D31)</f>
-        <v>0.86708544811130239</v>
+        <f t="shared" si="1"/>
+        <v>86.708544811130238</v>
       </c>
       <c r="I31">
-        <f t="shared" ref="I31:I63" si="5">G31/(C31/1000)</f>
+        <f t="shared" ref="I31:I63" si="3">G31/(C31/1000)</f>
         <v>0.69679997212800115</v>
       </c>
     </row>
@@ -1847,7 +1853,7 @@
         <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C32">
         <v>50000002</v>
@@ -1865,11 +1871,11 @@
         <v>34689</v>
       </c>
       <c r="H32">
-        <f t="shared" si="4"/>
-        <v>0.86986503035550478</v>
+        <f t="shared" si="1"/>
+        <v>86.986503035550484</v>
       </c>
       <c r="I32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.69377997224880106</v>
       </c>
     </row>
@@ -1878,7 +1884,7 @@
         <v>27</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C33">
         <v>50000002</v>
@@ -1896,11 +1902,11 @@
         <v>31797</v>
       </c>
       <c r="H33">
-        <f t="shared" si="4"/>
-        <v>0.87093187302914654</v>
+        <f t="shared" si="1"/>
+        <v>87.093187302914657</v>
       </c>
       <c r="I33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.63593997456240103</v>
       </c>
     </row>
@@ -1909,7 +1915,7 @@
         <v>27</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C34">
         <v>50000002</v>
@@ -1928,11 +1934,11 @@
         <v>1004</v>
       </c>
       <c r="H34">
-        <f t="shared" si="4"/>
-        <v>0.87093187302914654</v>
+        <f t="shared" si="1"/>
+        <v>87.093187302914657</v>
       </c>
       <c r="I34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>2.0079999196800032E-2</v>
       </c>
       <c r="J34">
@@ -1945,7 +1951,7 @@
         <v>13</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C35">
         <v>50000000</v>
@@ -1963,11 +1969,11 @@
         <v>21925</v>
       </c>
       <c r="H35">
-        <f t="shared" si="4"/>
-        <v>1.1112592790149798</v>
+        <f t="shared" si="1"/>
+        <v>111.12592790149797</v>
       </c>
       <c r="I35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.4385</v>
       </c>
     </row>
@@ -1976,7 +1982,7 @@
         <v>13</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C36">
         <v>50000000</v>
@@ -1994,11 +2000,11 @@
         <v>21071</v>
       </c>
       <c r="H36">
-        <f t="shared" si="4"/>
-        <v>1.1119536507473229</v>
+        <f t="shared" si="1"/>
+        <v>111.19536507473229</v>
       </c>
       <c r="I36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.42142000000000002</v>
       </c>
     </row>
@@ -2007,7 +2013,7 @@
         <v>13</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C37">
         <v>50000000</v>
@@ -2025,11 +2031,11 @@
         <v>10122</v>
       </c>
       <c r="H37">
-        <f t="shared" si="4"/>
-        <v>1.1217057213564985</v>
+        <f t="shared" si="1"/>
+        <v>112.17057213564985</v>
       </c>
       <c r="I37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.20244000000000001</v>
       </c>
     </row>
@@ -2038,7 +2044,7 @@
         <v>13</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C38">
         <v>50000000</v>
@@ -2057,11 +2063,11 @@
         <v>1563</v>
       </c>
       <c r="H38">
-        <f t="shared" si="4"/>
-        <v>1.1217057213564985</v>
+        <f t="shared" si="1"/>
+        <v>112.17057213564985</v>
       </c>
       <c r="I38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>3.1260000000000003E-2</v>
       </c>
       <c r="J38">
@@ -2074,7 +2080,7 @@
         <v>4</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C39">
         <v>50000000</v>
@@ -2092,11 +2098,11 @@
         <v>1480793</v>
       </c>
       <c r="H39">
-        <f t="shared" si="4"/>
-        <v>0.53612768228164276</v>
+        <f t="shared" si="1"/>
+        <v>53.612768228164278</v>
       </c>
       <c r="I39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>29.615860000000001</v>
       </c>
     </row>
@@ -2105,7 +2111,7 @@
         <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C40">
         <v>50000000</v>
@@ -2123,11 +2129,11 @@
         <v>1542270</v>
       </c>
       <c r="H40">
-        <f t="shared" si="4"/>
-        <v>0.52872795772798831</v>
+        <f t="shared" si="1"/>
+        <v>52.872795772798831</v>
       </c>
       <c r="I40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>30.845400000000001</v>
       </c>
     </row>
@@ -2136,7 +2142,7 @@
         <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C41">
         <v>50000000</v>
@@ -2154,11 +2160,11 @@
         <v>1758698</v>
       </c>
       <c r="H41">
-        <f t="shared" si="4"/>
-        <v>0.60657587204471231</v>
+        <f t="shared" si="1"/>
+        <v>60.657587204471227</v>
       </c>
       <c r="I41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>35.173960000000001</v>
       </c>
     </row>
@@ -2167,7 +2173,7 @@
         <v>4</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C42">
         <v>50000000</v>
@@ -2186,11 +2192,11 @@
         <v>35581</v>
       </c>
       <c r="H42">
-        <f t="shared" si="4"/>
-        <v>0.60657587204471231</v>
+        <f t="shared" si="1"/>
+        <v>60.657587204471227</v>
       </c>
       <c r="I42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.71162000000000003</v>
       </c>
       <c r="J42">
@@ -2203,7 +2209,7 @@
         <v>33</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C43">
         <v>50000000</v>
@@ -2221,11 +2227,11 @@
         <v>1186020</v>
       </c>
       <c r="H43">
-        <f t="shared" si="4"/>
-        <v>0.46778434692533771</v>
+        <f t="shared" si="1"/>
+        <v>46.778434692533772</v>
       </c>
       <c r="I43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>23.720400000000001</v>
       </c>
     </row>
@@ -2234,7 +2240,7 @@
         <v>33</v>
       </c>
       <c r="B44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C44">
         <v>50000000</v>
@@ -2252,11 +2258,11 @@
         <v>1179769</v>
       </c>
       <c r="H44">
-        <f t="shared" si="4"/>
-        <v>0.46882319648662396</v>
+        <f t="shared" si="1"/>
+        <v>46.882319648662396</v>
       </c>
       <c r="I44">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>23.595379999999999</v>
       </c>
     </row>
@@ -2265,7 +2271,7 @@
         <v>33</v>
       </c>
       <c r="B45" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C45">
         <v>50000000</v>
@@ -2283,11 +2289,11 @@
         <v>1515306</v>
       </c>
       <c r="H45">
-        <f t="shared" si="4"/>
-        <v>0.46999729497756848</v>
+        <f t="shared" si="1"/>
+        <v>46.999729497756846</v>
       </c>
       <c r="I45">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>30.30612</v>
       </c>
     </row>
@@ -2296,7 +2302,7 @@
         <v>33</v>
       </c>
       <c r="B46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C46">
         <v>50000000</v>
@@ -2315,11 +2321,11 @@
         <v>35658</v>
       </c>
       <c r="H46">
-        <f t="shared" si="4"/>
-        <v>0.46999729497756848</v>
+        <f t="shared" si="1"/>
+        <v>46.999729497756846</v>
       </c>
       <c r="I46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.71316000000000002</v>
       </c>
       <c r="J46">
@@ -2332,7 +2338,7 @@
         <v>26</v>
       </c>
       <c r="B47" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C47">
         <v>50000001</v>
@@ -2350,11 +2356,11 @@
         <v>1617780</v>
       </c>
       <c r="H47">
-        <f t="shared" si="4"/>
-        <v>0.43524860590309566</v>
+        <f t="shared" si="1"/>
+        <v>43.524860590309565</v>
       </c>
       <c r="I47">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>32.355599352888014</v>
       </c>
     </row>
@@ -2363,7 +2369,7 @@
         <v>26</v>
       </c>
       <c r="B48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C48">
         <v>50000001</v>
@@ -2381,11 +2387,11 @@
         <v>1700011</v>
       </c>
       <c r="H48">
-        <f t="shared" si="4"/>
-        <v>0.42754201491637622</v>
+        <f t="shared" si="1"/>
+        <v>42.754201491637623</v>
       </c>
       <c r="I48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>34.000219319995615</v>
       </c>
     </row>
@@ -2394,7 +2400,7 @@
         <v>26</v>
       </c>
       <c r="B49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C49">
         <v>50000001</v>
@@ -2412,11 +2418,11 @@
         <v>2080232</v>
       </c>
       <c r="H49">
-        <f t="shared" si="4"/>
-        <v>0.45563303483781048</v>
+        <f t="shared" si="1"/>
+        <v>45.563303483781048</v>
       </c>
       <c r="I49">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>41.604639167907223</v>
       </c>
     </row>
@@ -2425,7 +2431,7 @@
         <v>26</v>
       </c>
       <c r="B50" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C50">
         <v>50000001</v>
@@ -2444,11 +2450,11 @@
         <v>49697</v>
       </c>
       <c r="H50">
-        <f t="shared" si="4"/>
-        <v>0.45563303483781048</v>
+        <f t="shared" si="1"/>
+        <v>45.563303483781048</v>
       </c>
       <c r="I50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.99393998012120044</v>
       </c>
       <c r="J50">
@@ -2461,7 +2467,7 @@
         <v>15</v>
       </c>
       <c r="B51" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C51">
         <v>50000001</v>
@@ -2479,11 +2485,11 @@
         <v>3581162</v>
       </c>
       <c r="H51">
-        <f t="shared" si="4"/>
-        <v>9.8855279219379893E-2</v>
+        <f t="shared" si="1"/>
+        <v>9.8855279219379888</v>
       </c>
       <c r="I51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>71.623238567535239</v>
       </c>
     </row>
@@ -2492,7 +2498,7 @@
         <v>15</v>
       </c>
       <c r="B52" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C52">
         <v>50000001</v>
@@ -2510,11 +2516,11 @@
         <v>3448279</v>
       </c>
       <c r="H52">
-        <f t="shared" si="4"/>
-        <v>0.10071219067343981</v>
+        <f t="shared" si="1"/>
+        <v>10.07121906734398</v>
       </c>
       <c r="I52">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>68.965578620688433</v>
       </c>
     </row>
@@ -2523,7 +2529,7 @@
         <v>15</v>
       </c>
       <c r="B53" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C53">
         <v>50000001</v>
@@ -2541,11 +2547,11 @@
         <v>3215361</v>
       </c>
       <c r="H53">
-        <f t="shared" si="4"/>
-        <v>0.11189435817535065</v>
+        <f t="shared" si="1"/>
+        <v>11.189435817535065</v>
       </c>
       <c r="I53">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>64.307218713855633</v>
       </c>
     </row>
@@ -2554,7 +2560,7 @@
         <v>15</v>
       </c>
       <c r="B54" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C54">
         <v>50000001</v>
@@ -2573,11 +2579,11 @@
         <v>81826</v>
       </c>
       <c r="H54">
-        <f t="shared" si="4"/>
-        <v>0.11189435817535065</v>
+        <f t="shared" si="1"/>
+        <v>11.189435817535065</v>
       </c>
       <c r="I54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1.6365199672696007</v>
       </c>
       <c r="J54">
@@ -2590,7 +2596,7 @@
         <v>20</v>
       </c>
       <c r="B55" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C55">
         <v>50000002</v>
@@ -2608,11 +2614,11 @@
         <v>1184616</v>
       </c>
       <c r="H55">
-        <f t="shared" si="4"/>
-        <v>0.41144798678837274</v>
+        <f t="shared" si="1"/>
+        <v>41.144798678837276</v>
       </c>
       <c r="I55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>23.692319052307237</v>
       </c>
     </row>
@@ -2621,7 +2627,7 @@
         <v>20</v>
       </c>
       <c r="B56" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C56">
         <v>50000002</v>
@@ -2639,11 +2645,11 @@
         <v>1210391</v>
       </c>
       <c r="H56">
-        <f t="shared" si="4"/>
-        <v>0.40866732022921465</v>
+        <f t="shared" si="1"/>
+        <v>40.866732022921468</v>
       </c>
       <c r="I56">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>24.20781903168724</v>
       </c>
     </row>
@@ -2652,7 +2658,7 @@
         <v>20</v>
       </c>
       <c r="B57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C57">
         <v>50000002</v>
@@ -2670,11 +2676,11 @@
         <v>1471540</v>
       </c>
       <c r="H57">
-        <f t="shared" si="4"/>
-        <v>0.4159021408254075</v>
+        <f t="shared" si="1"/>
+        <v>41.590214082540747</v>
       </c>
       <c r="I57">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>29.430798822768047</v>
       </c>
     </row>
@@ -2683,7 +2689,7 @@
         <v>20</v>
       </c>
       <c r="B58" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C58">
         <v>50000002</v>
@@ -2702,11 +2708,11 @@
         <v>32166</v>
       </c>
       <c r="H58">
-        <f t="shared" si="4"/>
-        <v>0.4159021408254075</v>
+        <f t="shared" si="1"/>
+        <v>41.590214082540747</v>
       </c>
       <c r="I58">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.643319974267201</v>
       </c>
       <c r="J58">
@@ -2719,7 +2725,7 @@
         <v>5</v>
       </c>
       <c r="B59" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C59">
         <v>50000001</v>
@@ -2737,11 +2743,11 @@
         <v>341714</v>
       </c>
       <c r="H59">
-        <f t="shared" si="4"/>
-        <v>0.35310253643363099</v>
+        <f t="shared" si="1"/>
+        <v>35.310253643363097</v>
       </c>
       <c r="I59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>6.8342798633144035</v>
       </c>
     </row>
@@ -2750,7 +2756,7 @@
         <v>5</v>
       </c>
       <c r="B60" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C60">
         <v>50000001</v>
@@ -2768,11 +2774,11 @@
         <v>254361</v>
       </c>
       <c r="H60">
-        <f t="shared" si="4"/>
-        <v>0.36126249795715093</v>
+        <f t="shared" si="1"/>
+        <v>36.12624979571509</v>
       </c>
       <c r="I60">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>5.0872198982556025</v>
       </c>
     </row>
@@ -2781,7 +2787,7 @@
         <v>5</v>
       </c>
       <c r="B61" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C61">
         <v>50000001</v>
@@ -2799,11 +2805,11 @@
         <v>265842</v>
       </c>
       <c r="H61">
-        <f t="shared" si="4"/>
-        <v>0.35718865587139698</v>
+        <f t="shared" si="1"/>
+        <v>35.718865587139696</v>
       </c>
       <c r="I61">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>5.3168398936632029</v>
       </c>
     </row>
@@ -2812,7 +2818,7 @@
         <v>5</v>
       </c>
       <c r="B62" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C62">
         <v>50000001</v>
@@ -2831,11 +2837,11 @@
         <v>3085</v>
       </c>
       <c r="H62">
-        <f t="shared" si="4"/>
-        <v>0.35718865587139698</v>
+        <f t="shared" si="1"/>
+        <v>35.718865587139696</v>
       </c>
       <c r="I62">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>6.1699998766000026E-2</v>
       </c>
       <c r="J62">
@@ -2848,7 +2854,7 @@
         <v>16</v>
       </c>
       <c r="B63" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C63">
         <v>50000000</v>
@@ -2866,11 +2872,11 @@
         <v>1318666</v>
       </c>
       <c r="H63">
-        <f t="shared" si="4"/>
-        <v>0.29845220893731855</v>
+        <f t="shared" si="1"/>
+        <v>29.845220893731856</v>
       </c>
       <c r="I63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>26.37332</v>
       </c>
     </row>
@@ -2879,7 +2885,7 @@
         <v>16</v>
       </c>
       <c r="B64" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C64">
         <v>50000000</v>
@@ -2897,11 +2903,11 @@
         <v>1235010</v>
       </c>
       <c r="H64">
-        <f t="shared" ref="H64:H82" si="6">(C64/D64)</f>
-        <v>0.30707278221273787</v>
+        <f t="shared" si="1"/>
+        <v>30.707278221273786</v>
       </c>
       <c r="I64">
-        <f t="shared" ref="I64:I82" si="7">G64/(C64/1000)</f>
+        <f t="shared" ref="I64:I82" si="4">G64/(C64/1000)</f>
         <v>24.700199999999999</v>
       </c>
     </row>
@@ -2910,7 +2916,7 @@
         <v>16</v>
       </c>
       <c r="B65" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C65">
         <v>50000000</v>
@@ -2928,11 +2934,11 @@
         <v>1241252</v>
       </c>
       <c r="H65">
-        <f t="shared" si="6"/>
-        <v>0.31862572696530672</v>
+        <f t="shared" si="1"/>
+        <v>31.862572696530673</v>
       </c>
       <c r="I65">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>24.825040000000001</v>
       </c>
     </row>
@@ -2941,7 +2947,7 @@
         <v>16</v>
       </c>
       <c r="B66" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C66">
         <v>50000000</v>
@@ -2960,11 +2966,11 @@
         <v>28285</v>
       </c>
       <c r="H66">
-        <f t="shared" si="6"/>
-        <v>0.31862572696530672</v>
+        <f t="shared" si="1"/>
+        <v>31.862572696530673</v>
       </c>
       <c r="I66">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>0.56569999999999998</v>
       </c>
       <c r="J66">
@@ -2977,7 +2983,7 @@
         <v>19</v>
       </c>
       <c r="B67" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C67">
         <v>50000000</v>
@@ -2995,11 +3001,11 @@
         <v>594001</v>
       </c>
       <c r="H67">
-        <f t="shared" si="6"/>
-        <v>0.53897695383053346</v>
+        <f t="shared" si="1"/>
+        <v>53.897695383053346</v>
       </c>
       <c r="I67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>11.88002</v>
       </c>
     </row>
@@ -3008,7 +3014,7 @@
         <v>19</v>
       </c>
       <c r="B68" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C68">
         <v>50000000</v>
@@ -3026,11 +3032,11 @@
         <v>539116</v>
       </c>
       <c r="H68">
-        <f t="shared" si="6"/>
-        <v>0.55711612448273995</v>
+        <f t="shared" ref="H68:H82" si="5">(C68/D68)*100</f>
+        <v>55.711612448273996</v>
       </c>
       <c r="I68">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>10.78232</v>
       </c>
     </row>
@@ -3039,7 +3045,7 @@
         <v>19</v>
       </c>
       <c r="B69" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C69">
         <v>50000000</v>
@@ -3057,11 +3063,11 @@
         <v>377542</v>
       </c>
       <c r="H69">
-        <f t="shared" si="6"/>
-        <v>0.64006848425548657</v>
+        <f t="shared" si="5"/>
+        <v>64.006848425548654</v>
       </c>
       <c r="I69">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>7.55084</v>
       </c>
     </row>
@@ -3070,7 +3076,7 @@
         <v>19</v>
       </c>
       <c r="B70" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C70">
         <v>50000000</v>
@@ -3089,11 +3095,11 @@
         <v>11093</v>
       </c>
       <c r="H70">
-        <f t="shared" si="6"/>
-        <v>0.64006848425548657</v>
+        <f t="shared" si="5"/>
+        <v>64.006848425548654</v>
       </c>
       <c r="I70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>0.22186</v>
       </c>
       <c r="J70">
@@ -3106,7 +3112,7 @@
         <v>12</v>
       </c>
       <c r="B71" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C71">
         <v>50000000</v>
@@ -3124,11 +3130,11 @@
         <v>204437</v>
       </c>
       <c r="H71">
-        <f t="shared" si="6"/>
-        <v>0.62386126603111336</v>
+        <f t="shared" si="5"/>
+        <v>62.386126603111336</v>
       </c>
       <c r="I71">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>4.0887399999999996</v>
       </c>
     </row>
@@ -3137,7 +3143,7 @@
         <v>12</v>
       </c>
       <c r="B72" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C72">
         <v>50000000</v>
@@ -3155,11 +3161,11 @@
         <v>206688</v>
       </c>
       <c r="H72">
-        <f t="shared" si="6"/>
-        <v>0.62506214680394601</v>
+        <f t="shared" si="5"/>
+        <v>62.506214680394599</v>
       </c>
       <c r="I72">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>4.1337599999999997</v>
       </c>
     </row>
@@ -3168,7 +3174,7 @@
         <v>12</v>
       </c>
       <c r="B73" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C73">
         <v>50000000</v>
@@ -3186,11 +3192,11 @@
         <v>122950</v>
       </c>
       <c r="H73">
-        <f t="shared" si="6"/>
-        <v>0.68902095950771269</v>
+        <f t="shared" si="5"/>
+        <v>68.902095950771269</v>
       </c>
       <c r="I73">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>2.4590000000000001</v>
       </c>
     </row>
@@ -3199,7 +3205,7 @@
         <v>12</v>
       </c>
       <c r="B74" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C74">
         <v>50000000</v>
@@ -3218,11 +3224,11 @@
         <v>2630</v>
       </c>
       <c r="H74">
-        <f t="shared" si="6"/>
-        <v>0.68902095950771269</v>
+        <f t="shared" si="5"/>
+        <v>68.902095950771269</v>
       </c>
       <c r="I74">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>5.2600000000000001E-2</v>
       </c>
       <c r="J74">
@@ -3235,7 +3241,7 @@
         <v>22</v>
       </c>
       <c r="B75" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C75">
         <v>50000000</v>
@@ -3253,11 +3259,11 @@
         <v>1452769</v>
       </c>
       <c r="H75">
-        <f t="shared" si="6"/>
-        <v>0.20528993991225045</v>
+        <f t="shared" si="5"/>
+        <v>20.528993991225043</v>
       </c>
       <c r="I75">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>29.05538</v>
       </c>
     </row>
@@ -3266,7 +3272,7 @@
         <v>22</v>
       </c>
       <c r="B76" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C76">
         <v>50000000</v>
@@ -3284,11 +3290,11 @@
         <v>1425177</v>
       </c>
       <c r="H76">
-        <f t="shared" si="6"/>
-        <v>0.207164070832495</v>
+        <f t="shared" si="5"/>
+        <v>20.7164070832495</v>
       </c>
       <c r="I76">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>28.503540000000001</v>
       </c>
     </row>
@@ -3297,7 +3303,7 @@
         <v>22</v>
       </c>
       <c r="B77" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C77">
         <v>50000000</v>
@@ -3315,11 +3321,11 @@
         <v>1224215</v>
       </c>
       <c r="H77">
-        <f t="shared" si="6"/>
-        <v>0.21927080502684285</v>
+        <f t="shared" si="5"/>
+        <v>21.927080502684284</v>
       </c>
       <c r="I77">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>24.484300000000001</v>
       </c>
     </row>
@@ -3328,7 +3334,7 @@
         <v>22</v>
       </c>
       <c r="B78" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C78">
         <v>50000000</v>
@@ -3347,11 +3353,11 @@
         <v>30792</v>
       </c>
       <c r="H78">
-        <f t="shared" si="6"/>
-        <v>0.21927080502684285</v>
+        <f t="shared" si="5"/>
+        <v>21.927080502684284</v>
       </c>
       <c r="I78">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>0.61584000000000005</v>
       </c>
       <c r="J78">
@@ -3364,7 +3370,7 @@
         <v>23</v>
       </c>
       <c r="B79" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C79">
         <v>50000000</v>
@@ -3382,11 +3388,11 @@
         <v>251526</v>
       </c>
       <c r="H79">
-        <f t="shared" si="6"/>
-        <v>1.1464893521521153</v>
+        <f t="shared" si="5"/>
+        <v>114.64893521521154</v>
       </c>
       <c r="I79">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>5.0305200000000001</v>
       </c>
     </row>
@@ -3395,7 +3401,7 @@
         <v>23</v>
       </c>
       <c r="B80" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C80">
         <v>50000000</v>
@@ -3413,11 +3419,11 @@
         <v>266471</v>
       </c>
       <c r="H80">
-        <f t="shared" si="6"/>
-        <v>1.1387878050220359</v>
+        <f t="shared" si="5"/>
+        <v>113.8787805022036</v>
       </c>
       <c r="I80">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>5.3294199999999998</v>
       </c>
     </row>
@@ -3426,7 +3432,7 @@
         <v>23</v>
       </c>
       <c r="B81" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C81">
         <v>50000000</v>
@@ -3444,11 +3450,11 @@
         <v>328367</v>
       </c>
       <c r="H81">
-        <f t="shared" si="6"/>
-        <v>1.1476317895015609</v>
+        <f t="shared" si="5"/>
+        <v>114.76317895015609</v>
       </c>
       <c r="I81">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>6.5673399999999997</v>
       </c>
     </row>
@@ -3457,7 +3463,7 @@
         <v>23</v>
       </c>
       <c r="B82" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C82">
         <v>50000000</v>
@@ -3476,11 +3482,11 @@
         <v>7440</v>
       </c>
       <c r="H82">
-        <f t="shared" si="6"/>
-        <v>1.1476317895015609</v>
+        <f t="shared" si="5"/>
+        <v>114.76317895015609</v>
       </c>
       <c r="I82">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>0.14879999999999999</v>
       </c>
       <c r="J82">
@@ -3502,7 +3508,7 @@
   <dimension ref="A2:L82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3523,7 +3529,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>34</v>
@@ -3541,13 +3547,13 @@
         <v>38</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
@@ -3557,7 +3563,7 @@
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3">
         <v>50000002</v>
@@ -3575,8 +3581,8 @@
         <v>138391</v>
       </c>
       <c r="H3">
-        <f>(C3/D3)</f>
-        <v>0.38087877993988939</v>
+        <f>(C3/D3)*100</f>
+        <v>38.08787799398894</v>
       </c>
       <c r="I3">
         <f>G3/(C3/1000)</f>
@@ -3588,7 +3594,7 @@
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4">
         <v>50000002</v>
@@ -3606,8 +3612,8 @@
         <v>145179</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H67" si="0">(C4/D4)</f>
-        <v>0.3806582003312366</v>
+        <f t="shared" ref="H4:H67" si="0">(C4/D4)*100</f>
+        <v>38.065820033123657</v>
       </c>
       <c r="I4">
         <f t="shared" ref="I4:I67" si="1">G4/(C4/1000)</f>
@@ -3619,7 +3625,7 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5">
         <v>50000002</v>
@@ -3638,7 +3644,7 @@
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>0.38050076135535799</v>
+        <v>38.050076135535797</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
@@ -3650,7 +3656,7 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6">
         <v>50000002</v>
@@ -3670,7 +3676,7 @@
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>0.38050076135535799</v>
+        <v>38.050076135535797</v>
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
@@ -3686,7 +3692,7 @@
         <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7">
         <v>50000001</v>
@@ -3705,7 +3711,7 @@
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>0.7409131962416734</v>
+        <v>74.09131962416734</v>
       </c>
       <c r="I7">
         <f t="shared" si="1"/>
@@ -3717,7 +3723,7 @@
         <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8">
         <v>50000001</v>
@@ -3736,7 +3742,7 @@
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>0.73770340658737854</v>
+        <v>73.770340658737851</v>
       </c>
       <c r="I8">
         <f t="shared" si="1"/>
@@ -3748,7 +3754,7 @@
         <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9">
         <v>50000001</v>
@@ -3767,7 +3773,7 @@
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>0.7475730191931893</v>
+        <v>74.757301919318934</v>
       </c>
       <c r="I9">
         <f t="shared" si="1"/>
@@ -3779,7 +3785,7 @@
         <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10">
         <v>50000001</v>
@@ -3799,7 +3805,7 @@
       </c>
       <c r="H10">
         <f t="shared" si="0"/>
-        <v>0.7475730191931893</v>
+        <v>74.757301919318934</v>
       </c>
       <c r="I10">
         <f t="shared" si="1"/>
@@ -3815,7 +3821,7 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11">
         <v>50000000</v>
@@ -3834,7 +3840,7 @@
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>2.0662415553740754</v>
+        <v>206.62415553740755</v>
       </c>
       <c r="I11">
         <f t="shared" si="1"/>
@@ -3846,7 +3852,7 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12">
         <v>50000000</v>
@@ -3865,7 +3871,7 @@
       </c>
       <c r="H12">
         <f t="shared" si="0"/>
-        <v>2.0683938417131</v>
+        <v>206.83938417131</v>
       </c>
       <c r="I12">
         <f t="shared" si="1"/>
@@ -3877,7 +3883,7 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13">
         <v>50000000</v>
@@ -3896,7 +3902,7 @@
       </c>
       <c r="H13">
         <f t="shared" si="0"/>
-        <v>2.0278643980055384</v>
+        <v>202.78643980055384</v>
       </c>
       <c r="I13">
         <f t="shared" si="1"/>
@@ -3908,7 +3914,7 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14">
         <v>50000000</v>
@@ -3928,7 +3934,7 @@
       </c>
       <c r="H14">
         <f t="shared" si="0"/>
-        <v>2.0278643980055384</v>
+        <v>202.78643980055384</v>
       </c>
       <c r="I14">
         <f t="shared" si="1"/>
@@ -3944,7 +3950,7 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15">
         <v>50000000</v>
@@ -3963,7 +3969,7 @@
       </c>
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>0.28026129926817778</v>
+        <v>28.026129926817777</v>
       </c>
       <c r="I15">
         <f t="shared" si="1"/>
@@ -3975,7 +3981,7 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16">
         <v>50000000</v>
@@ -3994,7 +4000,7 @@
       </c>
       <c r="H16">
         <f t="shared" si="0"/>
-        <v>0.28028533495555014</v>
+        <v>28.028533495555013</v>
       </c>
       <c r="I16">
         <f t="shared" si="1"/>
@@ -4006,7 +4012,7 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17">
         <v>50000000</v>
@@ -4025,7 +4031,7 @@
       </c>
       <c r="H17">
         <f t="shared" si="0"/>
-        <v>0.2809231604756755</v>
+        <v>28.09231604756755</v>
       </c>
       <c r="I17">
         <f t="shared" si="1"/>
@@ -4037,7 +4043,7 @@
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18">
         <v>50000000</v>
@@ -4057,7 +4063,7 @@
       </c>
       <c r="H18">
         <f t="shared" si="0"/>
-        <v>0.2809231604756755</v>
+        <v>28.09231604756755</v>
       </c>
       <c r="I18">
         <f t="shared" si="1"/>
@@ -4073,7 +4079,7 @@
         <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19">
         <v>50000001</v>
@@ -4092,7 +4098,7 @@
       </c>
       <c r="H19">
         <f t="shared" si="0"/>
-        <v>0.60779819904048604</v>
+        <v>60.779819904048601</v>
       </c>
       <c r="I19">
         <f t="shared" si="1"/>
@@ -4104,7 +4110,7 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20">
         <v>50000001</v>
@@ -4123,7 +4129,7 @@
       </c>
       <c r="H20">
         <f t="shared" si="0"/>
-        <v>0.6027188889624876</v>
+        <v>60.271888896248761</v>
       </c>
       <c r="I20">
         <f t="shared" si="1"/>
@@ -4135,7 +4141,7 @@
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C21">
         <v>50000001</v>
@@ -4154,7 +4160,7 @@
       </c>
       <c r="H21">
         <f t="shared" si="0"/>
-        <v>0.62079319191515714</v>
+        <v>62.079319191515715</v>
       </c>
       <c r="I21">
         <f t="shared" si="1"/>
@@ -4166,7 +4172,7 @@
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C22">
         <v>50000001</v>
@@ -4186,7 +4192,7 @@
       </c>
       <c r="H22">
         <f t="shared" si="0"/>
-        <v>0.62079319191515714</v>
+        <v>62.079319191515715</v>
       </c>
       <c r="I22">
         <f t="shared" si="1"/>
@@ -4202,7 +4208,7 @@
         <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23">
         <v>50000000</v>
@@ -4221,7 +4227,7 @@
       </c>
       <c r="H23">
         <f t="shared" si="0"/>
-        <v>0.42905280620614933</v>
+        <v>42.905280620614931</v>
       </c>
       <c r="I23">
         <f t="shared" si="1"/>
@@ -4233,7 +4239,7 @@
         <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C24">
         <v>50000000</v>
@@ -4252,7 +4258,7 @@
       </c>
       <c r="H24">
         <f t="shared" si="0"/>
-        <v>0.42903479963898955</v>
+        <v>42.903479963898953</v>
       </c>
       <c r="I24">
         <f t="shared" si="1"/>
@@ -4264,7 +4270,7 @@
         <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C25">
         <v>50000000</v>
@@ -4283,7 +4289,7 @@
       </c>
       <c r="H25">
         <f t="shared" si="0"/>
-        <v>0.42897387347492816</v>
+        <v>42.897387347492817</v>
       </c>
       <c r="I25">
         <f t="shared" si="1"/>
@@ -4295,7 +4301,7 @@
         <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C26">
         <v>50000000</v>
@@ -4315,7 +4321,7 @@
       </c>
       <c r="H26">
         <f t="shared" si="0"/>
-        <v>0.42897387347492816</v>
+        <v>42.897387347492817</v>
       </c>
       <c r="I26">
         <f t="shared" si="1"/>
@@ -4331,7 +4337,7 @@
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C27">
         <v>50000001</v>
@@ -4350,7 +4356,7 @@
       </c>
       <c r="H27">
         <f t="shared" si="0"/>
-        <v>0.40106994067646284</v>
+        <v>40.106994067646283</v>
       </c>
       <c r="I27">
         <f t="shared" si="1"/>
@@ -4362,7 +4368,7 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C28">
         <v>50000001</v>
@@ -4381,7 +4387,7 @@
       </c>
       <c r="H28">
         <f t="shared" si="0"/>
-        <v>0.40106979912226998</v>
+        <v>40.106979912226997</v>
       </c>
       <c r="I28">
         <f t="shared" si="1"/>
@@ -4393,7 +4399,7 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C29">
         <v>50000001</v>
@@ -4412,7 +4418,7 @@
       </c>
       <c r="H29">
         <f t="shared" si="0"/>
-        <v>0.40106773372927595</v>
+        <v>40.106773372927599</v>
       </c>
       <c r="I29">
         <f t="shared" si="1"/>
@@ -4424,7 +4430,7 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C30">
         <v>50000001</v>
@@ -4444,7 +4450,7 @@
       </c>
       <c r="H30">
         <f t="shared" si="0"/>
-        <v>0.40106773372927595</v>
+        <v>40.106773372927599</v>
       </c>
       <c r="I30">
         <f t="shared" si="1"/>
@@ -4460,7 +4466,7 @@
         <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C31">
         <v>50000002</v>
@@ -4479,7 +4485,7 @@
       </c>
       <c r="H31">
         <f t="shared" si="0"/>
-        <v>0.8858851830836687</v>
+        <v>88.588518308366872</v>
       </c>
       <c r="I31">
         <f t="shared" si="1"/>
@@ -4491,7 +4497,7 @@
         <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C32">
         <v>50000002</v>
@@ -4510,7 +4516,7 @@
       </c>
       <c r="H32">
         <f t="shared" si="0"/>
-        <v>0.88772456123727073</v>
+        <v>88.772456123727068</v>
       </c>
       <c r="I32">
         <f t="shared" si="1"/>
@@ -4522,7 +4528,7 @@
         <v>27</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C33">
         <v>50000002</v>
@@ -4541,7 +4547,7 @@
       </c>
       <c r="H33">
         <f t="shared" si="0"/>
-        <v>0.89055715568879878</v>
+        <v>89.055715568879876</v>
       </c>
       <c r="I33">
         <f t="shared" si="1"/>
@@ -4553,7 +4559,7 @@
         <v>27</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C34">
         <v>50000002</v>
@@ -4573,7 +4579,7 @@
       </c>
       <c r="H34">
         <f t="shared" si="0"/>
-        <v>0.89055715568879878</v>
+        <v>89.055715568879876</v>
       </c>
       <c r="I34">
         <f t="shared" si="1"/>
@@ -4589,7 +4595,7 @@
         <v>13</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C35">
         <v>50000000</v>
@@ -4608,7 +4614,7 @@
       </c>
       <c r="H35">
         <f t="shared" si="0"/>
-        <v>1.1497043351349507</v>
+        <v>114.97043351349507</v>
       </c>
       <c r="I35">
         <f t="shared" si="1"/>
@@ -4620,7 +4626,7 @@
         <v>13</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C36">
         <v>50000000</v>
@@ -4639,7 +4645,7 @@
       </c>
       <c r="H36">
         <f t="shared" si="0"/>
-        <v>1.1496202206608643</v>
+        <v>114.96202206608643</v>
       </c>
       <c r="I36">
         <f t="shared" si="1"/>
@@ -4651,7 +4657,7 @@
         <v>13</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C37">
         <v>50000000</v>
@@ -4670,7 +4676,7 @@
       </c>
       <c r="H37">
         <f t="shared" si="0"/>
-        <v>1.1484425373560794</v>
+        <v>114.84425373560794</v>
       </c>
       <c r="I37">
         <f t="shared" si="1"/>
@@ -4682,7 +4688,7 @@
         <v>13</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C38">
         <v>50000000</v>
@@ -4701,7 +4707,7 @@
       </c>
       <c r="H38">
         <f t="shared" si="0"/>
-        <v>1.1484425373560794</v>
+        <v>114.84425373560794</v>
       </c>
       <c r="I38">
         <f t="shared" si="1"/>
@@ -4717,7 +4723,7 @@
         <v>4</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C39">
         <v>50000000</v>
@@ -4736,7 +4742,7 @@
       </c>
       <c r="H39">
         <f t="shared" si="0"/>
-        <v>0.6214414785017478</v>
+        <v>62.144147850174782</v>
       </c>
       <c r="I39">
         <f t="shared" si="1"/>
@@ -4748,7 +4754,7 @@
         <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C40">
         <v>50000000</v>
@@ -4767,7 +4773,7 @@
       </c>
       <c r="H40">
         <f t="shared" si="0"/>
-        <v>0.61157898330351457</v>
+        <v>61.157898330351458</v>
       </c>
       <c r="I40">
         <f t="shared" si="1"/>
@@ -4779,7 +4785,7 @@
         <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C41">
         <v>50000000</v>
@@ -4798,7 +4804,7 @@
       </c>
       <c r="H41">
         <f t="shared" si="0"/>
-        <v>0.69991388259588538</v>
+        <v>69.991388259588533</v>
       </c>
       <c r="I41">
         <f t="shared" si="1"/>
@@ -4810,7 +4816,7 @@
         <v>4</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C42">
         <v>50000000</v>
@@ -4830,7 +4836,7 @@
       </c>
       <c r="H42">
         <f t="shared" si="0"/>
-        <v>0.69991388259588538</v>
+        <v>69.991388259588533</v>
       </c>
       <c r="I42">
         <f t="shared" si="1"/>
@@ -4846,7 +4852,7 @@
         <v>33</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C43">
         <v>50000000</v>
@@ -4865,7 +4871,7 @@
       </c>
       <c r="H43">
         <f t="shared" si="0"/>
-        <v>0.65095984745563162</v>
+        <v>65.095984745563158</v>
       </c>
       <c r="I43">
         <f t="shared" si="1"/>
@@ -4877,7 +4883,7 @@
         <v>33</v>
       </c>
       <c r="B44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C44">
         <v>50000000</v>
@@ -4896,7 +4902,7 @@
       </c>
       <c r="H44">
         <f t="shared" si="0"/>
-        <v>0.65126816043355495</v>
+        <v>65.12681604335549</v>
       </c>
       <c r="I44">
         <f t="shared" si="1"/>
@@ -4908,7 +4914,7 @@
         <v>33</v>
       </c>
       <c r="B45" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C45">
         <v>50000000</v>
@@ -4927,7 +4933,7 @@
       </c>
       <c r="H45">
         <f t="shared" si="0"/>
-        <v>0.64921824255479121</v>
+        <v>64.921824255479123</v>
       </c>
       <c r="I45">
         <f t="shared" si="1"/>
@@ -4939,7 +4945,7 @@
         <v>33</v>
       </c>
       <c r="B46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C46">
         <v>50000000</v>
@@ -4959,7 +4965,7 @@
       </c>
       <c r="H46">
         <f t="shared" si="0"/>
-        <v>0.64921824255479121</v>
+        <v>64.921824255479123</v>
       </c>
       <c r="I46">
         <f t="shared" si="1"/>
@@ -4975,7 +4981,7 @@
         <v>26</v>
       </c>
       <c r="B47" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C47">
         <v>50000000</v>
@@ -4994,7 +5000,7 @@
       </c>
       <c r="H47">
         <f t="shared" si="0"/>
-        <v>0.55068272322386758</v>
+        <v>55.068272322386761</v>
       </c>
       <c r="I47">
         <f t="shared" si="1"/>
@@ -5006,7 +5012,7 @@
         <v>26</v>
       </c>
       <c r="B48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C48">
         <v>50000000</v>
@@ -5025,7 +5031,7 @@
       </c>
       <c r="H48">
         <f t="shared" si="0"/>
-        <v>0.53845072305747654</v>
+        <v>53.845072305747657</v>
       </c>
       <c r="I48">
         <f t="shared" si="1"/>
@@ -5037,7 +5043,7 @@
         <v>26</v>
       </c>
       <c r="B49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C49">
         <v>50000000</v>
@@ -5056,7 +5062,7 @@
       </c>
       <c r="H49">
         <f t="shared" si="0"/>
-        <v>0.5809985538481196</v>
+        <v>58.09985538481196</v>
       </c>
       <c r="I49">
         <f t="shared" si="1"/>
@@ -5068,7 +5074,7 @@
         <v>26</v>
       </c>
       <c r="B50" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C50">
         <v>50000000</v>
@@ -5088,7 +5094,7 @@
       </c>
       <c r="H50">
         <f t="shared" si="0"/>
-        <v>0.5809985538481196</v>
+        <v>58.09985538481196</v>
       </c>
       <c r="I50">
         <f t="shared" si="1"/>
@@ -5104,7 +5110,7 @@
         <v>15</v>
       </c>
       <c r="B51" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C51">
         <v>50000000</v>
@@ -5123,7 +5129,7 @@
       </c>
       <c r="H51">
         <f t="shared" si="0"/>
-        <v>0.11429835816603466</v>
+        <v>11.429835816603466</v>
       </c>
       <c r="I51">
         <f t="shared" si="1"/>
@@ -5135,7 +5141,7 @@
         <v>15</v>
       </c>
       <c r="B52" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C52">
         <v>50000000</v>
@@ -5154,7 +5160,7 @@
       </c>
       <c r="H52">
         <f t="shared" si="0"/>
-        <v>0.11339835312161432</v>
+        <v>11.339835312161432</v>
       </c>
       <c r="I52">
         <f t="shared" si="1"/>
@@ -5166,7 +5172,7 @@
         <v>15</v>
       </c>
       <c r="B53" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C53">
         <v>50000000</v>
@@ -5185,7 +5191,7 @@
       </c>
       <c r="H53">
         <f t="shared" si="0"/>
-        <v>0.12027532860524762</v>
+        <v>12.027532860524762</v>
       </c>
       <c r="I53">
         <f t="shared" si="1"/>
@@ -5197,7 +5203,7 @@
         <v>15</v>
       </c>
       <c r="B54" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C54">
         <v>50000000</v>
@@ -5217,7 +5223,7 @@
       </c>
       <c r="H54">
         <f t="shared" si="0"/>
-        <v>0.12027532860524762</v>
+        <v>12.027532860524762</v>
       </c>
       <c r="I54">
         <f t="shared" si="1"/>
@@ -5233,7 +5239,7 @@
         <v>20</v>
       </c>
       <c r="B55" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C55">
         <v>50000002</v>
@@ -5252,7 +5258,7 @@
       </c>
       <c r="H55">
         <f t="shared" si="0"/>
-        <v>0.53761272327122711</v>
+        <v>53.761272327122711</v>
       </c>
       <c r="I55">
         <f t="shared" si="1"/>
@@ -5264,7 +5270,7 @@
         <v>20</v>
       </c>
       <c r="B56" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C56">
         <v>50000002</v>
@@ -5283,7 +5289,7 @@
       </c>
       <c r="H56">
         <f t="shared" si="0"/>
-        <v>0.53446073331045418</v>
+        <v>53.446073331045419</v>
       </c>
       <c r="I56">
         <f t="shared" si="1"/>
@@ -5295,7 +5301,7 @@
         <v>20</v>
       </c>
       <c r="B57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C57">
         <v>50000002</v>
@@ -5314,7 +5320,7 @@
       </c>
       <c r="H57">
         <f t="shared" si="0"/>
-        <v>0.53949176101702823</v>
+        <v>53.949176101702825</v>
       </c>
       <c r="I57">
         <f t="shared" si="1"/>
@@ -5326,7 +5332,7 @@
         <v>20</v>
       </c>
       <c r="B58" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C58">
         <v>50000002</v>
@@ -5346,7 +5352,7 @@
       </c>
       <c r="H58">
         <f t="shared" si="0"/>
-        <v>0.53949176101702823</v>
+        <v>53.949176101702825</v>
       </c>
       <c r="I58">
         <f t="shared" si="1"/>
@@ -5362,7 +5368,7 @@
         <v>5</v>
       </c>
       <c r="B59" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C59">
         <v>50000001</v>
@@ -5381,7 +5387,7 @@
       </c>
       <c r="H59">
         <f t="shared" si="0"/>
-        <v>0.33008123662160144</v>
+        <v>33.008123662160145</v>
       </c>
       <c r="I59">
         <f t="shared" si="1"/>
@@ -5393,7 +5399,7 @@
         <v>5</v>
       </c>
       <c r="B60" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C60">
         <v>50000001</v>
@@ -5412,7 +5418,7 @@
       </c>
       <c r="H60">
         <f t="shared" si="0"/>
-        <v>0.33954896258931777</v>
+        <v>33.954896258931775</v>
       </c>
       <c r="I60">
         <f t="shared" si="1"/>
@@ -5424,7 +5430,7 @@
         <v>5</v>
       </c>
       <c r="B61" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C61">
         <v>50000001</v>
@@ -5443,7 +5449,7 @@
       </c>
       <c r="H61">
         <f t="shared" si="0"/>
-        <v>0.36306369931419374</v>
+        <v>36.306369931419376</v>
       </c>
       <c r="I61">
         <f t="shared" si="1"/>
@@ -5455,7 +5461,7 @@
         <v>5</v>
       </c>
       <c r="B62" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C62">
         <v>50000001</v>
@@ -5475,7 +5481,7 @@
       </c>
       <c r="H62">
         <f t="shared" si="0"/>
-        <v>0.36306369931419374</v>
+        <v>36.306369931419376</v>
       </c>
       <c r="I62">
         <f t="shared" si="1"/>
@@ -5491,7 +5497,7 @@
         <v>16</v>
       </c>
       <c r="B63" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C63">
         <v>50000000</v>
@@ -5510,7 +5516,7 @@
       </c>
       <c r="H63">
         <f t="shared" si="0"/>
-        <v>0.39410533186995195</v>
+        <v>39.410533186995195</v>
       </c>
       <c r="I63">
         <f t="shared" si="1"/>
@@ -5522,7 +5528,7 @@
         <v>16</v>
       </c>
       <c r="B64" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C64">
         <v>50000000</v>
@@ -5541,7 +5547,7 @@
       </c>
       <c r="H64">
         <f t="shared" si="0"/>
-        <v>0.40003180412855543</v>
+        <v>40.003180412855542</v>
       </c>
       <c r="I64">
         <f t="shared" si="1"/>
@@ -5553,7 +5559,7 @@
         <v>16</v>
       </c>
       <c r="B65" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C65">
         <v>50000000</v>
@@ -5572,7 +5578,7 @@
       </c>
       <c r="H65">
         <f t="shared" si="0"/>
-        <v>0.4036170350476655</v>
+        <v>40.361703504766552</v>
       </c>
       <c r="I65">
         <f t="shared" si="1"/>
@@ -5584,7 +5590,7 @@
         <v>16</v>
       </c>
       <c r="B66" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C66">
         <v>50000000</v>
@@ -5604,7 +5610,7 @@
       </c>
       <c r="H66">
         <f t="shared" si="0"/>
-        <v>0.4036170350476655</v>
+        <v>40.361703504766552</v>
       </c>
       <c r="I66">
         <f t="shared" si="1"/>
@@ -5620,7 +5626,7 @@
         <v>19</v>
       </c>
       <c r="B67" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C67">
         <v>50000000</v>
@@ -5639,7 +5645,7 @@
       </c>
       <c r="H67">
         <f t="shared" si="0"/>
-        <v>0.82817449636638441</v>
+        <v>82.817449636638443</v>
       </c>
       <c r="I67">
         <f t="shared" si="1"/>
@@ -5651,7 +5657,7 @@
         <v>19</v>
       </c>
       <c r="B68" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C68">
         <v>50000000</v>
@@ -5669,8 +5675,8 @@
         <v>620713</v>
       </c>
       <c r="H68">
-        <f t="shared" ref="H68:H82" si="2">(C68/D68)</f>
-        <v>0.85554505098329847</v>
+        <f t="shared" ref="H68:H82" si="2">(C68/D68)*100</f>
+        <v>85.554505098329841</v>
       </c>
       <c r="I68">
         <f t="shared" ref="I68:I82" si="3">G68/(C68/1000)</f>
@@ -5682,7 +5688,7 @@
         <v>19</v>
       </c>
       <c r="B69" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C69">
         <v>50000000</v>
@@ -5701,7 +5707,7 @@
       </c>
       <c r="H69">
         <f t="shared" si="2"/>
-        <v>0.9387414151158846</v>
+        <v>93.874141511588462</v>
       </c>
       <c r="I69">
         <f t="shared" si="3"/>
@@ -5713,7 +5719,7 @@
         <v>19</v>
       </c>
       <c r="B70" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C70">
         <v>50000000</v>
@@ -5733,7 +5739,7 @@
       </c>
       <c r="H70">
         <f t="shared" si="2"/>
-        <v>0.9387414151158846</v>
+        <v>93.874141511588462</v>
       </c>
       <c r="I70">
         <f t="shared" si="3"/>
@@ -5749,7 +5755,7 @@
         <v>12</v>
       </c>
       <c r="B71" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C71">
         <v>50000000</v>
@@ -5768,7 +5774,7 @@
       </c>
       <c r="H71">
         <f t="shared" si="2"/>
-        <v>0.82727660689918581</v>
+        <v>82.727660689918579</v>
       </c>
       <c r="I71">
         <f t="shared" si="3"/>
@@ -5780,7 +5786,7 @@
         <v>12</v>
       </c>
       <c r="B72" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C72">
         <v>50000000</v>
@@ -5799,7 +5805,7 @@
       </c>
       <c r="H72">
         <f t="shared" si="2"/>
-        <v>0.83316393721883109</v>
+        <v>83.316393721883102</v>
       </c>
       <c r="I72">
         <f t="shared" si="3"/>
@@ -5811,7 +5817,7 @@
         <v>12</v>
       </c>
       <c r="B73" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C73">
         <v>50000000</v>
@@ -5830,7 +5836,7 @@
       </c>
       <c r="H73">
         <f t="shared" si="2"/>
-        <v>0.86461539201117166</v>
+        <v>86.461539201117162</v>
       </c>
       <c r="I73">
         <f t="shared" si="3"/>
@@ -5842,7 +5848,7 @@
         <v>12</v>
       </c>
       <c r="B74" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C74">
         <v>50000000</v>
@@ -5862,7 +5868,7 @@
       </c>
       <c r="H74">
         <f t="shared" si="2"/>
-        <v>0.86461539201117166</v>
+        <v>86.461539201117162</v>
       </c>
       <c r="I74">
         <f t="shared" si="3"/>
@@ -5878,7 +5884,7 @@
         <v>22</v>
       </c>
       <c r="B75" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C75">
         <v>50000000</v>
@@ -5897,7 +5903,7 @@
       </c>
       <c r="H75">
         <f t="shared" si="2"/>
-        <v>0.25786801072287391</v>
+        <v>25.786801072287389</v>
       </c>
       <c r="I75">
         <f t="shared" si="3"/>
@@ -5909,7 +5915,7 @@
         <v>22</v>
       </c>
       <c r="B76" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C76">
         <v>50000000</v>
@@ -5928,7 +5934,7 @@
       </c>
       <c r="H76">
         <f t="shared" si="2"/>
-        <v>0.25947786763288749</v>
+        <v>25.94778676328875</v>
       </c>
       <c r="I76">
         <f t="shared" si="3"/>
@@ -5940,7 +5946,7 @@
         <v>22</v>
       </c>
       <c r="B77" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C77">
         <v>50000000</v>
@@ -5959,7 +5965,7 @@
       </c>
       <c r="H77">
         <f t="shared" si="2"/>
-        <v>0.268103087224208</v>
+        <v>26.8103087224208</v>
       </c>
       <c r="I77">
         <f t="shared" si="3"/>
@@ -5971,7 +5977,7 @@
         <v>22</v>
       </c>
       <c r="B78" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C78">
         <v>50000000</v>
@@ -5991,7 +5997,7 @@
       </c>
       <c r="H78">
         <f t="shared" si="2"/>
-        <v>0.268103087224208</v>
+        <v>26.8103087224208</v>
       </c>
       <c r="I78">
         <f t="shared" si="3"/>
@@ -6007,7 +6013,7 @@
         <v>23</v>
       </c>
       <c r="B79" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C79">
         <v>50000001</v>
@@ -6026,7 +6032,7 @@
       </c>
       <c r="H79">
         <f t="shared" si="2"/>
-        <v>1.4565732454592422</v>
+        <v>145.65732454592421</v>
       </c>
       <c r="I79">
         <f t="shared" si="3"/>
@@ -6038,7 +6044,7 @@
         <v>23</v>
       </c>
       <c r="B80" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C80">
         <v>50000002</v>
@@ -6057,7 +6063,7 @@
       </c>
       <c r="H80">
         <f t="shared" si="2"/>
-        <v>1.4472331436058998</v>
+        <v>144.72331436059</v>
       </c>
       <c r="I80">
         <f t="shared" si="3"/>
@@ -6069,7 +6075,7 @@
         <v>23</v>
       </c>
       <c r="B81" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C81">
         <v>50000001</v>
@@ -6088,7 +6094,7 @@
       </c>
       <c r="H81">
         <f t="shared" si="2"/>
-        <v>1.4534420093219118</v>
+        <v>145.34420093219117</v>
       </c>
       <c r="I81">
         <f t="shared" si="3"/>
@@ -6100,7 +6106,7 @@
         <v>23</v>
       </c>
       <c r="B82" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C82">
         <v>50000001</v>
@@ -6120,7 +6126,7 @@
       </c>
       <c r="H82">
         <f t="shared" si="2"/>
-        <v>1.4534420093219118</v>
+        <v>145.34420093219117</v>
       </c>
       <c r="I82">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Added average results to simulation
</commit_message>
<xml_diff>
--- a/Reports/Simulation_Results.xlsx
+++ b/Reports/Simulation_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glodp\Desktop\Spring 2019\CSCE614 - Computer Architecture\BeladyCacheReplacement\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7251149A-CDB5-4E97-8717-BF6944BBA6E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625A7D15-3D6B-4DAA-977D-D7C5EDB5B606}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{97E21B71-3375-4992-AB3C-5A8BB98BB2E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Benchmarks" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="50">
   <si>
     <t>Benchmark</t>
   </si>
@@ -180,12 +180,15 @@
   <si>
     <t>IPC(%)</t>
   </si>
+  <si>
+    <t>Average</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,6 +227,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -245,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -268,12 +279,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,11 +613,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
       <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -745,7 +757,7 @@
       <c r="B14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>33</v>
       </c>
     </row>
@@ -756,7 +768,7 @@
       <c r="B15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="10" t="s">
         <v>26</v>
       </c>
     </row>
@@ -860,10 +872,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4DAA02D-4B80-49E4-98A1-4EF8777A053B}">
-  <dimension ref="A2:L82"/>
+  <dimension ref="A2:L87"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G85" sqref="G85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3494,6 +3506,67 @@
         <v>0.1712153280605993</v>
       </c>
     </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A84" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6">
+        <v>56.74</v>
+      </c>
+      <c r="I84" s="6">
+        <v>14.32</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A85" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="6"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6">
+        <v>56.85</v>
+      </c>
+      <c r="I85" s="6">
+        <v>14.05</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A86" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6">
+        <v>58.52</v>
+      </c>
+      <c r="I86" s="6">
+        <v>14.02</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H87" s="6"/>
+      <c r="I87" s="6"/>
+    </row>
   </sheetData>
   <sortState ref="B3:B20">
     <sortCondition ref="B3"/>
@@ -3505,10 +3578,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E5CF80-89BD-41BF-8339-D77E14018905}">
-  <dimension ref="A2:L82"/>
+  <dimension ref="A2:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="H86" sqref="H86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6137,6 +6210,63 @@
         <v>0.33050150726226363</v>
       </c>
     </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A84" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6">
+        <v>61.55</v>
+      </c>
+      <c r="I84" s="12">
+        <v>17.989999999999998</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A85" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="6"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6">
+        <v>61.66</v>
+      </c>
+      <c r="I85" s="12">
+        <v>17.760000000000002</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A86" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6">
+        <v>62.89</v>
+      </c>
+      <c r="I86" s="12">
+        <v>17.98</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>